<commit_message>
CASE All-electric low-rise runs and results
</commit_message>
<xml_diff>
--- a/framework/analysis/lr/TDVAnnual.xlsx
+++ b/framework/analysis/lr/TDVAnnual.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">CZ</t>
   </si>
@@ -28,6 +28,12 @@
   </si>
   <si>
     <t xml:space="preserve">kTDV_Total_NG_2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source_kBtu_Elec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source_kBtu_NG</t>
   </si>
   <si>
     <t xml:space="preserve">kWh_Elec_Comp</t>
@@ -45,13 +51,19 @@
     <t xml:space="preserve">Measure</t>
   </si>
   <si>
-    <t xml:space="preserve">lrlc-flat-tier2env</t>
+    <t xml:space="preserve">lrlc-baseline-all</t>
   </si>
   <si>
-    <t xml:space="preserve">lrgs-low-tier2env</t>
+    <t xml:space="preserve">lrlc-flat19-base</t>
   </si>
   <si>
-    <t xml:space="preserve">LifeTime: ,30,TDVMultiplier: ,res,DHW Removed: ,TRUE</t>
+    <t xml:space="preserve">lrgs-low-baseszac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lrgs-low-base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LifeTime: ,30,TDVMultiplier: ,res,DHW Removed: ,FALSE</t>
   </si>
 </sst>
 </file>
@@ -414,37 +426,49 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>43408.7507443</v>
+        <v>22828.66470122</v>
       </c>
       <c r="C2" t="n">
-        <v>1344.308552</v>
+        <v>8696.770195</v>
       </c>
       <c r="D2" t="n">
-        <v>64.7397488111797</v>
+        <v>48.6544565957884</v>
       </c>
       <c r="E2" t="n">
-        <v>12.0145824112502</v>
+        <v>78.2650760720572</v>
       </c>
       <c r="F2" t="n">
-        <v>62966.1897262482</v>
+        <v>320987.265577084</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>761666.888603171</v>
       </c>
       <c r="H2" t="n">
-        <v>47.8128437022488</v>
+        <v>42586.8161831916</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
+        <v>7352.46149568424</v>
+      </c>
+      <c r="J2" t="n">
+        <v>31.8627964983222</v>
+      </c>
+      <c r="K2" t="n">
+        <v>66.2504924891521</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -452,31 +476,37 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>26277.45108358</v>
+        <v>13735.97324775</v>
       </c>
       <c r="C3" t="n">
-        <v>1344.308458</v>
+        <v>7341.997463</v>
       </c>
       <c r="D3" t="n">
-        <v>54.4080951346868</v>
+        <v>44.6929948508488</v>
       </c>
       <c r="E3" t="n">
-        <v>12.0145815052065</v>
+        <v>66.2800542546027</v>
       </c>
       <c r="F3" t="n">
-        <v>47721.2239294756</v>
+        <v>303886.28683166</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>643015.307796756</v>
       </c>
       <c r="H3" t="n">
-        <v>42.5815585619085</v>
+        <v>35232.7420231726</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>10</v>
+        <v>5997.6890156942</v>
+      </c>
+      <c r="J3" t="n">
+        <v>32.916111155739</v>
+      </c>
+      <c r="K3" t="n">
+        <v>54.2654728395149</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -484,31 +514,37 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>14481.37557129</v>
+        <v>9771.5712423</v>
       </c>
       <c r="C4" t="n">
-        <v>1344.308536</v>
+        <v>6625.982674</v>
       </c>
       <c r="D4" t="n">
-        <v>43.2992169384408</v>
+        <v>39.0981204970025</v>
       </c>
       <c r="E4" t="n">
-        <v>12.0145821372652</v>
+        <v>59.4585968502382</v>
       </c>
       <c r="F4" t="n">
-        <v>33105.7717890154</v>
+        <v>282809.245132173</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>580306.423428968</v>
       </c>
       <c r="H4" t="n">
-        <v>27.7149957514402</v>
+        <v>28498.1004077125</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>10</v>
+        <v>5281.6741805551</v>
+      </c>
+      <c r="J4" t="n">
+        <v>23.5884503389445</v>
+      </c>
+      <c r="K4" t="n">
+        <v>47.4440151078061</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -516,31 +552,37 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>13377.314</v>
+        <v>7589.46405997</v>
       </c>
       <c r="C5" t="n">
-        <v>1344.308619</v>
+        <v>6375.030487</v>
       </c>
       <c r="D5" t="n">
-        <v>46.6476545476161</v>
+        <v>40.9924438776492</v>
       </c>
       <c r="E5" t="n">
-        <v>12.0145828940284</v>
+        <v>57.279707155273</v>
       </c>
       <c r="F5" t="n">
-        <v>40884.3998326058</v>
+        <v>297628.713179168</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>558327.922540173</v>
       </c>
       <c r="H5" t="n">
-        <v>40.8723035352456</v>
+        <v>35134.3757147033</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>10</v>
+        <v>5030.7218267762</v>
+      </c>
+      <c r="J5" t="n">
+        <v>35.2501284085163</v>
+      </c>
+      <c r="K5" t="n">
+        <v>45.265123941294</v>
+      </c>
+      <c r="L5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -548,31 +590,37 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>15222.91653777</v>
+        <v>10328.69193727</v>
       </c>
       <c r="C6" t="n">
-        <v>1344.308603</v>
+        <v>6554.546615</v>
       </c>
       <c r="D6" t="n">
-        <v>41.9356678334007</v>
+        <v>37.6707374426873</v>
       </c>
       <c r="E6" t="n">
-        <v>12.0145827263932</v>
+        <v>58.7383453960818</v>
       </c>
       <c r="F6" t="n">
-        <v>33722.6063045806</v>
+        <v>274106.989041872</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>574050.022538453</v>
       </c>
       <c r="H6" t="n">
-        <v>26.3572660625163</v>
+        <v>28949.4752215308</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>10</v>
+        <v>5210.237931358</v>
+      </c>
+      <c r="J6" t="n">
+        <v>22.1835100841028</v>
+      </c>
+      <c r="K6" t="n">
+        <v>46.7237619116295</v>
+      </c>
+      <c r="L6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -580,31 +628,37 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>4771.78789619999</v>
+        <v>137982.19015</v>
       </c>
       <c r="C7" t="n">
-        <v>1344.308916</v>
+        <v>5810.479147</v>
       </c>
       <c r="D7" t="n">
-        <v>39.5221645216591</v>
+        <v>106.695609919442</v>
       </c>
       <c r="E7" t="n">
-        <v>12.0339303724351</v>
+        <v>52.0435003408487</v>
       </c>
       <c r="F7" t="n">
-        <v>33207.1703256339</v>
+        <v>359662.3957553</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>501728.010235828</v>
       </c>
       <c r="H7" t="n">
-        <v>32.9388299360901</v>
+        <v>30949.3851436631</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>10</v>
+        <v>4466.1702918795</v>
+      </c>
+      <c r="J7" t="n">
+        <v>30.6945074197909</v>
+      </c>
+      <c r="K7" t="n">
+        <v>40.0095705356774</v>
+      </c>
+      <c r="L7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -612,31 +666,37 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>3397.58357159999</v>
+        <v>136360.83874</v>
       </c>
       <c r="C8" t="n">
-        <v>1344.308695</v>
+        <v>5760.495689</v>
       </c>
       <c r="D8" t="n">
-        <v>37.2278961493206</v>
+        <v>102.546228153802</v>
       </c>
       <c r="E8" t="n">
-        <v>12.0628469184915</v>
+        <v>51.6950752895751</v>
       </c>
       <c r="F8" t="n">
-        <v>31019.0057168875</v>
+        <v>356757.074418852</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>497411.99768461</v>
       </c>
       <c r="H8" t="n">
-        <v>28.0998463172787</v>
+        <v>29093.0850377257</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>10</v>
+        <v>4416.187017021</v>
+      </c>
+      <c r="J8" t="n">
+        <v>25.9811005159642</v>
+      </c>
+      <c r="K8" t="n">
+        <v>39.6322285929515</v>
+      </c>
+      <c r="L8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -644,31 +704,37 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>5342.39020959999</v>
+        <v>2849.42372902</v>
       </c>
       <c r="C9" t="n">
-        <v>1344.308737</v>
+        <v>5649.62038</v>
       </c>
       <c r="D9" t="n">
-        <v>35.2573097378437</v>
+        <v>33.0278471158291</v>
       </c>
       <c r="E9" t="n">
-        <v>12.0339287804542</v>
+        <v>50.614321783342</v>
       </c>
       <c r="F9" t="n">
-        <v>42520.369730709</v>
+        <v>284191.940232869</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>487838.045733061</v>
       </c>
       <c r="H9" t="n">
-        <v>41.1572208882947</v>
+        <v>39993.7012375079</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>10</v>
+        <v>4305.311699464</v>
+      </c>
+      <c r="J9" t="n">
+        <v>38.9201490411927</v>
+      </c>
+      <c r="K9" t="n">
+        <v>38.5803935371693</v>
+      </c>
+      <c r="L9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -676,31 +742,37 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>5091.65777878999</v>
+        <v>4146.0636342</v>
       </c>
       <c r="C10" t="n">
-        <v>1344.308564</v>
+        <v>5770.703551</v>
       </c>
       <c r="D10" t="n">
-        <v>38.8588434596099</v>
+        <v>38.3855819107565</v>
       </c>
       <c r="E10" t="n">
-        <v>12.0339272515418</v>
+        <v>51.7548839427498</v>
       </c>
       <c r="F10" t="n">
-        <v>41604.1055333556</v>
+        <v>288714.10107434</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>498293.434509431</v>
       </c>
       <c r="H10" t="n">
-        <v>40.9785609475894</v>
+        <v>40566.4232453719</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>10</v>
+        <v>4426.394947388</v>
+      </c>
+      <c r="J10" t="n">
+        <v>40.4635656667657</v>
+      </c>
+      <c r="K10" t="n">
+        <v>39.7209563184306</v>
+      </c>
+      <c r="L10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -708,31 +780,37 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>9301.62312174999</v>
+        <v>6078.639046693</v>
       </c>
       <c r="C11" t="n">
-        <v>1344.308636</v>
+        <v>5928.14455</v>
       </c>
       <c r="D11" t="n">
-        <v>46.6041409563985</v>
+        <v>44.2677362795241</v>
       </c>
       <c r="E11" t="n">
-        <v>12.0339279093842</v>
+        <v>53.3281616110487</v>
       </c>
       <c r="F11" t="n">
-        <v>51298.3720282289</v>
+        <v>303345.350280852</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>511888.278782919</v>
       </c>
       <c r="H11" t="n">
-        <v>49.6185627277685</v>
+        <v>48118.6978464883</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="s">
-        <v>10</v>
+        <v>4583.835910441</v>
+      </c>
+      <c r="J11" t="n">
+        <v>47.3143877531963</v>
+      </c>
+      <c r="K11" t="n">
+        <v>41.2942336632156</v>
+      </c>
+      <c r="L11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -740,31 +818,37 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>24505.1654943</v>
+        <v>168927.06621</v>
       </c>
       <c r="C12" t="n">
-        <v>1344.308502</v>
+        <v>6840.718989</v>
       </c>
       <c r="D12" t="n">
-        <v>68.318478801708</v>
+        <v>136.504636442762</v>
       </c>
       <c r="E12" t="n">
-        <v>12.014581815015</v>
+        <v>61.9669056801819</v>
       </c>
       <c r="F12" t="n">
-        <v>74587.1877710962</v>
+        <v>441881.929519526</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>599113.122611406</v>
       </c>
       <c r="H12" t="n">
-        <v>70.4695570628751</v>
+        <v>61895.6682311594</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="s">
-        <v>10</v>
+        <v>5496.4104890889</v>
+      </c>
+      <c r="J12" t="n">
+        <v>60.9481537796566</v>
+      </c>
+      <c r="K12" t="n">
+        <v>49.95232388295</v>
+      </c>
+      <c r="L12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13">
@@ -772,31 +856,37 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>23443.40286967</v>
+        <v>10780.8973734</v>
       </c>
       <c r="C13" t="n">
-        <v>1344.308579</v>
+        <v>6914.970738</v>
       </c>
       <c r="D13" t="n">
-        <v>63.5636967678254</v>
+        <v>52.6795034206022</v>
       </c>
       <c r="E13" t="n">
-        <v>12.0145825143981</v>
+        <v>62.4991409877888</v>
       </c>
       <c r="F13" t="n">
-        <v>56887.5979987525</v>
+        <v>325624.16878777</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>605616.122847826</v>
       </c>
       <c r="H13" t="n">
-        <v>57.1448443208908</v>
+        <v>44251.9394230849</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>10</v>
+        <v>5570.662225892</v>
+      </c>
+      <c r="J13" t="n">
+        <v>46.290917311368</v>
+      </c>
+      <c r="K13" t="n">
+        <v>50.4845590993907</v>
+      </c>
+      <c r="L13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14">
@@ -804,31 +894,37 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>18717.0900641</v>
+        <v>9582.03940256</v>
       </c>
       <c r="C14" t="n">
-        <v>1344.308529</v>
+        <v>6393.784235</v>
       </c>
       <c r="D14" t="n">
-        <v>64.6520233681838</v>
+        <v>57.594717061715</v>
       </c>
       <c r="E14" t="n">
-        <v>12.0145820588218</v>
+        <v>57.7931467903642</v>
       </c>
       <c r="F14" t="n">
-        <v>74143.3640761077</v>
+        <v>362131.625882005</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>559970.383887148</v>
       </c>
       <c r="H14" t="n">
-        <v>70.5264950125606</v>
+        <v>65045.247717797</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="s">
-        <v>10</v>
+        <v>5049.4757180326</v>
+      </c>
+      <c r="J14" t="n">
+        <v>63.4976705978154</v>
+      </c>
+      <c r="K14" t="n">
+        <v>45.7785648282996</v>
+      </c>
+      <c r="L14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15">
@@ -836,31 +932,37 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>25852.10742902</v>
+        <v>165480.29325</v>
       </c>
       <c r="C15" t="n">
-        <v>1344.308617</v>
+        <v>6754.363389</v>
       </c>
       <c r="D15" t="n">
-        <v>58.3276549965957</v>
+        <v>127.200380531781</v>
       </c>
       <c r="E15" t="n">
-        <v>12.0339277065089</v>
+        <v>61.2338668307596</v>
       </c>
       <c r="F15" t="n">
-        <v>71876.1783060095</v>
+        <v>438295.988692234</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>583231.299491435</v>
       </c>
       <c r="H15" t="n">
-        <v>64.7939648425317</v>
+        <v>58819.8813587715</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="s">
-        <v>10</v>
+        <v>5410.0548007928</v>
+      </c>
+      <c r="J15" t="n">
+        <v>53.792049413419</v>
+      </c>
+      <c r="K15" t="n">
+        <v>49.1999394187638</v>
+      </c>
+      <c r="L15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16">
@@ -868,31 +970,37 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>4163.11545128999</v>
+        <v>208205.55534</v>
       </c>
       <c r="C16" t="n">
-        <v>1344.308684</v>
+        <v>4919.170673</v>
       </c>
       <c r="D16" t="n">
-        <v>58.6027346671191</v>
+        <v>163.518263935285</v>
       </c>
       <c r="E16" t="n">
-        <v>12.0339283963091</v>
+        <v>44.2103882820078</v>
       </c>
       <c r="F16" t="n">
-        <v>101129.937236683</v>
+        <v>514813.13414919</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>424764.57643756</v>
       </c>
       <c r="H16" t="n">
-        <v>89.7250412708177</v>
+        <v>100229.835889598</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="s">
-        <v>10</v>
+        <v>3574.8619825</v>
+      </c>
+      <c r="J16" t="n">
+        <v>89.0403794961183</v>
+      </c>
+      <c r="K16" t="n">
+        <v>32.1764598235932</v>
+      </c>
+      <c r="L16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17">
@@ -900,31 +1008,37 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>56821.45446252</v>
+        <v>156324.88534</v>
       </c>
       <c r="C17" t="n">
-        <v>1344.308644</v>
+        <v>9471.761148</v>
       </c>
       <c r="D17" t="n">
-        <v>81.7115840854292</v>
+        <v>117.020260432414</v>
       </c>
       <c r="E17" t="n">
-        <v>12.033928036864</v>
+        <v>86.0533486654822</v>
       </c>
       <c r="F17" t="n">
-        <v>84522.5058607134</v>
+        <v>413258.495268811</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>817875.385830907</v>
       </c>
       <c r="H17" t="n">
-        <v>70.3120165399874</v>
+        <v>50065.887172835</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="s">
-        <v>10</v>
+        <v>8127.4525328601</v>
+      </c>
+      <c r="J17" t="n">
+        <v>39.5226900278527</v>
+      </c>
+      <c r="K17" t="n">
+        <v>74.0194207932843</v>
+      </c>
+      <c r="L17" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18">
@@ -932,31 +1046,37 @@
         <v>1</v>
       </c>
       <c r="B18" t="n">
-        <v>6948.1845358182</v>
+        <v>47614.03212243</v>
       </c>
       <c r="C18" t="n">
-        <v>293.89613924</v>
+        <v>6619.330973</v>
       </c>
       <c r="D18" t="n">
-        <v>59.7399005697486</v>
+        <v>67.8711178828148</v>
       </c>
       <c r="E18" t="n">
-        <v>14.1245572474564</v>
+        <v>59.1067270304137</v>
       </c>
       <c r="F18" t="n">
-        <v>9503.646363394</v>
+        <v>402783.858052294</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>579723.864583444</v>
       </c>
       <c r="H18" t="n">
-        <v>38.5865101199428</v>
+        <v>67286.8278348038</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
-        <v>11</v>
+        <v>5275.022421</v>
+      </c>
+      <c r="J18" t="n">
+        <v>51.0179576622851</v>
+      </c>
+      <c r="K18" t="n">
+        <v>47.0921446191635</v>
+      </c>
+      <c r="L18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19">
@@ -964,31 +1084,37 @@
         <v>2</v>
       </c>
       <c r="B19" t="n">
-        <v>3846.477172906</v>
+        <v>29109.84954024</v>
       </c>
       <c r="C19" t="n">
-        <v>293.8961718</v>
+        <v>6186.758084</v>
       </c>
       <c r="D19" t="n">
-        <v>48.1395285968774</v>
+        <v>56.2532783752974</v>
       </c>
       <c r="E19" t="n">
-        <v>14.1245588536401</v>
+        <v>55.31458802475</v>
       </c>
       <c r="F19" t="n">
-        <v>6516.0397152521</v>
+        <v>361077.021550051</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>541838.944196776</v>
       </c>
       <c r="H19" t="n">
-        <v>31.7622657651786</v>
+        <v>50560.2932897283</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" t="s">
-        <v>11</v>
+        <v>4842.449626</v>
+      </c>
+      <c r="J19" t="n">
+        <v>44.4427335927938</v>
+      </c>
+      <c r="K19" t="n">
+        <v>43.3000065195435</v>
+      </c>
+      <c r="L19" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20">
@@ -996,31 +1122,37 @@
         <v>3</v>
       </c>
       <c r="B20" t="n">
-        <v>1610.77029423</v>
+        <v>15993.09321725</v>
       </c>
       <c r="C20" t="n">
-        <v>293.89615828</v>
+        <v>6176.655733</v>
       </c>
       <c r="D20" t="n">
-        <v>37.6997877037874</v>
+        <v>44.0052167625924</v>
       </c>
       <c r="E20" t="n">
-        <v>14.1245582085327</v>
+        <v>55.1829882749937</v>
       </c>
       <c r="F20" t="n">
-        <v>3872.337140768</v>
+        <v>308343.833407084</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>540954.175934396</v>
       </c>
       <c r="H20" t="n">
-        <v>17.741732535794</v>
+        <v>34692.2513553354</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" t="s">
-        <v>11</v>
+        <v>4832.347197</v>
+      </c>
+      <c r="J20" t="n">
+        <v>28.4750778340043</v>
+      </c>
+      <c r="K20" t="n">
+        <v>43.1684061377285</v>
+      </c>
+      <c r="L20" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="21">
@@ -1028,31 +1160,37 @@
         <v>4</v>
       </c>
       <c r="B21" t="n">
-        <v>1372.68406039</v>
+        <v>14543.88697862</v>
       </c>
       <c r="C21" t="n">
-        <v>293.89614521</v>
+        <v>5916.584654</v>
       </c>
       <c r="D21" t="n">
-        <v>40.0357606947059</v>
+        <v>47.5047222742376</v>
       </c>
       <c r="E21" t="n">
-        <v>14.1245576043495</v>
+        <v>52.9186196440184</v>
       </c>
       <c r="F21" t="n">
-        <v>4714.4629445678</v>
+        <v>325149.830646422</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>518177.038547061</v>
       </c>
       <c r="H21" t="n">
-        <v>28.1855241877169</v>
+        <v>42064.6325372254</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" t="s">
-        <v>11</v>
+        <v>4572.276035</v>
+      </c>
+      <c r="J21" t="n">
+        <v>41.746400837232</v>
+      </c>
+      <c r="K21" t="n">
+        <v>40.90403674999</v>
+      </c>
+      <c r="L21" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="22">
@@ -1060,31 +1198,37 @@
         <v>5</v>
       </c>
       <c r="B22" t="n">
-        <v>1650.524016147</v>
+        <v>16802.31111799</v>
       </c>
       <c r="C22" t="n">
-        <v>293.8961799</v>
+        <v>6177.467889</v>
       </c>
       <c r="D22" t="n">
-        <v>36.2439682695918</v>
+        <v>42.8477505694039</v>
       </c>
       <c r="E22" t="n">
-        <v>14.1245592578048</v>
+        <v>55.1824275327287</v>
       </c>
       <c r="F22" t="n">
-        <v>3864.551385184</v>
+        <v>299896.643751945</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>541025.304907534</v>
       </c>
       <c r="H22" t="n">
-        <v>15.9786449994983</v>
+        <v>35390.0035800967</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" t="s">
-        <v>11</v>
+        <v>4833.159286</v>
+      </c>
+      <c r="J22" t="n">
+        <v>27.3372585873033</v>
+      </c>
+      <c r="K22" t="n">
+        <v>43.1678448063354</v>
+      </c>
+      <c r="L22" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="23">
@@ -1092,31 +1236,37 @@
         <v>6</v>
       </c>
       <c r="B23" t="n">
-        <v>61.1221507400001</v>
+        <v>4283.03243748</v>
       </c>
       <c r="C23" t="n">
-        <v>293.89616515</v>
+        <v>5760.430606</v>
       </c>
       <c r="D23" t="n">
-        <v>33.2304239450428</v>
+        <v>39.0570892407645</v>
       </c>
       <c r="E23" t="n">
-        <v>14.1472536862422</v>
+        <v>51.5664691108899</v>
       </c>
       <c r="F23" t="n">
-        <v>2999.9266323149</v>
+        <v>274669.293505089</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>497406.377844445</v>
       </c>
       <c r="H23" t="n">
-        <v>18.979787283701</v>
+        <v>32684.9360938539</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" t="s">
-        <v>11</v>
+        <v>4416.12169</v>
+      </c>
+      <c r="J23" t="n">
+        <v>32.474559590281</v>
+      </c>
+      <c r="K23" t="n">
+        <v>39.5325387384548</v>
+      </c>
+      <c r="L23" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="24">
@@ -1124,31 +1274,37 @@
         <v>7</v>
       </c>
       <c r="B24" t="n">
-        <v>-58.1201381999999</v>
+        <v>2559.67625249</v>
       </c>
       <c r="C24" t="n">
-        <v>293.89617428</v>
+        <v>5747.447556</v>
       </c>
       <c r="D24" t="n">
-        <v>32.1922767594723</v>
+        <v>36.2180111601606</v>
       </c>
       <c r="E24" t="n">
-        <v>14.1811485516802</v>
+        <v>51.5693343359411</v>
       </c>
       <c r="F24" t="n">
-        <v>2948.86003494885</v>
+        <v>263523.02091084</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>496285.306814243</v>
       </c>
       <c r="H24" t="n">
-        <v>15.984778104753</v>
+        <v>30041.2095182028</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" t="s">
-        <v>11</v>
+        <v>4403.138861</v>
+      </c>
+      <c r="J24" t="n">
+        <v>27.040629985282</v>
+      </c>
+      <c r="K24" t="n">
+        <v>39.5064874174496</v>
+      </c>
+      <c r="L24" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="25">
@@ -1156,31 +1312,37 @@
         <v>8</v>
       </c>
       <c r="B25" t="n">
-        <v>105.66073072</v>
+        <v>4848.4429277</v>
       </c>
       <c r="C25" t="n">
-        <v>293.89616907</v>
+        <v>5624.593541</v>
       </c>
       <c r="D25" t="n">
-        <v>30.620780876145</v>
+        <v>35.0115725522357</v>
       </c>
       <c r="E25" t="n">
-        <v>14.1472538094163</v>
+        <v>50.3746175429341</v>
       </c>
       <c r="F25" t="n">
-        <v>5091.9233645687</v>
+        <v>291702.135486393</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>485677.007750429</v>
       </c>
       <c r="H25" t="n">
-        <v>29.9904502541164</v>
+        <v>41987.6102970714</v>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" t="s">
-        <v>11</v>
+        <v>4280.284804</v>
+      </c>
+      <c r="J25" t="n">
+        <v>40.9002613331147</v>
+      </c>
+      <c r="K25" t="n">
+        <v>38.3406887624799</v>
+      </c>
+      <c r="L25" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="26">
@@ -1188,31 +1350,37 @@
         <v>9</v>
       </c>
       <c r="B26" t="n">
-        <v>311.26334338</v>
+        <v>7304.06060409</v>
       </c>
       <c r="C26" t="n">
-        <v>293.8961447</v>
+        <v>5663.812742</v>
       </c>
       <c r="D26" t="n">
-        <v>35.0520301092107</v>
+        <v>41.2565072791277</v>
       </c>
       <c r="E26" t="n">
-        <v>14.1472526435387</v>
+        <v>50.7373254036727</v>
       </c>
       <c r="F26" t="n">
-        <v>5126.0561758177</v>
+        <v>300927.737288121</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>489063.539425863</v>
       </c>
       <c r="H26" t="n">
-        <v>30.8096778701923</v>
+        <v>43712.7240025002</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" t="s">
-        <v>11</v>
+        <v>4319.504178</v>
+      </c>
+      <c r="J26" t="n">
+        <v>43.3261238396236</v>
+      </c>
+      <c r="K26" t="n">
+        <v>38.7033981521308</v>
+      </c>
+      <c r="L26" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="27">
@@ -1220,31 +1388,37 @@
         <v>10</v>
       </c>
       <c r="B27" t="n">
-        <v>867.75766554</v>
+        <v>12117.939859348</v>
       </c>
       <c r="C27" t="n">
-        <v>293.89615833</v>
+        <v>5647.063745</v>
       </c>
       <c r="D27" t="n">
-        <v>43.3036348233734</v>
+        <v>49.4382821661371</v>
       </c>
       <c r="E27" t="n">
-        <v>14.1472533553139</v>
+        <v>50.6348891998656</v>
       </c>
       <c r="F27" t="n">
-        <v>6833.7186705736</v>
+        <v>327648.894587659</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>487617.283321047</v>
       </c>
       <c r="H27" t="n">
-        <v>40.0456563221751</v>
+        <v>54135.973846145</v>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" t="s">
-        <v>11</v>
+        <v>4302.755109</v>
+      </c>
+      <c r="J27" t="n">
+        <v>52.4689615473748</v>
+      </c>
+      <c r="K27" t="n">
+        <v>38.6009612904814</v>
+      </c>
+      <c r="L27" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="28">
@@ -1252,31 +1426,37 @@
         <v>11</v>
       </c>
       <c r="B28" t="n">
-        <v>3226.827568056</v>
+        <v>27761.9256227</v>
       </c>
       <c r="C28" t="n">
-        <v>293.89613076</v>
+        <v>5744.446926</v>
       </c>
       <c r="D28" t="n">
-        <v>63.8887757013138</v>
+        <v>71.2877197576623</v>
       </c>
       <c r="E28" t="n">
-        <v>14.1245568997883</v>
+        <v>51.4989934475539</v>
       </c>
       <c r="F28" t="n">
-        <v>10802.3300558487</v>
+        <v>417616.906715477</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>503101.142006486</v>
       </c>
       <c r="H28" t="n">
-        <v>60.1779959721545</v>
+        <v>77791.0292286628</v>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" t="s">
-        <v>11</v>
+        <v>4400.138424</v>
+      </c>
+      <c r="J28" t="n">
+        <v>73.4157137815196</v>
+      </c>
+      <c r="K28" t="n">
+        <v>39.4844116325389</v>
+      </c>
+      <c r="L28" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="29">
@@ -1284,31 +1464,37 @@
         <v>12</v>
       </c>
       <c r="B29" t="n">
-        <v>2909.3938274</v>
+        <v>24472.06069176</v>
       </c>
       <c r="C29" t="n">
-        <v>293.89614904</v>
+        <v>5917.944872</v>
       </c>
       <c r="D29" t="n">
-        <v>55.4941928131713</v>
+        <v>64.1822120764622</v>
       </c>
       <c r="E29" t="n">
-        <v>14.1245577726583</v>
+        <v>52.9795177173176</v>
       </c>
       <c r="F29" t="n">
-        <v>7313.3603627283</v>
+        <v>379618.155007707</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>518296.16702679</v>
       </c>
       <c r="H29" t="n">
-        <v>42.9768096681311</v>
+        <v>57907.2156753563</v>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
-      </c>
-      <c r="J29" t="s">
-        <v>11</v>
+        <v>4573.636293</v>
+      </c>
+      <c r="J29" t="n">
+        <v>57.7671898730524</v>
+      </c>
+      <c r="K29" t="n">
+        <v>40.9649352029195</v>
+      </c>
+      <c r="L29" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="30">
@@ -1316,31 +1502,37 @@
         <v>13</v>
       </c>
       <c r="B30" t="n">
-        <v>2267.22260482</v>
+        <v>21889.722123</v>
       </c>
       <c r="C30" t="n">
-        <v>293.89614248</v>
+        <v>5619.207819</v>
       </c>
       <c r="D30" t="n">
-        <v>58.3669128687196</v>
+        <v>67.540968812839</v>
       </c>
       <c r="E30" t="n">
-        <v>14.1245574822539</v>
+        <v>50.3839876701363</v>
       </c>
       <c r="F30" t="n">
-        <v>10535.4306318635</v>
+        <v>409962.245605398</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>492132.64694208</v>
       </c>
       <c r="H30" t="n">
-        <v>57.5792301997085</v>
+        <v>77323.7347515964</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
-      </c>
-      <c r="J30" t="s">
-        <v>11</v>
+        <v>4274.89929</v>
+      </c>
+      <c r="J30" t="n">
+        <v>73.4206159768654</v>
+      </c>
+      <c r="K30" t="n">
+        <v>38.3694056113146</v>
+      </c>
+      <c r="L30" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="31">
@@ -1348,31 +1540,37 @@
         <v>14</v>
       </c>
       <c r="B31" t="n">
-        <v>3389.746171417</v>
+        <v>29112.072347</v>
       </c>
       <c r="C31" t="n">
-        <v>293.89616024</v>
+        <v>5773.985992</v>
       </c>
       <c r="D31" t="n">
-        <v>52.1483683923263</v>
+        <v>61.2836289002466</v>
       </c>
       <c r="E31" t="n">
-        <v>14.1472533900588</v>
+        <v>51.860282639682</v>
       </c>
       <c r="F31" t="n">
-        <v>10251.5036307501</v>
+        <v>399174.897346415</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>498576.869412127</v>
       </c>
       <c r="H31" t="n">
-        <v>53.0008493281874</v>
+        <v>75088.843026052</v>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
-      </c>
-      <c r="J31" t="s">
-        <v>11</v>
+        <v>4429.677375</v>
+      </c>
+      <c r="J31" t="n">
+        <v>67.7271809432991</v>
+      </c>
+      <c r="K31" t="n">
+        <v>39.8263549331731</v>
+      </c>
+      <c r="L31" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="32">
@@ -1380,31 +1578,37 @@
         <v>15</v>
       </c>
       <c r="B32" t="n">
-        <v>-227.09393821</v>
+        <v>7432.8780636</v>
       </c>
       <c r="C32" t="n">
-        <v>293.89613573</v>
+        <v>4916.777897</v>
       </c>
       <c r="D32" t="n">
-        <v>53.7863561182953</v>
+        <v>61.709583780245</v>
       </c>
       <c r="E32" t="n">
-        <v>14.1472522315126</v>
+        <v>44.1874367512114</v>
       </c>
       <c r="F32" t="n">
-        <v>15491.3102920827</v>
+        <v>383016.825047318</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>424557.963056624</v>
       </c>
       <c r="H32" t="n">
-        <v>77.3810361989718</v>
+        <v>104436.356307479</v>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" t="s">
-        <v>11</v>
+        <v>3572.469213</v>
+      </c>
+      <c r="J32" t="n">
+        <v>92.8568541236453</v>
+      </c>
+      <c r="K32" t="n">
+        <v>32.1535083549023</v>
+      </c>
+      <c r="L32" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="33">
@@ -1412,31 +1616,1253 @@
         <v>16</v>
       </c>
       <c r="B33" t="n">
-        <v>9771.8432441</v>
+        <v>61420.96193581</v>
       </c>
       <c r="C33" t="n">
-        <v>293.89617009</v>
+        <v>6529.732686</v>
       </c>
       <c r="D33" t="n">
-        <v>78.764419805849</v>
+        <v>85.7922851761453</v>
       </c>
       <c r="E33" t="n">
-        <v>14.1472538826422</v>
+        <v>58.5492934473676</v>
       </c>
       <c r="F33" t="n">
-        <v>13422.7709757412</v>
+        <v>457108.845451775</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>563834.703650926</v>
       </c>
       <c r="H33" t="n">
-        <v>61.6678498723643</v>
+        <v>89082.5830168385</v>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
-      </c>
-      <c r="J33" t="s">
+        <v>5185.424042</v>
+      </c>
+      <c r="J33" t="n">
+        <v>74.3867678145332</v>
+      </c>
+      <c r="K33" t="n">
+        <v>46.5153654105036</v>
+      </c>
+      <c r="L33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1</v>
+      </c>
+      <c r="B34" t="n">
+        <v>-64.3772804</v>
+      </c>
+      <c r="C34" t="n">
+        <v>2109.97350786</v>
+      </c>
+      <c r="D34" t="n">
+        <v>30.5294900879817</v>
+      </c>
+      <c r="E34" t="n">
+        <v>102.510602155379</v>
+      </c>
+      <c r="F34" t="n">
+        <v>47319.4361747029</v>
+      </c>
+      <c r="G34" t="n">
+        <v>184792.390822377</v>
+      </c>
+      <c r="H34" t="n">
+        <v>2529.16017914569</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1816.07737098014</v>
+      </c>
+      <c r="J34" t="n">
+        <v>9.51917065356799</v>
+      </c>
+      <c r="K34" t="n">
+        <v>88.3860451304422</v>
+      </c>
+      <c r="L34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2</v>
+      </c>
+      <c r="B35" t="n">
+        <v>-178.187916255</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1580.90003854</v>
+      </c>
+      <c r="D35" t="n">
+        <v>31.8995860076216</v>
+      </c>
+      <c r="E35" t="n">
+        <v>77.3321558462802</v>
+      </c>
+      <c r="F35" t="n">
+        <v>47598.6027708911</v>
+      </c>
+      <c r="G35" t="n">
+        <v>138455.90794611</v>
+      </c>
+      <c r="H35" t="n">
+        <v>2521.11881163574</v>
+      </c>
+      <c r="I35" t="n">
+        <v>1287.0038841677</v>
+      </c>
+      <c r="J35" t="n">
+        <v>15.6279803108575</v>
+      </c>
+      <c r="K35" t="n">
+        <v>63.2075979046658</v>
+      </c>
+      <c r="L35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>3</v>
+      </c>
+      <c r="B36" t="n">
+        <v>-117.898311259</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1374.46742384</v>
+      </c>
+      <c r="D36" t="n">
+        <v>30.3592116359533</v>
+      </c>
+      <c r="E36" t="n">
+        <v>66.72803064856</v>
+      </c>
+      <c r="F36" t="n">
+        <v>46241.0010692274</v>
+      </c>
+      <c r="G36" t="n">
+        <v>120376.450421159</v>
+      </c>
+      <c r="H36" t="n">
+        <v>2171.42629957606</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1080.5712609843</v>
+      </c>
+      <c r="J36" t="n">
+        <v>10.5013610078282</v>
+      </c>
+      <c r="K36" t="n">
+        <v>52.6034721607589</v>
+      </c>
+      <c r="L36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>4</v>
+      </c>
+      <c r="B37" t="n">
+        <v>-401.2668456</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1281.7087638</v>
+      </c>
+      <c r="D37" t="n">
+        <v>30.8809313759158</v>
+      </c>
+      <c r="E37" t="n">
+        <v>62.3227211764989</v>
+      </c>
+      <c r="F37" t="n">
+        <v>48668.0054192861</v>
+      </c>
+      <c r="G37" t="n">
+        <v>112252.606925296</v>
+      </c>
+      <c r="H37" t="n">
+        <v>2965.21171576757</v>
+      </c>
+      <c r="I37" t="n">
+        <v>987.81262856462</v>
+      </c>
+      <c r="J37" t="n">
+        <v>19.1127050617248</v>
+      </c>
+      <c r="K37" t="n">
+        <v>48.198164044124</v>
+      </c>
+      <c r="L37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>5</v>
+      </c>
+      <c r="B38" t="n">
+        <v>-105.83629556</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1330.1573014</v>
+      </c>
+      <c r="D38" t="n">
+        <v>28.7475952573618</v>
+      </c>
+      <c r="E38" t="n">
+        <v>64.3889010001654</v>
+      </c>
+      <c r="F38" t="n">
+        <v>44342.6377586931</v>
+      </c>
+      <c r="G38" t="n">
+        <v>116495.750766486</v>
+      </c>
+      <c r="H38" t="n">
+        <v>2142.06295214739</v>
+      </c>
+      <c r="I38" t="n">
+        <v>1036.26116291667</v>
+      </c>
+      <c r="J38" t="n">
+        <v>8.60612409327883</v>
+      </c>
+      <c r="K38" t="n">
+        <v>50.2643437743682</v>
+      </c>
+      <c r="L38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>6</v>
+      </c>
+      <c r="B39" t="n">
+        <v>-342.57753472</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1094.31645402</v>
+      </c>
+      <c r="D39" t="n">
+        <v>31.0269353807736</v>
+      </c>
+      <c r="E39" t="n">
+        <v>52.8628290105597</v>
+      </c>
+      <c r="F39" t="n">
+        <v>45346.0215034122</v>
+      </c>
+      <c r="G39" t="n">
+        <v>94492.9330530789</v>
+      </c>
+      <c r="H39" t="n">
+        <v>2625.31581731824</v>
+      </c>
+      <c r="I39" t="n">
+        <v>800.4202732668</v>
+      </c>
+      <c r="J39" t="n">
+        <v>16.8807864172737</v>
+      </c>
+      <c r="K39" t="n">
+        <v>38.7155745127215</v>
+      </c>
+      <c r="L39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>7</v>
+      </c>
+      <c r="B40" t="n">
+        <v>-291.665022212</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1089.44321467</v>
+      </c>
+      <c r="D40" t="n">
+        <v>30.6578461082834</v>
+      </c>
+      <c r="E40" t="n">
+        <v>52.6458675040139</v>
+      </c>
+      <c r="F40" t="n">
+        <v>44916.1413997743</v>
+      </c>
+      <c r="G40" t="n">
+        <v>94072.1345921222</v>
+      </c>
+      <c r="H40" t="n">
+        <v>2746.2528246686</v>
+      </c>
+      <c r="I40" t="n">
+        <v>795.54703899072</v>
+      </c>
+      <c r="J40" t="n">
+        <v>14.5616778645056</v>
+      </c>
+      <c r="K40" t="n">
+        <v>38.4647188794018</v>
+      </c>
+      <c r="L40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>8</v>
+      </c>
+      <c r="B41" t="n">
+        <v>-429.481126746</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1041.96822101</v>
+      </c>
+      <c r="D41" t="n">
+        <v>28.1480529061108</v>
+      </c>
+      <c r="E41" t="n">
+        <v>50.3130887356167</v>
+      </c>
+      <c r="F41" t="n">
+        <v>50171.0468595344</v>
+      </c>
+      <c r="G41" t="n">
+        <v>89972.7249733323</v>
+      </c>
+      <c r="H41" t="n">
+        <v>4581.23745280582</v>
+      </c>
+      <c r="I41" t="n">
+        <v>748.07204671984</v>
+      </c>
+      <c r="J41" t="n">
+        <v>27.6021779609433</v>
+      </c>
+      <c r="K41" t="n">
+        <v>36.1658346612252</v>
+      </c>
+      <c r="L41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>9</v>
+      </c>
+      <c r="B42" t="n">
+        <v>-470.539472578</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1075.12231205</v>
+      </c>
+      <c r="D42" t="n">
+        <v>31.6400813324271</v>
+      </c>
+      <c r="E42" t="n">
+        <v>52.0264230709302</v>
+      </c>
+      <c r="F42" t="n">
+        <v>49922.500890885</v>
+      </c>
+      <c r="G42" t="n">
+        <v>92835.5415686324</v>
+      </c>
+      <c r="H42" t="n">
+        <v>4368.3335429612</v>
+      </c>
+      <c r="I42" t="n">
+        <v>781.2261764717</v>
+      </c>
+      <c r="J42" t="n">
+        <v>27.479545599953</v>
+      </c>
+      <c r="K42" t="n">
+        <v>37.8791709070342</v>
+      </c>
+      <c r="L42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>10</v>
+      </c>
+      <c r="B43" t="n">
+        <v>-562.65088883</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1120.20199518</v>
+      </c>
+      <c r="D43" t="n">
+        <v>37.1900564554788</v>
+      </c>
+      <c r="E43" t="n">
+        <v>54.456515719586</v>
+      </c>
+      <c r="F43" t="n">
+        <v>51835.8979977267</v>
+      </c>
+      <c r="G43" t="n">
+        <v>96728.1189528149</v>
+      </c>
+      <c r="H43" t="n">
+        <v>5426.9141796189</v>
+      </c>
+      <c r="I43" t="n">
+        <v>826.3058358483</v>
+      </c>
+      <c r="J43" t="n">
+        <v>34.0138954295134</v>
+      </c>
+      <c r="K43" t="n">
+        <v>40.309262321822</v>
+      </c>
+      <c r="L43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
         <v>11</v>
+      </c>
+      <c r="B44" t="n">
+        <v>-608.93018243</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1421.09476549</v>
+      </c>
+      <c r="D44" t="n">
+        <v>48.2485204091286</v>
+      </c>
+      <c r="E44" t="n">
+        <v>69.837867050281</v>
+      </c>
+      <c r="F44" t="n">
+        <v>57748.7240115068</v>
+      </c>
+      <c r="G44" t="n">
+        <v>124460.093134727</v>
+      </c>
+      <c r="H44" t="n">
+        <v>6988.90714459473</v>
+      </c>
+      <c r="I44" t="n">
+        <v>1127.19865573481</v>
+      </c>
+      <c r="J44" t="n">
+        <v>44.6179577092243</v>
+      </c>
+      <c r="K44" t="n">
+        <v>55.7133112090727</v>
+      </c>
+      <c r="L44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>12</v>
+      </c>
+      <c r="B45" t="n">
+        <v>-486.637527578</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1433.67323173</v>
+      </c>
+      <c r="D45" t="n">
+        <v>40.9744422185957</v>
+      </c>
+      <c r="E45" t="n">
+        <v>70.2604368080786</v>
+      </c>
+      <c r="F45" t="n">
+        <v>51918.3384889426</v>
+      </c>
+      <c r="G45" t="n">
+        <v>125561.720638916</v>
+      </c>
+      <c r="H45" t="n">
+        <v>3942.46287148064</v>
+      </c>
+      <c r="I45" t="n">
+        <v>1139.77708303009</v>
+      </c>
+      <c r="J45" t="n">
+        <v>28.5464985966722</v>
+      </c>
+      <c r="K45" t="n">
+        <v>56.1358790510155</v>
+      </c>
+      <c r="L45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>13</v>
+      </c>
+      <c r="B46" t="n">
+        <v>-641.77995094</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1293.96971283</v>
+      </c>
+      <c r="D46" t="n">
+        <v>46.261838524629</v>
+      </c>
+      <c r="E46" t="n">
+        <v>63.4464474354856</v>
+      </c>
+      <c r="F46" t="n">
+        <v>60023.9418728636</v>
+      </c>
+      <c r="G46" t="n">
+        <v>113326.426135141</v>
+      </c>
+      <c r="H46" t="n">
+        <v>7645.8934712822</v>
+      </c>
+      <c r="I46" t="n">
+        <v>1000.07356264392</v>
+      </c>
+      <c r="J46" t="n">
+        <v>45.5448177633257</v>
+      </c>
+      <c r="K46" t="n">
+        <v>49.3218895840806</v>
+      </c>
+      <c r="L46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>14</v>
+      </c>
+      <c r="B47" t="n">
+        <v>-589.59891455</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1359.74079552</v>
+      </c>
+      <c r="D47" t="n">
+        <v>34.3471299245332</v>
+      </c>
+      <c r="E47" t="n">
+        <v>66.834128246961</v>
+      </c>
+      <c r="F47" t="n">
+        <v>53225.5002740015</v>
+      </c>
+      <c r="G47" t="n">
+        <v>117412.011387214</v>
+      </c>
+      <c r="H47" t="n">
+        <v>6296.27529205534</v>
+      </c>
+      <c r="I47" t="n">
+        <v>1065.84462763463</v>
+      </c>
+      <c r="J47" t="n">
+        <v>35.2806189234038</v>
+      </c>
+      <c r="K47" t="n">
+        <v>52.6868745376419</v>
+      </c>
+      <c r="L47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>15</v>
+      </c>
+      <c r="B48" t="n">
+        <v>-809.1596098</v>
+      </c>
+      <c r="C48" t="n">
+        <v>847.71650831</v>
+      </c>
+      <c r="D48" t="n">
+        <v>51.4998674995846</v>
+      </c>
+      <c r="E48" t="n">
+        <v>41.1137036774873</v>
+      </c>
+      <c r="F48" t="n">
+        <v>68356.7042621477</v>
+      </c>
+      <c r="G48" t="n">
+        <v>73199.3190575408</v>
+      </c>
+      <c r="H48" t="n">
+        <v>14925.0356490264</v>
+      </c>
+      <c r="I48" t="n">
+        <v>553.8203714833</v>
+      </c>
+      <c r="J48" t="n">
+        <v>75.1518529256129</v>
+      </c>
+      <c r="K48" t="n">
+        <v>26.9664513892842</v>
+      </c>
+      <c r="L48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>16</v>
+      </c>
+      <c r="B49" t="n">
+        <v>-436.047479559</v>
+      </c>
+      <c r="C49" t="n">
+        <v>2189.08371792</v>
+      </c>
+      <c r="D49" t="n">
+        <v>30.2596353398219</v>
+      </c>
+      <c r="E49" t="n">
+        <v>107.632350620382</v>
+      </c>
+      <c r="F49" t="n">
+        <v>48118.2502217115</v>
+      </c>
+      <c r="G49" t="n">
+        <v>189024.793006739</v>
+      </c>
+      <c r="H49" t="n">
+        <v>3253.3613152666</v>
+      </c>
+      <c r="I49" t="n">
+        <v>1895.1876262228</v>
+      </c>
+      <c r="J49" t="n">
+        <v>13.3046884508655</v>
+      </c>
+      <c r="K49" t="n">
+        <v>93.4851007054751</v>
+      </c>
+      <c r="L49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1</v>
+      </c>
+      <c r="B50" t="n">
+        <v>8258.4571149</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1328.78917726</v>
+      </c>
+      <c r="D50" t="n">
+        <v>65.0195657311147</v>
+      </c>
+      <c r="E50" t="n">
+        <v>63.9254211578953</v>
+      </c>
+      <c r="F50" t="n">
+        <v>74288.8805150984</v>
+      </c>
+      <c r="G50" t="n">
+        <v>116375.929863603</v>
+      </c>
+      <c r="H50" t="n">
+        <v>10825.3347131744</v>
+      </c>
+      <c r="I50" t="n">
+        <v>1034.89303802</v>
+      </c>
+      <c r="J50" t="n">
+        <v>43.9068809473274</v>
+      </c>
+      <c r="K50" t="n">
+        <v>49.8008639104389</v>
+      </c>
+      <c r="L50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>2</v>
+      </c>
+      <c r="B51" t="n">
+        <v>4608.53912775</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1181.25209414</v>
+      </c>
+      <c r="D51" t="n">
+        <v>50.9701352671052</v>
+      </c>
+      <c r="E51" t="n">
+        <v>56.9669867387733</v>
+      </c>
+      <c r="F51" t="n">
+        <v>65261.5844954745</v>
+      </c>
+      <c r="G51" t="n">
+        <v>103454.568423214</v>
+      </c>
+      <c r="H51" t="n">
+        <v>7293.473423777</v>
+      </c>
+      <c r="I51" t="n">
+        <v>887.35592234</v>
+      </c>
+      <c r="J51" t="n">
+        <v>34.6422812339047</v>
+      </c>
+      <c r="K51" t="n">
+        <v>42.8424278851332</v>
+      </c>
+      <c r="L51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>3</v>
+      </c>
+      <c r="B52" t="n">
+        <v>2105.121545265</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1180.28488744</v>
+      </c>
+      <c r="D52" t="n">
+        <v>39.5586356022753</v>
+      </c>
+      <c r="E52" t="n">
+        <v>56.8230823603711</v>
+      </c>
+      <c r="F52" t="n">
+        <v>55238.0825473633</v>
+      </c>
+      <c r="G52" t="n">
+        <v>103369.860042826</v>
+      </c>
+      <c r="H52" t="n">
+        <v>4384.8393753676</v>
+      </c>
+      <c r="I52" t="n">
+        <v>886.38872916</v>
+      </c>
+      <c r="J52" t="n">
+        <v>19.6621832883062</v>
+      </c>
+      <c r="K52" t="n">
+        <v>42.6985241518383</v>
+      </c>
+      <c r="L52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>4</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1789.57090256</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1107.1874831</v>
+      </c>
+      <c r="D53" t="n">
+        <v>41.9567789875829</v>
+      </c>
+      <c r="E53" t="n">
+        <v>53.4144432284655</v>
+      </c>
+      <c r="F53" t="n">
+        <v>57330.1049567581</v>
+      </c>
+      <c r="G53" t="n">
+        <v>96967.9578101296</v>
+      </c>
+      <c r="H53" t="n">
+        <v>5148.134068229</v>
+      </c>
+      <c r="I53" t="n">
+        <v>813.29133789</v>
+      </c>
+      <c r="J53" t="n">
+        <v>30.1613083051692</v>
+      </c>
+      <c r="K53" t="n">
+        <v>39.289885624116</v>
+      </c>
+      <c r="L53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>5</v>
+      </c>
+      <c r="B54" t="n">
+        <v>2205.000093744</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1161.1911062</v>
+      </c>
+      <c r="D54" t="n">
+        <v>38.4447252645657</v>
+      </c>
+      <c r="E54" t="n">
+        <v>55.8479862847407</v>
+      </c>
+      <c r="F54" t="n">
+        <v>53413.6232396594</v>
+      </c>
+      <c r="G54" t="n">
+        <v>101697.618437879</v>
+      </c>
+      <c r="H54" t="n">
+        <v>4441.1625472791</v>
+      </c>
+      <c r="I54" t="n">
+        <v>867.2949263</v>
+      </c>
+      <c r="J54" t="n">
+        <v>18.2583930264168</v>
+      </c>
+      <c r="K54" t="n">
+        <v>41.7234270269359</v>
+      </c>
+      <c r="L54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>6</v>
+      </c>
+      <c r="B55" t="n">
+        <v>227.307412314</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1058.35661922</v>
+      </c>
+      <c r="D55" t="n">
+        <v>33.8165835321145</v>
+      </c>
+      <c r="E55" t="n">
+        <v>51.0161440534564</v>
+      </c>
+      <c r="F55" t="n">
+        <v>47721.0270717892</v>
+      </c>
+      <c r="G55" t="n">
+        <v>91387.843798619</v>
+      </c>
+      <c r="H55" t="n">
+        <v>3191.4987101027</v>
+      </c>
+      <c r="I55" t="n">
+        <v>764.46045407</v>
+      </c>
+      <c r="J55" t="n">
+        <v>19.6558107601317</v>
+      </c>
+      <c r="K55" t="n">
+        <v>36.8688903672142</v>
+      </c>
+      <c r="L55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>7</v>
+      </c>
+      <c r="B56" t="n">
+        <v>-29.143622614</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1075.48238307</v>
+      </c>
+      <c r="D56" t="n">
+        <v>32.0100322190701</v>
+      </c>
+      <c r="E56" t="n">
+        <v>51.9219771661029</v>
+      </c>
+      <c r="F56" t="n">
+        <v>46031.0177095372</v>
+      </c>
+      <c r="G56" t="n">
+        <v>92866.6332758458</v>
+      </c>
+      <c r="H56" t="n">
+        <v>3007.114908791</v>
+      </c>
+      <c r="I56" t="n">
+        <v>781.58620879</v>
+      </c>
+      <c r="J56" t="n">
+        <v>15.9073743682145</v>
+      </c>
+      <c r="K56" t="n">
+        <v>37.7408286144227</v>
+      </c>
+      <c r="L56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>8</v>
+      </c>
+      <c r="B57" t="n">
+        <v>79.726635245</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1026.47003241</v>
+      </c>
+      <c r="D57" t="n">
+        <v>30.8209653308786</v>
+      </c>
+      <c r="E57" t="n">
+        <v>49.5157372603914</v>
+      </c>
+      <c r="F57" t="n">
+        <v>52182.261167194</v>
+      </c>
+      <c r="G57" t="n">
+        <v>88634.4746962355</v>
+      </c>
+      <c r="H57" t="n">
+        <v>5088.2789614688</v>
+      </c>
+      <c r="I57" t="n">
+        <v>732.57386334</v>
+      </c>
+      <c r="J57" t="n">
+        <v>30.26670334708</v>
+      </c>
+      <c r="K57" t="n">
+        <v>35.3684834509751</v>
+      </c>
+      <c r="L57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>9</v>
+      </c>
+      <c r="B58" t="n">
+        <v>443.87846584</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1026.00030815</v>
+      </c>
+      <c r="D58" t="n">
+        <v>35.9577626154439</v>
+      </c>
+      <c r="E58" t="n">
+        <v>49.5092849118198</v>
+      </c>
+      <c r="F58" t="n">
+        <v>53571.8963520385</v>
+      </c>
+      <c r="G58" t="n">
+        <v>88593.914561285</v>
+      </c>
+      <c r="H58" t="n">
+        <v>5278.3648292043</v>
+      </c>
+      <c r="I58" t="n">
+        <v>732.10416345</v>
+      </c>
+      <c r="J58" t="n">
+        <v>31.779855167847</v>
+      </c>
+      <c r="K58" t="n">
+        <v>35.3620322682811</v>
+      </c>
+      <c r="L58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>10</v>
+      </c>
+      <c r="B59" t="n">
+        <v>1139.203523219</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1019.49318628</v>
+      </c>
+      <c r="D59" t="n">
+        <v>44.9001949912408</v>
+      </c>
+      <c r="E59" t="n">
+        <v>49.2692583060921</v>
+      </c>
+      <c r="F59" t="n">
+        <v>58805.459900072</v>
+      </c>
+      <c r="G59" t="n">
+        <v>88032.0322748848</v>
+      </c>
+      <c r="H59" t="n">
+        <v>7122.1085625549</v>
+      </c>
+      <c r="I59" t="n">
+        <v>725.59702795</v>
+      </c>
+      <c r="J59" t="n">
+        <v>41.6979987959261</v>
+      </c>
+      <c r="K59" t="n">
+        <v>35.1220049507782</v>
+      </c>
+      <c r="L59" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>11</v>
+      </c>
+      <c r="B60" t="n">
+        <v>3969.46783926</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1069.76081079</v>
+      </c>
+      <c r="D60" t="n">
+        <v>67.4050831953612</v>
+      </c>
+      <c r="E60" t="n">
+        <v>51.8209032565899</v>
+      </c>
+      <c r="F60" t="n">
+        <v>75602.7157132169</v>
+      </c>
+      <c r="G60" t="n">
+        <v>93690.1136898472</v>
+      </c>
+      <c r="H60" t="n">
+        <v>11555.9107257463</v>
+      </c>
+      <c r="I60" t="n">
+        <v>775.86468003</v>
+      </c>
+      <c r="J60" t="n">
+        <v>63.7279721857703</v>
+      </c>
+      <c r="K60" t="n">
+        <v>37.6963463568015</v>
+      </c>
+      <c r="L60" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>12</v>
+      </c>
+      <c r="B61" t="n">
+        <v>3501.320827441</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1107.70706023</v>
+      </c>
+      <c r="D61" t="n">
+        <v>58.3894615491085</v>
+      </c>
+      <c r="E61" t="n">
+        <v>53.5479610122171</v>
+      </c>
+      <c r="F61" t="n">
+        <v>67714.3610813534</v>
+      </c>
+      <c r="G61" t="n">
+        <v>97013.4625995081</v>
+      </c>
+      <c r="H61" t="n">
+        <v>7919.531663948</v>
+      </c>
+      <c r="I61" t="n">
+        <v>813.81091119</v>
+      </c>
+      <c r="J61" t="n">
+        <v>45.9175732204687</v>
+      </c>
+      <c r="K61" t="n">
+        <v>39.4234032395588</v>
+      </c>
+      <c r="L61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>13</v>
+      </c>
+      <c r="B62" t="n">
+        <v>2900.84930507</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1034.58997803</v>
+      </c>
+      <c r="D62" t="n">
+        <v>61.4973152628231</v>
+      </c>
+      <c r="E62" t="n">
+        <v>50.1147803875143</v>
+      </c>
+      <c r="F62" t="n">
+        <v>74013.3742364495</v>
+      </c>
+      <c r="G62" t="n">
+        <v>90609.836971337</v>
+      </c>
+      <c r="H62" t="n">
+        <v>11179.6821328472</v>
+      </c>
+      <c r="I62" t="n">
+        <v>740.69383555</v>
+      </c>
+      <c r="J62" t="n">
+        <v>60.7424368239093</v>
+      </c>
+      <c r="K62" t="n">
+        <v>35.9902229052603</v>
+      </c>
+      <c r="L62" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>14</v>
+      </c>
+      <c r="B63" t="n">
+        <v>4267.09104502</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1030.46181732</v>
+      </c>
+      <c r="D63" t="n">
+        <v>56.1882413883208</v>
+      </c>
+      <c r="E63" t="n">
+        <v>49.920815174173</v>
+      </c>
+      <c r="F63" t="n">
+        <v>72869.0238984282</v>
+      </c>
+      <c r="G63" t="n">
+        <v>88979.1606075889</v>
+      </c>
+      <c r="H63" t="n">
+        <v>11140.7236489092</v>
+      </c>
+      <c r="I63" t="n">
+        <v>736.56565708</v>
+      </c>
+      <c r="J63" t="n">
+        <v>57.0779875603305</v>
+      </c>
+      <c r="K63" t="n">
+        <v>35.7735617841142</v>
+      </c>
+      <c r="L63" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>15</v>
+      </c>
+      <c r="B64" t="n">
+        <v>151.0818007</v>
+      </c>
+      <c r="C64" t="n">
+        <v>843.41277021</v>
+      </c>
+      <c r="D64" t="n">
+        <v>56.2098101963724</v>
+      </c>
+      <c r="E64" t="n">
+        <v>40.8915209502375</v>
+      </c>
+      <c r="F64" t="n">
+        <v>71271.4190562468</v>
+      </c>
+      <c r="G64" t="n">
+        <v>72827.6963567513</v>
+      </c>
+      <c r="H64" t="n">
+        <v>15884.4790040952</v>
+      </c>
+      <c r="I64" t="n">
+        <v>549.51663448</v>
+      </c>
+      <c r="J64" t="n">
+        <v>79.8586770822312</v>
+      </c>
+      <c r="K64" t="n">
+        <v>26.744268718725</v>
+      </c>
+      <c r="L64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>16</v>
+      </c>
+      <c r="B65" t="n">
+        <v>11250.1492971</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1247.39889322</v>
+      </c>
+      <c r="D65" t="n">
+        <v>85.5205283965017</v>
+      </c>
+      <c r="E65" t="n">
+        <v>60.3360520595744</v>
+      </c>
+      <c r="F65" t="n">
+        <v>85315.9997534122</v>
+      </c>
+      <c r="G65" t="n">
+        <v>107711.420836745</v>
+      </c>
+      <c r="H65" t="n">
+        <v>14916.3700450375</v>
+      </c>
+      <c r="I65" t="n">
+        <v>953.50272313</v>
+      </c>
+      <c r="J65" t="n">
+        <v>68.4760140985721</v>
+      </c>
+      <c r="K65" t="n">
+        <v>46.1887981769321</v>
+      </c>
+      <c r="L65" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1455,7 +2881,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated LRLC Runs and Results
</commit_message>
<xml_diff>
--- a/framework/analysis/lr/TDVAnnual.xlsx
+++ b/framework/analysis/lr/TDVAnnual.xlsx
@@ -51,19 +51,19 @@
     <t xml:space="preserve">Measure</t>
   </si>
   <si>
+    <t xml:space="preserve">lrgs-low-baseszac</t>
+  </si>
+  <si>
     <t xml:space="preserve">lrlc-baseline-all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lrgs-low-base</t>
   </si>
   <si>
     <t xml:space="preserve">lrlc-flat19-base</t>
   </si>
   <si>
-    <t xml:space="preserve">lrgs-low-baseszac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lrgs-low-base</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LifeTime: ,30,TDVMultiplier: ,res,DHW Removed: ,FALSE</t>
+    <t xml:space="preserve">LifeTime: ,30,TDVMultiplier: ,res,DHW Removed: ,FALSE,PVB Removed: ,TRUE</t>
   </si>
 </sst>
 </file>
@@ -438,34 +438,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>22828.66470122</v>
+        <v>22412.338059469</v>
       </c>
       <c r="C2" t="n">
-        <v>8696.770195</v>
+        <v>2109.97350786</v>
       </c>
       <c r="D2" t="n">
-        <v>48.6544565957884</v>
+        <v>88.2884163202638</v>
       </c>
       <c r="E2" t="n">
-        <v>78.2650760720572</v>
+        <v>102.510602155379</v>
       </c>
       <c r="F2" t="n">
-        <v>320987.265577084</v>
+        <v>59114.4892718639</v>
       </c>
       <c r="G2" t="n">
-        <v>761666.888603171</v>
+        <v>184792.390822377</v>
       </c>
       <c r="H2" t="n">
-        <v>42586.8161831916</v>
+        <v>2529.16017914569</v>
       </c>
       <c r="I2" t="n">
-        <v>7352.46149568424</v>
+        <v>1816.07737098014</v>
       </c>
       <c r="J2" t="n">
-        <v>31.8627964983222</v>
+        <v>9.51917065356799</v>
       </c>
       <c r="K2" t="n">
-        <v>66.2504924891521</v>
+        <v>88.3860451304422</v>
       </c>
       <c r="L2" t="s">
         <v>12</v>
@@ -476,34 +476,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>13735.97324775</v>
+        <v>22543.519555299</v>
       </c>
       <c r="C3" t="n">
-        <v>7341.997463</v>
+        <v>1580.90003854</v>
       </c>
       <c r="D3" t="n">
-        <v>44.6929948508488</v>
+        <v>92.6769216449942</v>
       </c>
       <c r="E3" t="n">
-        <v>66.2800542546027</v>
+        <v>77.3321558462802</v>
       </c>
       <c r="F3" t="n">
-        <v>303886.28683166</v>
+        <v>59800.5719615755</v>
       </c>
       <c r="G3" t="n">
-        <v>643015.307796756</v>
+        <v>138455.90794611</v>
       </c>
       <c r="H3" t="n">
-        <v>35232.7420231726</v>
+        <v>2521.11881163574</v>
       </c>
       <c r="I3" t="n">
-        <v>5997.6890156942</v>
+        <v>1287.0038841677</v>
       </c>
       <c r="J3" t="n">
-        <v>32.916111155739</v>
+        <v>15.6279803108575</v>
       </c>
       <c r="K3" t="n">
-        <v>54.2654728395149</v>
+        <v>63.2075979046658</v>
       </c>
       <c r="L3" t="s">
         <v>12</v>
@@ -514,34 +514,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>9771.5712423</v>
+        <v>22162.690861452</v>
       </c>
       <c r="C4" t="n">
-        <v>6625.982674</v>
+        <v>1374.46742384</v>
       </c>
       <c r="D4" t="n">
-        <v>39.0981204970025</v>
+        <v>88.60930678235</v>
       </c>
       <c r="E4" t="n">
-        <v>59.4585968502382</v>
+        <v>66.72803064856</v>
       </c>
       <c r="F4" t="n">
-        <v>282809.245132173</v>
+        <v>58644.3115179705</v>
       </c>
       <c r="G4" t="n">
-        <v>580306.423428968</v>
+        <v>120376.450421159</v>
       </c>
       <c r="H4" t="n">
-        <v>28498.1004077125</v>
+        <v>2171.42629957606</v>
       </c>
       <c r="I4" t="n">
-        <v>5281.6741805551</v>
+        <v>1080.5712609843</v>
       </c>
       <c r="J4" t="n">
-        <v>23.5884503389445</v>
+        <v>10.5013610078282</v>
       </c>
       <c r="K4" t="n">
-        <v>47.4440151078061</v>
+        <v>52.6034721607589</v>
       </c>
       <c r="L4" t="s">
         <v>12</v>
@@ -552,34 +552,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>7589.46405997</v>
+        <v>23103.489031248</v>
       </c>
       <c r="C5" t="n">
-        <v>6375.030487</v>
+        <v>1281.7087638</v>
       </c>
       <c r="D5" t="n">
-        <v>40.9924438776492</v>
+        <v>96.2718150811335</v>
       </c>
       <c r="E5" t="n">
-        <v>57.279707155273</v>
+        <v>62.3227211764989</v>
       </c>
       <c r="F5" t="n">
-        <v>297628.713179168</v>
+        <v>61743.3095376734</v>
       </c>
       <c r="G5" t="n">
-        <v>558327.922540173</v>
+        <v>112252.606925296</v>
       </c>
       <c r="H5" t="n">
-        <v>35134.3757147033</v>
+        <v>2965.21171576757</v>
       </c>
       <c r="I5" t="n">
-        <v>5030.7218267762</v>
+        <v>987.81262856462</v>
       </c>
       <c r="J5" t="n">
-        <v>35.2501284085163</v>
+        <v>19.1127050617248</v>
       </c>
       <c r="K5" t="n">
-        <v>45.265123941294</v>
+        <v>48.198164044124</v>
       </c>
       <c r="L5" t="s">
         <v>12</v>
@@ -590,34 +590,34 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>10328.69193727</v>
+        <v>22153.317999506</v>
       </c>
       <c r="C6" t="n">
-        <v>6554.546615</v>
+        <v>1330.1573014</v>
       </c>
       <c r="D6" t="n">
-        <v>37.6707374426873</v>
+        <v>87.49378582589</v>
       </c>
       <c r="E6" t="n">
-        <v>58.7383453960818</v>
+        <v>64.3889010001654</v>
       </c>
       <c r="F6" t="n">
-        <v>274106.989041872</v>
+        <v>58582.3834437173</v>
       </c>
       <c r="G6" t="n">
-        <v>574050.022538453</v>
+        <v>116495.750766486</v>
       </c>
       <c r="H6" t="n">
-        <v>28949.4752215308</v>
+        <v>2142.06295214739</v>
       </c>
       <c r="I6" t="n">
-        <v>5210.237931358</v>
+        <v>1036.26116291667</v>
       </c>
       <c r="J6" t="n">
-        <v>22.1835100841028</v>
+        <v>8.60612409327883</v>
       </c>
       <c r="K6" t="n">
-        <v>46.7237619116295</v>
+        <v>50.2643437743682</v>
       </c>
       <c r="L6" t="s">
         <v>12</v>
@@ -628,34 +628,34 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>137982.19015</v>
+        <v>22824.736391637</v>
       </c>
       <c r="C7" t="n">
-        <v>5810.479147</v>
+        <v>1094.31645402</v>
       </c>
       <c r="D7" t="n">
-        <v>106.695609919442</v>
+        <v>94.8985928965348</v>
       </c>
       <c r="E7" t="n">
-        <v>52.0435003408487</v>
+        <v>52.8628290105597</v>
       </c>
       <c r="F7" t="n">
-        <v>359662.3957553</v>
+        <v>61068.3480344425</v>
       </c>
       <c r="G7" t="n">
-        <v>501728.010235828</v>
+        <v>94492.9330530789</v>
       </c>
       <c r="H7" t="n">
-        <v>30949.3851436631</v>
+        <v>2625.31581731824</v>
       </c>
       <c r="I7" t="n">
-        <v>4466.1702918795</v>
+        <v>800.4202732668</v>
       </c>
       <c r="J7" t="n">
-        <v>30.6945074197909</v>
+        <v>16.8807864172737</v>
       </c>
       <c r="K7" t="n">
-        <v>40.0095705356774</v>
+        <v>38.7155745127215</v>
       </c>
       <c r="L7" t="s">
         <v>12</v>
@@ -666,34 +666,34 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>136360.83874</v>
+        <v>22972.210245018</v>
       </c>
       <c r="C8" t="n">
-        <v>5760.495689</v>
+        <v>1089.44321467</v>
       </c>
       <c r="D8" t="n">
-        <v>102.546228153802</v>
+        <v>93.2347998011782</v>
       </c>
       <c r="E8" t="n">
-        <v>51.6950752895751</v>
+        <v>52.6458675040139</v>
       </c>
       <c r="F8" t="n">
-        <v>356757.074418852</v>
+        <v>61667.3231348664</v>
       </c>
       <c r="G8" t="n">
-        <v>497411.99768461</v>
+        <v>94072.1345921222</v>
       </c>
       <c r="H8" t="n">
-        <v>29093.0850377257</v>
+        <v>2746.2528246686</v>
       </c>
       <c r="I8" t="n">
-        <v>4416.187017021</v>
+        <v>795.54703899072</v>
       </c>
       <c r="J8" t="n">
-        <v>25.9811005159642</v>
+        <v>14.5616778645056</v>
       </c>
       <c r="K8" t="n">
-        <v>39.6322285929515</v>
+        <v>38.4647188794018</v>
       </c>
       <c r="L8" t="s">
         <v>12</v>
@@ -704,34 +704,34 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>2849.42372902</v>
+        <v>24891.113121748</v>
       </c>
       <c r="C9" t="n">
-        <v>5649.62038</v>
+        <v>1041.96822101</v>
       </c>
       <c r="D9" t="n">
-        <v>33.0278471158291</v>
+        <v>103.665282581345</v>
       </c>
       <c r="E9" t="n">
-        <v>50.614321783342</v>
+        <v>50.3130887356167</v>
       </c>
       <c r="F9" t="n">
-        <v>284191.940232869</v>
+        <v>67358.1377059218</v>
       </c>
       <c r="G9" t="n">
-        <v>487838.045733061</v>
+        <v>89972.7249733323</v>
       </c>
       <c r="H9" t="n">
-        <v>39993.7012375079</v>
+        <v>4581.23745280582</v>
       </c>
       <c r="I9" t="n">
-        <v>4305.311699464</v>
+        <v>748.07204671984</v>
       </c>
       <c r="J9" t="n">
-        <v>38.9201490411927</v>
+        <v>27.6021779609433</v>
       </c>
       <c r="K9" t="n">
-        <v>38.5803935371693</v>
+        <v>36.1658346612252</v>
       </c>
       <c r="L9" t="s">
         <v>12</v>
@@ -742,34 +742,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>4146.0636342</v>
+        <v>24637.782387486</v>
       </c>
       <c r="C10" t="n">
-        <v>5770.703551</v>
+        <v>1075.12231205</v>
       </c>
       <c r="D10" t="n">
-        <v>38.3855819107565</v>
+        <v>103.402841217832</v>
       </c>
       <c r="E10" t="n">
-        <v>51.7548839427498</v>
+        <v>52.0264230709302</v>
       </c>
       <c r="F10" t="n">
-        <v>288714.10107434</v>
+        <v>66766.1146227962</v>
       </c>
       <c r="G10" t="n">
-        <v>498293.434509431</v>
+        <v>92835.5415686324</v>
       </c>
       <c r="H10" t="n">
-        <v>40566.4232453719</v>
+        <v>4368.3335429612</v>
       </c>
       <c r="I10" t="n">
-        <v>4426.394947388</v>
+        <v>781.2261764717</v>
       </c>
       <c r="J10" t="n">
-        <v>40.4635656667657</v>
+        <v>27.479545599953</v>
       </c>
       <c r="K10" t="n">
-        <v>39.7209563184306</v>
+        <v>37.8791709070342</v>
       </c>
       <c r="L10" t="s">
         <v>12</v>
@@ -780,34 +780,34 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>6078.639046693</v>
+        <v>25699.259990046</v>
       </c>
       <c r="C11" t="n">
-        <v>5928.14455</v>
+        <v>1120.20199518</v>
       </c>
       <c r="D11" t="n">
-        <v>44.2677362795241</v>
+        <v>110.578477409453</v>
       </c>
       <c r="E11" t="n">
-        <v>53.3281616110487</v>
+        <v>54.456515719586</v>
       </c>
       <c r="F11" t="n">
-        <v>303345.350280852</v>
+        <v>69676.7140988046</v>
       </c>
       <c r="G11" t="n">
-        <v>511888.278782919</v>
+        <v>96728.1189528149</v>
       </c>
       <c r="H11" t="n">
-        <v>48118.6978464883</v>
+        <v>5426.9141796189</v>
       </c>
       <c r="I11" t="n">
-        <v>4583.835910441</v>
+        <v>826.3058358483</v>
       </c>
       <c r="J11" t="n">
-        <v>47.3143877531963</v>
+        <v>34.0138954295134</v>
       </c>
       <c r="K11" t="n">
-        <v>41.2942336632156</v>
+        <v>40.309262321822</v>
       </c>
       <c r="L11" t="s">
         <v>12</v>
@@ -818,34 +818,34 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>168927.06621</v>
+        <v>27196.29254902</v>
       </c>
       <c r="C12" t="n">
-        <v>6840.718989</v>
+        <v>1421.09476549</v>
       </c>
       <c r="D12" t="n">
-        <v>136.504636442762</v>
+        <v>122.230661607986</v>
       </c>
       <c r="E12" t="n">
-        <v>61.9669056801819</v>
+        <v>69.837867050281</v>
       </c>
       <c r="F12" t="n">
-        <v>441881.929519526</v>
+        <v>73012.0443149839</v>
       </c>
       <c r="G12" t="n">
-        <v>599113.122611406</v>
+        <v>124460.093134727</v>
       </c>
       <c r="H12" t="n">
-        <v>61895.6682311594</v>
+        <v>6988.90714459473</v>
       </c>
       <c r="I12" t="n">
-        <v>5496.4104890889</v>
+        <v>1127.19865573481</v>
       </c>
       <c r="J12" t="n">
-        <v>60.9481537796566</v>
+        <v>44.6179577092243</v>
       </c>
       <c r="K12" t="n">
-        <v>49.95232388295</v>
+        <v>55.7133112090727</v>
       </c>
       <c r="L12" t="s">
         <v>12</v>
@@ -856,34 +856,34 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>10780.8973734</v>
+        <v>24091.675496012</v>
       </c>
       <c r="C13" t="n">
-        <v>6914.970738</v>
+        <v>1433.67323173</v>
       </c>
       <c r="D13" t="n">
-        <v>52.6795034206022</v>
+        <v>106.063459218684</v>
       </c>
       <c r="E13" t="n">
-        <v>62.4991409877888</v>
+        <v>70.2604368080786</v>
       </c>
       <c r="F13" t="n">
-        <v>325624.16878777</v>
+        <v>64778.6269724753</v>
       </c>
       <c r="G13" t="n">
-        <v>605616.122847826</v>
+        <v>125561.720638916</v>
       </c>
       <c r="H13" t="n">
-        <v>44251.9394230849</v>
+        <v>3942.46287148064</v>
       </c>
       <c r="I13" t="n">
-        <v>5570.662225892</v>
+        <v>1139.77708303009</v>
       </c>
       <c r="J13" t="n">
-        <v>46.290917311368</v>
+        <v>28.5464985966722</v>
       </c>
       <c r="K13" t="n">
-        <v>50.4845590993907</v>
+        <v>56.1358790510155</v>
       </c>
       <c r="L13" t="s">
         <v>12</v>
@@ -894,34 +894,34 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>9582.03940256</v>
+        <v>27895.3627617635</v>
       </c>
       <c r="C14" t="n">
-        <v>6393.784235</v>
+        <v>1293.96971283</v>
       </c>
       <c r="D14" t="n">
-        <v>57.594717061715</v>
+        <v>123.036424866407</v>
       </c>
       <c r="E14" t="n">
-        <v>57.7931467903642</v>
+        <v>63.4464474354856</v>
       </c>
       <c r="F14" t="n">
-        <v>362131.625882005</v>
+        <v>75546.1545320567</v>
       </c>
       <c r="G14" t="n">
-        <v>559970.383887148</v>
+        <v>113326.426135141</v>
       </c>
       <c r="H14" t="n">
-        <v>65045.247717797</v>
+        <v>7645.8934712822</v>
       </c>
       <c r="I14" t="n">
-        <v>5049.4757180326</v>
+        <v>1000.07356264392</v>
       </c>
       <c r="J14" t="n">
-        <v>63.4976705978154</v>
+        <v>45.5448177633257</v>
       </c>
       <c r="K14" t="n">
-        <v>45.7785648282996</v>
+        <v>49.3218895840806</v>
       </c>
       <c r="L14" t="s">
         <v>12</v>
@@ -932,34 +932,34 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>165480.29325</v>
+        <v>26492.45677319</v>
       </c>
       <c r="C15" t="n">
-        <v>6754.363389</v>
+        <v>1359.74079552</v>
       </c>
       <c r="D15" t="n">
-        <v>127.200380531781</v>
+        <v>110.557331935402</v>
       </c>
       <c r="E15" t="n">
-        <v>61.2338668307596</v>
+        <v>66.834128246961</v>
       </c>
       <c r="F15" t="n">
-        <v>438295.988692234</v>
+        <v>71822.0066868266</v>
       </c>
       <c r="G15" t="n">
-        <v>583231.299491435</v>
+        <v>117412.011387214</v>
       </c>
       <c r="H15" t="n">
-        <v>58819.8813587715</v>
+        <v>6296.27529205534</v>
       </c>
       <c r="I15" t="n">
-        <v>5410.0548007928</v>
+        <v>1065.84462763463</v>
       </c>
       <c r="J15" t="n">
-        <v>53.792049413419</v>
+        <v>35.2806189234038</v>
       </c>
       <c r="K15" t="n">
-        <v>49.1999394187638</v>
+        <v>52.6868745376419</v>
       </c>
       <c r="L15" t="s">
         <v>12</v>
@@ -970,34 +970,34 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>208205.55534</v>
+        <v>35387.785734647</v>
       </c>
       <c r="C16" t="n">
-        <v>4919.170673</v>
+        <v>847.71650831</v>
       </c>
       <c r="D16" t="n">
-        <v>163.518263935285</v>
+        <v>151.824172414797</v>
       </c>
       <c r="E16" t="n">
-        <v>44.2103882820078</v>
+        <v>41.1137036774873</v>
       </c>
       <c r="F16" t="n">
-        <v>514813.13414919</v>
+        <v>93769.1497170609</v>
       </c>
       <c r="G16" t="n">
-        <v>424764.57643756</v>
+        <v>73199.3190575408</v>
       </c>
       <c r="H16" t="n">
-        <v>100229.835889598</v>
+        <v>14925.0356490264</v>
       </c>
       <c r="I16" t="n">
-        <v>3574.8619825</v>
+        <v>553.8203714833</v>
       </c>
       <c r="J16" t="n">
-        <v>89.0403794961183</v>
+        <v>75.1518529256129</v>
       </c>
       <c r="K16" t="n">
-        <v>32.1764598235932</v>
+        <v>26.9664513892842</v>
       </c>
       <c r="L16" t="s">
         <v>12</v>
@@ -1008,34 +1008,34 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>156324.88534</v>
+        <v>23297.692842667</v>
       </c>
       <c r="C17" t="n">
-        <v>9471.761148</v>
+        <v>2189.08371792</v>
       </c>
       <c r="D17" t="n">
-        <v>117.020260432414</v>
+        <v>93.275593705566</v>
       </c>
       <c r="E17" t="n">
-        <v>86.0533486654822</v>
+        <v>107.632350620382</v>
       </c>
       <c r="F17" t="n">
-        <v>413258.495268811</v>
+        <v>62385.293211311</v>
       </c>
       <c r="G17" t="n">
-        <v>817875.385830907</v>
+        <v>189024.793006739</v>
       </c>
       <c r="H17" t="n">
-        <v>50065.887172835</v>
+        <v>3253.3613152666</v>
       </c>
       <c r="I17" t="n">
-        <v>8127.4525328601</v>
+        <v>1895.1876262228</v>
       </c>
       <c r="J17" t="n">
-        <v>39.5226900278527</v>
+        <v>13.3046884508655</v>
       </c>
       <c r="K17" t="n">
-        <v>74.0194207932843</v>
+        <v>93.4851007054751</v>
       </c>
       <c r="L17" t="s">
         <v>12</v>
@@ -1046,34 +1046,34 @@
         <v>1</v>
       </c>
       <c r="B18" t="n">
-        <v>47614.03212243</v>
+        <v>149753.982479712</v>
       </c>
       <c r="C18" t="n">
-        <v>6619.330973</v>
+        <v>8696.770195</v>
       </c>
       <c r="D18" t="n">
-        <v>67.8711178828148</v>
+        <v>109.294308175781</v>
       </c>
       <c r="E18" t="n">
-        <v>59.1067270304137</v>
+        <v>78.2650760720572</v>
       </c>
       <c r="F18" t="n">
-        <v>402783.858052294</v>
+        <v>387593.56732525</v>
       </c>
       <c r="G18" t="n">
-        <v>579723.864583444</v>
+        <v>761666.888603171</v>
       </c>
       <c r="H18" t="n">
-        <v>67286.8278348038</v>
+        <v>42586.8161831916</v>
       </c>
       <c r="I18" t="n">
-        <v>5275.022421</v>
+        <v>7352.46149568424</v>
       </c>
       <c r="J18" t="n">
-        <v>51.0179576622851</v>
+        <v>31.8627964983222</v>
       </c>
       <c r="K18" t="n">
-        <v>47.0921446191635</v>
+        <v>66.2504924891521</v>
       </c>
       <c r="L18" t="s">
         <v>13</v>
@@ -1084,34 +1084,34 @@
         <v>2</v>
       </c>
       <c r="B19" t="n">
-        <v>29109.84954024</v>
+        <v>143041.6992896</v>
       </c>
       <c r="C19" t="n">
-        <v>6186.758084</v>
+        <v>7341.997463</v>
       </c>
       <c r="D19" t="n">
-        <v>56.2532783752974</v>
+        <v>108.997595565136</v>
       </c>
       <c r="E19" t="n">
-        <v>55.31458802475</v>
+        <v>66.2800542546027</v>
       </c>
       <c r="F19" t="n">
-        <v>361077.021550051</v>
+        <v>373325.813865395</v>
       </c>
       <c r="G19" t="n">
-        <v>541838.944196776</v>
+        <v>643015.307796756</v>
       </c>
       <c r="H19" t="n">
-        <v>50560.2932897283</v>
+        <v>35232.7420231726</v>
       </c>
       <c r="I19" t="n">
-        <v>4842.449626</v>
+        <v>5997.6890156942</v>
       </c>
       <c r="J19" t="n">
-        <v>44.4427335927938</v>
+        <v>32.916111155739</v>
       </c>
       <c r="K19" t="n">
-        <v>43.3000065195435</v>
+        <v>54.2654728395149</v>
       </c>
       <c r="L19" t="s">
         <v>13</v>
@@ -1122,34 +1122,34 @@
         <v>3</v>
       </c>
       <c r="B20" t="n">
-        <v>15993.09321725</v>
+        <v>136229.96591973</v>
       </c>
       <c r="C20" t="n">
-        <v>6176.655733</v>
+        <v>6625.982674</v>
       </c>
       <c r="D20" t="n">
-        <v>44.0052167625924</v>
+        <v>100.565010403691</v>
       </c>
       <c r="E20" t="n">
-        <v>55.1829882749937</v>
+        <v>59.4585968502382</v>
       </c>
       <c r="F20" t="n">
-        <v>308343.833407084</v>
+        <v>353206.967151864</v>
       </c>
       <c r="G20" t="n">
-        <v>540954.175934396</v>
+        <v>580306.423428968</v>
       </c>
       <c r="H20" t="n">
-        <v>34692.2513553354</v>
+        <v>28498.1004077125</v>
       </c>
       <c r="I20" t="n">
-        <v>4832.347197</v>
+        <v>5281.6741805551</v>
       </c>
       <c r="J20" t="n">
-        <v>28.4750778340043</v>
+        <v>23.5884503389445</v>
       </c>
       <c r="K20" t="n">
-        <v>43.1684061377285</v>
+        <v>47.4440151078061</v>
       </c>
       <c r="L20" t="s">
         <v>13</v>
@@ -1160,34 +1160,34 @@
         <v>4</v>
       </c>
       <c r="B21" t="n">
-        <v>14543.88697862</v>
+        <v>143535.24887464</v>
       </c>
       <c r="C21" t="n">
-        <v>5916.584654</v>
+        <v>6375.030487</v>
       </c>
       <c r="D21" t="n">
-        <v>47.5047222742376</v>
+        <v>111.307895238578</v>
       </c>
       <c r="E21" t="n">
-        <v>52.9186196440184</v>
+        <v>57.279707155273</v>
       </c>
       <c r="F21" t="n">
-        <v>325149.830646422</v>
+        <v>373253.095152146</v>
       </c>
       <c r="G21" t="n">
-        <v>518177.038547061</v>
+        <v>558327.922540173</v>
       </c>
       <c r="H21" t="n">
-        <v>42064.6325372254</v>
+        <v>35134.3757147033</v>
       </c>
       <c r="I21" t="n">
-        <v>4572.276035</v>
+        <v>5030.7218267762</v>
       </c>
       <c r="J21" t="n">
-        <v>41.746400837232</v>
+        <v>35.2501284085163</v>
       </c>
       <c r="K21" t="n">
-        <v>40.90403674999</v>
+        <v>45.265123941294</v>
       </c>
       <c r="L21" t="s">
         <v>13</v>
@@ -1198,34 +1198,34 @@
         <v>5</v>
       </c>
       <c r="B22" t="n">
-        <v>16802.31111799</v>
+        <v>136820.48302102</v>
       </c>
       <c r="C22" t="n">
-        <v>6177.467889</v>
+        <v>6554.546615</v>
       </c>
       <c r="D22" t="n">
-        <v>42.8477505694039</v>
+        <v>99.7372002783615</v>
       </c>
       <c r="E22" t="n">
-        <v>55.1824275327287</v>
+        <v>58.7383453960818</v>
       </c>
       <c r="F22" t="n">
-        <v>299896.643751945</v>
+        <v>355026.99625769</v>
       </c>
       <c r="G22" t="n">
-        <v>541025.304907534</v>
+        <v>574050.022538453</v>
       </c>
       <c r="H22" t="n">
-        <v>35390.0035800967</v>
+        <v>28949.4752215308</v>
       </c>
       <c r="I22" t="n">
-        <v>4833.159286</v>
+        <v>5210.237931358</v>
       </c>
       <c r="J22" t="n">
-        <v>27.3372585873033</v>
+        <v>22.1835100841028</v>
       </c>
       <c r="K22" t="n">
-        <v>43.1678448063354</v>
+        <v>46.7237619116295</v>
       </c>
       <c r="L22" t="s">
         <v>13</v>
@@ -1236,34 +1236,34 @@
         <v>6</v>
       </c>
       <c r="B23" t="n">
-        <v>4283.03243748</v>
+        <v>139719.99736543</v>
       </c>
       <c r="C23" t="n">
-        <v>5760.430606</v>
+        <v>5810.479147</v>
       </c>
       <c r="D23" t="n">
-        <v>39.0570892407645</v>
+        <v>107.586362881489</v>
       </c>
       <c r="E23" t="n">
-        <v>51.5664691108899</v>
+        <v>52.0435003408487</v>
       </c>
       <c r="F23" t="n">
-        <v>274669.293505089</v>
+        <v>360841.743775931</v>
       </c>
       <c r="G23" t="n">
-        <v>497406.377844445</v>
+        <v>501728.010235828</v>
       </c>
       <c r="H23" t="n">
-        <v>32684.9360938539</v>
+        <v>30949.3851436631</v>
       </c>
       <c r="I23" t="n">
-        <v>4416.12169</v>
+        <v>4466.1702918795</v>
       </c>
       <c r="J23" t="n">
-        <v>32.474559590281</v>
+        <v>30.6945074197909</v>
       </c>
       <c r="K23" t="n">
-        <v>39.5325387384548</v>
+        <v>40.0095705356774</v>
       </c>
       <c r="L23" t="s">
         <v>13</v>
@@ -1274,34 +1274,34 @@
         <v>7</v>
       </c>
       <c r="B24" t="n">
-        <v>2559.67625249</v>
+        <v>137992.0018959</v>
       </c>
       <c r="C24" t="n">
-        <v>5747.447556</v>
+        <v>5760.495689</v>
       </c>
       <c r="D24" t="n">
-        <v>36.2180111601606</v>
+        <v>103.36197207864</v>
       </c>
       <c r="E24" t="n">
-        <v>51.5693343359411</v>
+        <v>51.6950752895751</v>
       </c>
       <c r="F24" t="n">
-        <v>263523.02091084</v>
+        <v>357931.598064233</v>
       </c>
       <c r="G24" t="n">
-        <v>496285.306814243</v>
+        <v>497411.99768461</v>
       </c>
       <c r="H24" t="n">
-        <v>30041.2095182028</v>
+        <v>29093.0850377257</v>
       </c>
       <c r="I24" t="n">
-        <v>4403.138861</v>
+        <v>4416.187017021</v>
       </c>
       <c r="J24" t="n">
-        <v>27.040629985282</v>
+        <v>25.9811005159642</v>
       </c>
       <c r="K24" t="n">
-        <v>39.5064874174496</v>
+        <v>39.6322285929515</v>
       </c>
       <c r="L24" t="s">
         <v>13</v>
@@ -1312,34 +1312,34 @@
         <v>8</v>
       </c>
       <c r="B25" t="n">
-        <v>4848.4429277</v>
+        <v>149113.68023369</v>
       </c>
       <c r="C25" t="n">
-        <v>5624.593541</v>
+        <v>5649.62038</v>
       </c>
       <c r="D25" t="n">
-        <v>35.0115725522357</v>
+        <v>114.130295366572</v>
       </c>
       <c r="E25" t="n">
-        <v>50.3746175429341</v>
+        <v>50.614321783342</v>
       </c>
       <c r="F25" t="n">
-        <v>291702.135486393</v>
+        <v>383473.062026314</v>
       </c>
       <c r="G25" t="n">
-        <v>485677.007750429</v>
+        <v>487838.045733061</v>
       </c>
       <c r="H25" t="n">
-        <v>41987.6102970714</v>
+        <v>39993.7012375079</v>
       </c>
       <c r="I25" t="n">
-        <v>4280.284804</v>
+        <v>4305.311699464</v>
       </c>
       <c r="J25" t="n">
-        <v>40.9002613331147</v>
+        <v>38.9201490411927</v>
       </c>
       <c r="K25" t="n">
-        <v>38.3406887624799</v>
+        <v>38.5803935371693</v>
       </c>
       <c r="L25" t="s">
         <v>13</v>
@@ -1350,34 +1350,34 @@
         <v>9</v>
       </c>
       <c r="B26" t="n">
-        <v>7304.06060409</v>
+        <v>149508.53552941</v>
       </c>
       <c r="C26" t="n">
-        <v>5663.812742</v>
+        <v>5770.703551</v>
       </c>
       <c r="D26" t="n">
-        <v>41.2565072791277</v>
+        <v>115.628263460512</v>
       </c>
       <c r="E26" t="n">
-        <v>50.7373254036727</v>
+        <v>51.7548839427498</v>
       </c>
       <c r="F26" t="n">
-        <v>300927.737288121</v>
+        <v>386228.761938985</v>
       </c>
       <c r="G26" t="n">
-        <v>489063.539425863</v>
+        <v>498293.434509431</v>
       </c>
       <c r="H26" t="n">
-        <v>43712.7240025002</v>
+        <v>40566.4232453719</v>
       </c>
       <c r="I26" t="n">
-        <v>4319.504178</v>
+        <v>4426.394947388</v>
       </c>
       <c r="J26" t="n">
-        <v>43.3261238396236</v>
+        <v>40.4635656667657</v>
       </c>
       <c r="K26" t="n">
-        <v>38.7033981521308</v>
+        <v>39.7209563184306</v>
       </c>
       <c r="L26" t="s">
         <v>13</v>
@@ -1388,34 +1388,34 @@
         <v>10</v>
       </c>
       <c r="B27" t="n">
-        <v>12117.939859348</v>
+        <v>157035.044007763</v>
       </c>
       <c r="C27" t="n">
-        <v>5647.063745</v>
+        <v>5928.14455</v>
       </c>
       <c r="D27" t="n">
-        <v>49.4382821661371</v>
+        <v>122.696684221462</v>
       </c>
       <c r="E27" t="n">
-        <v>50.6348891998656</v>
+        <v>53.3281616110487</v>
       </c>
       <c r="F27" t="n">
-        <v>327648.894587659</v>
+        <v>405896.3527276</v>
       </c>
       <c r="G27" t="n">
-        <v>487617.283321047</v>
+        <v>511888.278782919</v>
       </c>
       <c r="H27" t="n">
-        <v>54135.973846145</v>
+        <v>48118.6978464883</v>
       </c>
       <c r="I27" t="n">
-        <v>4302.755109</v>
+        <v>4583.835910441</v>
       </c>
       <c r="J27" t="n">
-        <v>52.4689615473748</v>
+        <v>47.3143877531963</v>
       </c>
       <c r="K27" t="n">
-        <v>38.6009612904814</v>
+        <v>41.2942336632156</v>
       </c>
       <c r="L27" t="s">
         <v>13</v>
@@ -1426,34 +1426,34 @@
         <v>11</v>
       </c>
       <c r="B28" t="n">
-        <v>27761.9256227</v>
+        <v>170484.51045498</v>
       </c>
       <c r="C28" t="n">
-        <v>5744.446926</v>
+        <v>6840.718989</v>
       </c>
       <c r="D28" t="n">
-        <v>71.2877197576623</v>
+        <v>137.275071783378</v>
       </c>
       <c r="E28" t="n">
-        <v>51.4989934475539</v>
+        <v>61.9669056801819</v>
       </c>
       <c r="F28" t="n">
-        <v>417616.906715477</v>
+        <v>442736.873909379</v>
       </c>
       <c r="G28" t="n">
-        <v>503101.142006486</v>
+        <v>599113.122611406</v>
       </c>
       <c r="H28" t="n">
-        <v>77791.0292286628</v>
+        <v>61895.6682311594</v>
       </c>
       <c r="I28" t="n">
-        <v>4400.138424</v>
+        <v>5496.4104890889</v>
       </c>
       <c r="J28" t="n">
-        <v>73.4157137815196</v>
+        <v>60.9481537796566</v>
       </c>
       <c r="K28" t="n">
-        <v>39.4844116325389</v>
+        <v>49.95232388295</v>
       </c>
       <c r="L28" t="s">
         <v>13</v>
@@ -1464,34 +1464,34 @@
         <v>12</v>
       </c>
       <c r="B29" t="n">
-        <v>24472.06069176</v>
+        <v>152637.976425711</v>
       </c>
       <c r="C29" t="n">
-        <v>5917.944872</v>
+        <v>6914.970738</v>
       </c>
       <c r="D29" t="n">
-        <v>64.1822120764622</v>
+        <v>122.523691735952</v>
       </c>
       <c r="E29" t="n">
-        <v>52.9795177173176</v>
+        <v>62.4991409877888</v>
       </c>
       <c r="F29" t="n">
-        <v>379618.155007707</v>
+        <v>399849.078186213</v>
       </c>
       <c r="G29" t="n">
-        <v>518296.16702679</v>
+        <v>605616.122847826</v>
       </c>
       <c r="H29" t="n">
-        <v>57907.2156753563</v>
+        <v>44251.9394230849</v>
       </c>
       <c r="I29" t="n">
-        <v>4573.636293</v>
+        <v>5570.662225892</v>
       </c>
       <c r="J29" t="n">
-        <v>57.7671898730524</v>
+        <v>46.290917311368</v>
       </c>
       <c r="K29" t="n">
-        <v>40.9649352029195</v>
+        <v>50.4845590993907</v>
       </c>
       <c r="L29" t="s">
         <v>13</v>
@@ -1502,34 +1502,34 @@
         <v>13</v>
       </c>
       <c r="B30" t="n">
-        <v>21889.722123</v>
+        <v>173851.647550698</v>
       </c>
       <c r="C30" t="n">
-        <v>5619.207819</v>
+        <v>6393.784235</v>
       </c>
       <c r="D30" t="n">
-        <v>67.540968812839</v>
+        <v>139.759897715118</v>
       </c>
       <c r="E30" t="n">
-        <v>50.3839876701363</v>
+        <v>57.7931467903642</v>
       </c>
       <c r="F30" t="n">
-        <v>409962.245605398</v>
+        <v>451482.82266961</v>
       </c>
       <c r="G30" t="n">
-        <v>492132.64694208</v>
+        <v>559970.383887148</v>
       </c>
       <c r="H30" t="n">
-        <v>77323.7347515964</v>
+        <v>65045.247717797</v>
       </c>
       <c r="I30" t="n">
-        <v>4274.89929</v>
+        <v>5049.4757180326</v>
       </c>
       <c r="J30" t="n">
-        <v>73.4206159768654</v>
+        <v>63.4976705978154</v>
       </c>
       <c r="K30" t="n">
-        <v>38.3694056113146</v>
+        <v>45.7785648282996</v>
       </c>
       <c r="L30" t="s">
         <v>13</v>
@@ -1540,34 +1540,34 @@
         <v>14</v>
       </c>
       <c r="B31" t="n">
-        <v>29112.072347</v>
+        <v>167366.62840467</v>
       </c>
       <c r="C31" t="n">
-        <v>5773.985992</v>
+        <v>6754.363389</v>
       </c>
       <c r="D31" t="n">
-        <v>61.2836289002466</v>
+        <v>128.18728039526</v>
       </c>
       <c r="E31" t="n">
-        <v>51.860282639682</v>
+        <v>61.2338668307596</v>
       </c>
       <c r="F31" t="n">
-        <v>399174.897346415</v>
+        <v>439591.284920256</v>
       </c>
       <c r="G31" t="n">
-        <v>498576.869412127</v>
+        <v>583231.299491435</v>
       </c>
       <c r="H31" t="n">
-        <v>75088.843026052</v>
+        <v>58819.8813587715</v>
       </c>
       <c r="I31" t="n">
-        <v>4429.677375</v>
+        <v>5410.0548007928</v>
       </c>
       <c r="J31" t="n">
-        <v>67.7271809432991</v>
+        <v>53.792049413419</v>
       </c>
       <c r="K31" t="n">
-        <v>39.8263549331731</v>
+        <v>49.1999394187638</v>
       </c>
       <c r="L31" t="s">
         <v>13</v>
@@ -1578,34 +1578,34 @@
         <v>15</v>
       </c>
       <c r="B32" t="n">
-        <v>7432.8780636</v>
+        <v>209942.47879774</v>
       </c>
       <c r="C32" t="n">
-        <v>4916.777897</v>
+        <v>4919.170673</v>
       </c>
       <c r="D32" t="n">
-        <v>61.709583780245</v>
+        <v>164.413306323774</v>
       </c>
       <c r="E32" t="n">
-        <v>44.1874367512114</v>
+        <v>44.2103882820078</v>
       </c>
       <c r="F32" t="n">
-        <v>383016.825047318</v>
+        <v>516032.561230557</v>
       </c>
       <c r="G32" t="n">
-        <v>424557.963056624</v>
+        <v>424764.57643756</v>
       </c>
       <c r="H32" t="n">
-        <v>104436.356307479</v>
+        <v>100229.835889598</v>
       </c>
       <c r="I32" t="n">
-        <v>3572.469213</v>
+        <v>3574.8619825</v>
       </c>
       <c r="J32" t="n">
-        <v>92.8568541236453</v>
+        <v>89.0403794961183</v>
       </c>
       <c r="K32" t="n">
-        <v>32.1535083549023</v>
+        <v>32.1764598235932</v>
       </c>
       <c r="L32" t="s">
         <v>13</v>
@@ -1616,34 +1616,34 @@
         <v>16</v>
       </c>
       <c r="B33" t="n">
-        <v>61420.96193581</v>
+        <v>158004.16494594</v>
       </c>
       <c r="C33" t="n">
-        <v>6529.732686</v>
+        <v>9471.761148</v>
       </c>
       <c r="D33" t="n">
-        <v>85.7922851761453</v>
+        <v>117.849214719056</v>
       </c>
       <c r="E33" t="n">
-        <v>58.5492934473676</v>
+        <v>86.0533486654822</v>
       </c>
       <c r="F33" t="n">
-        <v>457108.845451775</v>
+        <v>414267.954531748</v>
       </c>
       <c r="G33" t="n">
-        <v>563834.703650926</v>
+        <v>817875.385830907</v>
       </c>
       <c r="H33" t="n">
-        <v>89082.5830168385</v>
+        <v>50065.887172835</v>
       </c>
       <c r="I33" t="n">
-        <v>5185.424042</v>
+        <v>8127.4525328601</v>
       </c>
       <c r="J33" t="n">
-        <v>74.3867678145332</v>
+        <v>39.5226900278527</v>
       </c>
       <c r="K33" t="n">
-        <v>46.5153654105036</v>
+        <v>74.0194207932843</v>
       </c>
       <c r="L33" t="s">
         <v>13</v>
@@ -1654,34 +1654,34 @@
         <v>1</v>
       </c>
       <c r="B34" t="n">
-        <v>-64.3772804</v>
+        <v>30735.172454769</v>
       </c>
       <c r="C34" t="n">
-        <v>2109.97350786</v>
+        <v>1328.78917726</v>
       </c>
       <c r="D34" t="n">
-        <v>30.5294900879817</v>
+        <v>122.778491963397</v>
       </c>
       <c r="E34" t="n">
-        <v>102.510602155379</v>
+        <v>63.9254211578953</v>
       </c>
       <c r="F34" t="n">
-        <v>47319.4361747029</v>
+        <v>86083.9336122595</v>
       </c>
       <c r="G34" t="n">
-        <v>184792.390822377</v>
+        <v>116375.929863603</v>
       </c>
       <c r="H34" t="n">
-        <v>2529.16017914569</v>
+        <v>10825.3347131744</v>
       </c>
       <c r="I34" t="n">
-        <v>1816.07737098014</v>
+        <v>1034.89303802</v>
       </c>
       <c r="J34" t="n">
-        <v>9.51917065356799</v>
+        <v>43.9068809473274</v>
       </c>
       <c r="K34" t="n">
-        <v>88.3860451304422</v>
+        <v>49.8008639104389</v>
       </c>
       <c r="L34" t="s">
         <v>14</v>
@@ -1692,34 +1692,34 @@
         <v>2</v>
       </c>
       <c r="B35" t="n">
-        <v>-178.187916255</v>
+        <v>27330.246599304</v>
       </c>
       <c r="C35" t="n">
-        <v>1580.90003854</v>
+        <v>1181.25209414</v>
       </c>
       <c r="D35" t="n">
-        <v>31.8995860076216</v>
+        <v>111.747470904478</v>
       </c>
       <c r="E35" t="n">
-        <v>77.3321558462802</v>
+        <v>56.9669867387733</v>
       </c>
       <c r="F35" t="n">
-        <v>47598.6027708911</v>
+        <v>77463.5536861589</v>
       </c>
       <c r="G35" t="n">
-        <v>138455.90794611</v>
+        <v>103454.568423214</v>
       </c>
       <c r="H35" t="n">
-        <v>2521.11881163574</v>
+        <v>7293.473423777</v>
       </c>
       <c r="I35" t="n">
-        <v>1287.0038841677</v>
+        <v>887.35592234</v>
       </c>
       <c r="J35" t="n">
-        <v>15.6279803108575</v>
+        <v>34.6422812339047</v>
       </c>
       <c r="K35" t="n">
-        <v>63.2075979046658</v>
+        <v>42.8424278851332</v>
       </c>
       <c r="L35" t="s">
         <v>14</v>
@@ -1730,34 +1730,34 @@
         <v>3</v>
       </c>
       <c r="B36" t="n">
-        <v>-117.898311259</v>
+        <v>24385.710717976</v>
       </c>
       <c r="C36" t="n">
-        <v>1374.46742384</v>
+        <v>1180.28488744</v>
       </c>
       <c r="D36" t="n">
-        <v>30.3592116359533</v>
+        <v>97.808730748672</v>
       </c>
       <c r="E36" t="n">
-        <v>66.72803064856</v>
+        <v>56.8230823603711</v>
       </c>
       <c r="F36" t="n">
-        <v>46241.0010692274</v>
+        <v>67641.3929961064</v>
       </c>
       <c r="G36" t="n">
-        <v>120376.450421159</v>
+        <v>103369.860042826</v>
       </c>
       <c r="H36" t="n">
-        <v>2171.42629957606</v>
+        <v>4384.8393753676</v>
       </c>
       <c r="I36" t="n">
-        <v>1080.5712609843</v>
+        <v>886.38872916</v>
       </c>
       <c r="J36" t="n">
-        <v>10.5013610078282</v>
+        <v>19.6621832883062</v>
       </c>
       <c r="K36" t="n">
-        <v>52.6034721607589</v>
+        <v>42.6985241518383</v>
       </c>
       <c r="L36" t="s">
         <v>14</v>
@@ -1768,34 +1768,34 @@
         <v>4</v>
       </c>
       <c r="B37" t="n">
-        <v>-401.2668456</v>
+        <v>25294.326779408</v>
       </c>
       <c r="C37" t="n">
-        <v>1281.7087638</v>
+        <v>1107.1874831</v>
       </c>
       <c r="D37" t="n">
-        <v>30.8809313759158</v>
+        <v>107.347662692801</v>
       </c>
       <c r="E37" t="n">
-        <v>62.3227211764989</v>
+        <v>53.4144432284655</v>
       </c>
       <c r="F37" t="n">
-        <v>48668.0054192861</v>
+        <v>70405.4090751455</v>
       </c>
       <c r="G37" t="n">
-        <v>112252.606925296</v>
+        <v>96967.9578101296</v>
       </c>
       <c r="H37" t="n">
-        <v>2965.21171576757</v>
+        <v>5148.134068229</v>
       </c>
       <c r="I37" t="n">
-        <v>987.81262856462</v>
+        <v>813.29133789</v>
       </c>
       <c r="J37" t="n">
-        <v>19.1127050617248</v>
+        <v>30.1613083051692</v>
       </c>
       <c r="K37" t="n">
-        <v>48.198164044124</v>
+        <v>39.289885624116</v>
       </c>
       <c r="L37" t="s">
         <v>14</v>
@@ -1806,34 +1806,34 @@
         <v>5</v>
       </c>
       <c r="B38" t="n">
-        <v>-105.83629556</v>
+        <v>24464.15438881</v>
       </c>
       <c r="C38" t="n">
-        <v>1330.1573014</v>
+        <v>1161.1911062</v>
       </c>
       <c r="D38" t="n">
-        <v>28.7475952573618</v>
+        <v>97.1909158330939</v>
       </c>
       <c r="E38" t="n">
-        <v>64.3889010001654</v>
+        <v>55.8479862847407</v>
       </c>
       <c r="F38" t="n">
-        <v>44342.6377586931</v>
+        <v>67653.3689246836</v>
       </c>
       <c r="G38" t="n">
-        <v>116495.750766486</v>
+        <v>101697.618437879</v>
       </c>
       <c r="H38" t="n">
-        <v>2142.06295214739</v>
+        <v>4441.1625472791</v>
       </c>
       <c r="I38" t="n">
-        <v>1036.26116291667</v>
+        <v>867.2949263</v>
       </c>
       <c r="J38" t="n">
-        <v>8.60612409327883</v>
+        <v>18.2583930264168</v>
       </c>
       <c r="K38" t="n">
-        <v>50.2643437743682</v>
+        <v>41.7234270269359</v>
       </c>
       <c r="L38" t="s">
         <v>14</v>
@@ -1844,34 +1844,34 @@
         <v>6</v>
       </c>
       <c r="B39" t="n">
-        <v>-342.57753472</v>
+        <v>23394.621338671</v>
       </c>
       <c r="C39" t="n">
-        <v>1094.31645402</v>
+        <v>1058.35661922</v>
       </c>
       <c r="D39" t="n">
-        <v>31.0269353807736</v>
+        <v>97.6882410478758</v>
       </c>
       <c r="E39" t="n">
-        <v>52.8628290105597</v>
+        <v>51.0161440534564</v>
       </c>
       <c r="F39" t="n">
-        <v>45346.0215034122</v>
+        <v>63443.3536028196</v>
       </c>
       <c r="G39" t="n">
-        <v>94492.9330530789</v>
+        <v>91387.843798619</v>
       </c>
       <c r="H39" t="n">
-        <v>2625.31581731824</v>
+        <v>3191.4987101027</v>
       </c>
       <c r="I39" t="n">
-        <v>800.4202732668</v>
+        <v>764.46045407</v>
       </c>
       <c r="J39" t="n">
-        <v>16.8807864172737</v>
+        <v>19.6558107601317</v>
       </c>
       <c r="K39" t="n">
-        <v>38.7155745127215</v>
+        <v>36.8688903672142</v>
       </c>
       <c r="L39" t="s">
         <v>14</v>
@@ -1882,34 +1882,34 @@
         <v>7</v>
       </c>
       <c r="B40" t="n">
-        <v>-291.665022212</v>
+        <v>23234.731644616</v>
       </c>
       <c r="C40" t="n">
-        <v>1089.44321467</v>
+        <v>1075.48238307</v>
       </c>
       <c r="D40" t="n">
-        <v>30.6578461082834</v>
+        <v>94.5869859119648</v>
       </c>
       <c r="E40" t="n">
-        <v>52.6458675040139</v>
+        <v>51.9219771661029</v>
       </c>
       <c r="F40" t="n">
-        <v>44916.1413997743</v>
+        <v>62782.1994446294</v>
       </c>
       <c r="G40" t="n">
-        <v>94072.1345921222</v>
+        <v>92866.6332758458</v>
       </c>
       <c r="H40" t="n">
-        <v>2746.2528246686</v>
+        <v>3007.114908791</v>
       </c>
       <c r="I40" t="n">
-        <v>795.54703899072</v>
+        <v>781.58620879</v>
       </c>
       <c r="J40" t="n">
-        <v>14.5616778645056</v>
+        <v>15.9073743682145</v>
       </c>
       <c r="K40" t="n">
-        <v>38.4647188794018</v>
+        <v>37.7408286144227</v>
       </c>
       <c r="L40" t="s">
         <v>14</v>
@@ -1920,34 +1920,34 @@
         <v>8</v>
       </c>
       <c r="B41" t="n">
-        <v>-429.481126746</v>
+        <v>25400.320883739</v>
       </c>
       <c r="C41" t="n">
-        <v>1041.96822101</v>
+        <v>1026.47003241</v>
       </c>
       <c r="D41" t="n">
-        <v>28.1480529061108</v>
+        <v>106.338195006113</v>
       </c>
       <c r="E41" t="n">
-        <v>50.3130887356167</v>
+        <v>49.5157372603914</v>
       </c>
       <c r="F41" t="n">
-        <v>50171.0468595344</v>
+        <v>69369.3520135814</v>
       </c>
       <c r="G41" t="n">
-        <v>89972.7249733323</v>
+        <v>88634.4746962355</v>
       </c>
       <c r="H41" t="n">
-        <v>4581.23745280582</v>
+        <v>5088.2789614688</v>
       </c>
       <c r="I41" t="n">
-        <v>748.07204671984</v>
+        <v>732.57386334</v>
       </c>
       <c r="J41" t="n">
-        <v>27.6021779609433</v>
+        <v>30.26670334708</v>
       </c>
       <c r="K41" t="n">
-        <v>36.1658346612252</v>
+        <v>35.3684834509751</v>
       </c>
       <c r="L41" t="s">
         <v>14</v>
@@ -1958,34 +1958,34 @@
         <v>9</v>
       </c>
       <c r="B42" t="n">
-        <v>-470.539472578</v>
+        <v>25552.200325904</v>
       </c>
       <c r="C42" t="n">
-        <v>1075.12231205</v>
+        <v>1026.00030815</v>
       </c>
       <c r="D42" t="n">
-        <v>31.6400813324271</v>
+        <v>107.720522500849</v>
       </c>
       <c r="E42" t="n">
-        <v>52.0264230709302</v>
+        <v>49.5092849118198</v>
       </c>
       <c r="F42" t="n">
-        <v>49922.500890885</v>
+        <v>70415.5100839497</v>
       </c>
       <c r="G42" t="n">
-        <v>92835.5415686324</v>
+        <v>88593.914561285</v>
       </c>
       <c r="H42" t="n">
-        <v>4368.3335429612</v>
+        <v>5278.3648292043</v>
       </c>
       <c r="I42" t="n">
-        <v>781.2261764717</v>
+        <v>732.10416345</v>
       </c>
       <c r="J42" t="n">
-        <v>27.479545599953</v>
+        <v>31.779855167847</v>
       </c>
       <c r="K42" t="n">
-        <v>37.8791709070342</v>
+        <v>35.3620322682811</v>
       </c>
       <c r="L42" t="s">
         <v>14</v>
@@ -1996,34 +1996,34 @@
         <v>10</v>
       </c>
       <c r="B43" t="n">
-        <v>-562.65088883</v>
+        <v>27401.114402095</v>
       </c>
       <c r="C43" t="n">
-        <v>1120.20199518</v>
+        <v>1019.49318628</v>
       </c>
       <c r="D43" t="n">
-        <v>37.1900564554788</v>
+        <v>118.288615945215</v>
       </c>
       <c r="E43" t="n">
-        <v>54.456515719586</v>
+        <v>49.2692583060921</v>
       </c>
       <c r="F43" t="n">
-        <v>51835.8979977267</v>
+        <v>76646.2760011499</v>
       </c>
       <c r="G43" t="n">
-        <v>96728.1189528149</v>
+        <v>88032.0322748848</v>
       </c>
       <c r="H43" t="n">
-        <v>5426.9141796189</v>
+        <v>7122.1085625549</v>
       </c>
       <c r="I43" t="n">
-        <v>826.3058358483</v>
+        <v>725.59702795</v>
       </c>
       <c r="J43" t="n">
-        <v>34.0138954295134</v>
+        <v>41.6979987959261</v>
       </c>
       <c r="K43" t="n">
-        <v>40.309262321822</v>
+        <v>35.1220049507782</v>
       </c>
       <c r="L43" t="s">
         <v>14</v>
@@ -2034,34 +2034,34 @@
         <v>11</v>
       </c>
       <c r="B44" t="n">
-        <v>-608.93018243</v>
+        <v>31774.69057071</v>
       </c>
       <c r="C44" t="n">
-        <v>1421.09476549</v>
+        <v>1069.76081079</v>
       </c>
       <c r="D44" t="n">
-        <v>48.2485204091286</v>
+        <v>141.387224394219</v>
       </c>
       <c r="E44" t="n">
-        <v>69.837867050281</v>
+        <v>51.8209032565899</v>
       </c>
       <c r="F44" t="n">
-        <v>57748.7240115068</v>
+        <v>90866.036016694</v>
       </c>
       <c r="G44" t="n">
-        <v>124460.093134727</v>
+        <v>93690.1136898472</v>
       </c>
       <c r="H44" t="n">
-        <v>6988.90714459473</v>
+        <v>11555.9107257463</v>
       </c>
       <c r="I44" t="n">
-        <v>1127.19865573481</v>
+        <v>775.86468003</v>
       </c>
       <c r="J44" t="n">
-        <v>44.6179577092243</v>
+        <v>63.7279721857703</v>
       </c>
       <c r="K44" t="n">
-        <v>55.7133112090727</v>
+        <v>37.6963463568015</v>
       </c>
       <c r="L44" t="s">
         <v>14</v>
@@ -2072,34 +2072,34 @@
         <v>12</v>
       </c>
       <c r="B45" t="n">
-        <v>-486.637527578</v>
+        <v>28079.633851031</v>
       </c>
       <c r="C45" t="n">
-        <v>1433.67323173</v>
+        <v>1107.70706023</v>
       </c>
       <c r="D45" t="n">
-        <v>40.9744422185957</v>
+        <v>123.478478549197</v>
       </c>
       <c r="E45" t="n">
-        <v>70.2604368080786</v>
+        <v>53.5479610122171</v>
       </c>
       <c r="F45" t="n">
-        <v>51918.3384889426</v>
+        <v>80574.649564886</v>
       </c>
       <c r="G45" t="n">
-        <v>125561.720638916</v>
+        <v>97013.4625995081</v>
       </c>
       <c r="H45" t="n">
-        <v>3942.46287148064</v>
+        <v>7919.531663948</v>
       </c>
       <c r="I45" t="n">
-        <v>1139.77708303009</v>
+        <v>813.81091119</v>
       </c>
       <c r="J45" t="n">
-        <v>28.5464985966722</v>
+        <v>45.9175732204687</v>
       </c>
       <c r="K45" t="n">
-        <v>56.1358790510155</v>
+        <v>39.4234032395588</v>
       </c>
       <c r="L45" t="s">
         <v>14</v>
@@ -2110,34 +2110,34 @@
         <v>13</v>
       </c>
       <c r="B46" t="n">
-        <v>-641.77995094</v>
+        <v>31437.9920177735</v>
       </c>
       <c r="C46" t="n">
-        <v>1293.96971283</v>
+        <v>1034.58997803</v>
       </c>
       <c r="D46" t="n">
-        <v>46.261838524629</v>
+        <v>138.271901604602</v>
       </c>
       <c r="E46" t="n">
-        <v>63.4464474354856</v>
+        <v>50.1147803875143</v>
       </c>
       <c r="F46" t="n">
-        <v>60023.9418728636</v>
+        <v>89535.5868956426</v>
       </c>
       <c r="G46" t="n">
-        <v>113326.426135141</v>
+        <v>90609.836971337</v>
       </c>
       <c r="H46" t="n">
-        <v>7645.8934712822</v>
+        <v>11179.6821328472</v>
       </c>
       <c r="I46" t="n">
-        <v>1000.07356264392</v>
+        <v>740.69383555</v>
       </c>
       <c r="J46" t="n">
-        <v>45.5448177633257</v>
+        <v>60.7424368239093</v>
       </c>
       <c r="K46" t="n">
-        <v>49.3218895840806</v>
+        <v>35.9902229052603</v>
       </c>
       <c r="L46" t="s">
         <v>14</v>
@@ -2148,34 +2148,34 @@
         <v>14</v>
       </c>
       <c r="B47" t="n">
-        <v>-589.59891455</v>
+        <v>31349.14673276</v>
       </c>
       <c r="C47" t="n">
-        <v>1359.74079552</v>
+        <v>1030.46181732</v>
       </c>
       <c r="D47" t="n">
-        <v>34.3471299245332</v>
+        <v>132.398443399189</v>
       </c>
       <c r="E47" t="n">
-        <v>66.834128246961</v>
+        <v>49.920815174173</v>
       </c>
       <c r="F47" t="n">
-        <v>53225.5002740015</v>
+        <v>91465.5303112534</v>
       </c>
       <c r="G47" t="n">
-        <v>117412.011387214</v>
+        <v>88979.1606075889</v>
       </c>
       <c r="H47" t="n">
-        <v>6296.27529205534</v>
+        <v>11140.7236489092</v>
       </c>
       <c r="I47" t="n">
-        <v>1065.84462763463</v>
+        <v>736.56565708</v>
       </c>
       <c r="J47" t="n">
-        <v>35.2806189234038</v>
+        <v>57.0779875603305</v>
       </c>
       <c r="K47" t="n">
-        <v>52.6868745376419</v>
+        <v>35.7735617841142</v>
       </c>
       <c r="L47" t="s">
         <v>14</v>
@@ -2186,34 +2186,34 @@
         <v>15</v>
       </c>
       <c r="B48" t="n">
-        <v>-809.1596098</v>
+        <v>36348.027145147</v>
       </c>
       <c r="C48" t="n">
-        <v>847.71650831</v>
+        <v>843.41277021</v>
       </c>
       <c r="D48" t="n">
-        <v>51.4998674995846</v>
+        <v>156.534115111584</v>
       </c>
       <c r="E48" t="n">
-        <v>41.1137036774873</v>
+        <v>40.8915209502375</v>
       </c>
       <c r="F48" t="n">
-        <v>68356.7042621477</v>
+        <v>96683.86451116</v>
       </c>
       <c r="G48" t="n">
-        <v>73199.3190575408</v>
+        <v>72827.6963567513</v>
       </c>
       <c r="H48" t="n">
-        <v>14925.0356490264</v>
+        <v>15884.4790040952</v>
       </c>
       <c r="I48" t="n">
-        <v>553.8203714833</v>
+        <v>549.51663448</v>
       </c>
       <c r="J48" t="n">
-        <v>75.1518529256129</v>
+        <v>79.8586770822312</v>
       </c>
       <c r="K48" t="n">
-        <v>26.9664513892842</v>
+        <v>26.744268718725</v>
       </c>
       <c r="L48" t="s">
         <v>14</v>
@@ -2224,34 +2224,34 @@
         <v>16</v>
       </c>
       <c r="B49" t="n">
-        <v>-436.047479559</v>
+        <v>34983.889619326</v>
       </c>
       <c r="C49" t="n">
-        <v>2189.08371792</v>
+        <v>1247.39889322</v>
       </c>
       <c r="D49" t="n">
-        <v>30.2596353398219</v>
+        <v>148.536486762246</v>
       </c>
       <c r="E49" t="n">
-        <v>107.632350620382</v>
+        <v>60.3360520595744</v>
       </c>
       <c r="F49" t="n">
-        <v>48118.2502217115</v>
+        <v>99583.0427430117</v>
       </c>
       <c r="G49" t="n">
-        <v>189024.793006739</v>
+        <v>107711.420836745</v>
       </c>
       <c r="H49" t="n">
-        <v>3253.3613152666</v>
+        <v>14916.3700450375</v>
       </c>
       <c r="I49" t="n">
-        <v>1895.1876262228</v>
+        <v>953.50272313</v>
       </c>
       <c r="J49" t="n">
-        <v>13.3046884508655</v>
+        <v>68.4760140985721</v>
       </c>
       <c r="K49" t="n">
-        <v>93.4851007054751</v>
+        <v>46.1887981769321</v>
       </c>
       <c r="L49" t="s">
         <v>14</v>
@@ -2262,34 +2262,34 @@
         <v>1</v>
       </c>
       <c r="B50" t="n">
-        <v>8258.4571149</v>
+        <v>174539.349900922</v>
       </c>
       <c r="C50" t="n">
-        <v>1328.78917726</v>
+        <v>6619.330973</v>
       </c>
       <c r="D50" t="n">
-        <v>65.0195657311147</v>
+        <v>128.510969462808</v>
       </c>
       <c r="E50" t="n">
-        <v>63.9254211578953</v>
+        <v>59.1067270304137</v>
       </c>
       <c r="F50" t="n">
-        <v>74288.8805150984</v>
+        <v>469390.159800459</v>
       </c>
       <c r="G50" t="n">
-        <v>116375.929863603</v>
+        <v>579723.864583444</v>
       </c>
       <c r="H50" t="n">
-        <v>10825.3347131744</v>
+        <v>67286.8278348038</v>
       </c>
       <c r="I50" t="n">
-        <v>1034.89303802</v>
+        <v>5275.022421</v>
       </c>
       <c r="J50" t="n">
-        <v>43.9068809473274</v>
+        <v>51.0179576622851</v>
       </c>
       <c r="K50" t="n">
-        <v>49.8008639104389</v>
+        <v>47.0921446191635</v>
       </c>
       <c r="L50" t="s">
         <v>15</v>
@@ -2300,34 +2300,34 @@
         <v>2</v>
       </c>
       <c r="B51" t="n">
-        <v>4608.53912775</v>
+        <v>158415.57558209</v>
       </c>
       <c r="C51" t="n">
-        <v>1181.25209414</v>
+        <v>6186.758084</v>
       </c>
       <c r="D51" t="n">
-        <v>50.9701352671052</v>
+        <v>120.557879089585</v>
       </c>
       <c r="E51" t="n">
-        <v>56.9669867387733</v>
+        <v>55.31458802475</v>
       </c>
       <c r="F51" t="n">
-        <v>65261.5844954745</v>
+        <v>430516.548583787</v>
       </c>
       <c r="G51" t="n">
-        <v>103454.568423214</v>
+        <v>541838.944196776</v>
       </c>
       <c r="H51" t="n">
-        <v>7293.473423777</v>
+        <v>50560.2932897283</v>
       </c>
       <c r="I51" t="n">
-        <v>887.35592234</v>
+        <v>4842.449626</v>
       </c>
       <c r="J51" t="n">
-        <v>34.6422812339047</v>
+        <v>44.4427335927938</v>
       </c>
       <c r="K51" t="n">
-        <v>42.8424278851332</v>
+        <v>43.3000065195435</v>
       </c>
       <c r="L51" t="s">
         <v>15</v>
@@ -2338,34 +2338,34 @@
         <v>3</v>
       </c>
       <c r="B52" t="n">
-        <v>2105.121545265</v>
+        <v>142451.48789468</v>
       </c>
       <c r="C52" t="n">
-        <v>1180.28488744</v>
+        <v>6176.655733</v>
       </c>
       <c r="D52" t="n">
-        <v>39.5586356022753</v>
+        <v>105.472106669281</v>
       </c>
       <c r="E52" t="n">
-        <v>56.8230823603711</v>
+        <v>55.1829882749937</v>
       </c>
       <c r="F52" t="n">
-        <v>55238.0825473633</v>
+        <v>378741.555426775</v>
       </c>
       <c r="G52" t="n">
-        <v>103369.860042826</v>
+        <v>540954.175934396</v>
       </c>
       <c r="H52" t="n">
-        <v>4384.8393753676</v>
+        <v>34692.2513553354</v>
       </c>
       <c r="I52" t="n">
-        <v>886.38872916</v>
+        <v>4832.347197</v>
       </c>
       <c r="J52" t="n">
-        <v>19.6621832883062</v>
+        <v>28.4750778340043</v>
       </c>
       <c r="K52" t="n">
-        <v>42.6985241518383</v>
+        <v>43.1684061377285</v>
       </c>
       <c r="L52" t="s">
         <v>15</v>
@@ -2376,34 +2376,34 @@
         <v>4</v>
       </c>
       <c r="B53" t="n">
-        <v>1789.57090256</v>
+        <v>150489.67179329</v>
       </c>
       <c r="C53" t="n">
-        <v>1107.1874831</v>
+        <v>5916.584654</v>
       </c>
       <c r="D53" t="n">
-        <v>41.9567789875829</v>
+        <v>117.820173635166</v>
       </c>
       <c r="E53" t="n">
-        <v>53.4144432284655</v>
+        <v>52.9186196440184</v>
       </c>
       <c r="F53" t="n">
-        <v>57330.1049567581</v>
+        <v>400774.212619399</v>
       </c>
       <c r="G53" t="n">
-        <v>96967.9578101296</v>
+        <v>518177.038547061</v>
       </c>
       <c r="H53" t="n">
-        <v>5148.134068229</v>
+        <v>42064.6325372254</v>
       </c>
       <c r="I53" t="n">
-        <v>813.29133789</v>
+        <v>4572.276035</v>
       </c>
       <c r="J53" t="n">
-        <v>30.1613083051692</v>
+        <v>41.746400837232</v>
       </c>
       <c r="K53" t="n">
-        <v>39.289885624116</v>
+        <v>40.90403674999</v>
       </c>
       <c r="L53" t="s">
         <v>15</v>
@@ -2414,34 +2414,34 @@
         <v>5</v>
       </c>
       <c r="B54" t="n">
-        <v>2205.000093744</v>
+        <v>143294.10220174</v>
       </c>
       <c r="C54" t="n">
-        <v>1161.1911062</v>
+        <v>6177.467889</v>
       </c>
       <c r="D54" t="n">
-        <v>38.4447252645657</v>
+        <v>104.914213405078</v>
       </c>
       <c r="E54" t="n">
-        <v>55.8479862847407</v>
+        <v>55.1824275327287</v>
       </c>
       <c r="F54" t="n">
-        <v>53413.6232396594</v>
+        <v>380816.650967763</v>
       </c>
       <c r="G54" t="n">
-        <v>101697.618437879</v>
+        <v>541025.304907534</v>
       </c>
       <c r="H54" t="n">
-        <v>4441.1625472791</v>
+        <v>35390.0035800967</v>
       </c>
       <c r="I54" t="n">
-        <v>867.2949263</v>
+        <v>4833.159286</v>
       </c>
       <c r="J54" t="n">
-        <v>18.2583930264168</v>
+        <v>27.3372585873033</v>
       </c>
       <c r="K54" t="n">
-        <v>41.7234270269359</v>
+        <v>43.1678448063354</v>
       </c>
       <c r="L54" t="s">
         <v>15</v>
@@ -2452,34 +2452,34 @@
         <v>6</v>
       </c>
       <c r="B55" t="n">
-        <v>227.307412314</v>
+        <v>141464.11055318</v>
       </c>
       <c r="C55" t="n">
-        <v>1058.35661922</v>
+        <v>5760.430606</v>
       </c>
       <c r="D55" t="n">
-        <v>33.8165835321145</v>
+        <v>109.372463989217</v>
       </c>
       <c r="E55" t="n">
-        <v>51.0161440534564</v>
+        <v>51.5664691108899</v>
       </c>
       <c r="F55" t="n">
-        <v>47721.0270717892</v>
+        <v>367766.217721587</v>
       </c>
       <c r="G55" t="n">
-        <v>91387.843798619</v>
+        <v>497406.377844445</v>
       </c>
       <c r="H55" t="n">
-        <v>3191.4987101027</v>
+        <v>32684.9360938539</v>
       </c>
       <c r="I55" t="n">
-        <v>764.46045407</v>
+        <v>4416.12169</v>
       </c>
       <c r="J55" t="n">
-        <v>19.6558107601317</v>
+        <v>32.474559590281</v>
       </c>
       <c r="K55" t="n">
-        <v>36.8688903672142</v>
+        <v>39.5325387384548</v>
       </c>
       <c r="L55" t="s">
         <v>15</v>
@@ -2490,34 +2490,34 @@
         <v>7</v>
       </c>
       <c r="B56" t="n">
-        <v>-29.143622614</v>
+        <v>138942.52003369</v>
       </c>
       <c r="C56" t="n">
-        <v>1075.48238307</v>
+        <v>5747.447556</v>
       </c>
       <c r="D56" t="n">
-        <v>32.0100322190701</v>
+        <v>104.422927870384</v>
       </c>
       <c r="E56" t="n">
-        <v>51.9219771661029</v>
+        <v>51.5693343359411</v>
       </c>
       <c r="F56" t="n">
-        <v>46031.0177095372</v>
+        <v>361725.655180016</v>
       </c>
       <c r="G56" t="n">
-        <v>92866.6332758458</v>
+        <v>496285.306814243</v>
       </c>
       <c r="H56" t="n">
-        <v>3007.114908791</v>
+        <v>30041.2095182028</v>
       </c>
       <c r="I56" t="n">
-        <v>781.58620879</v>
+        <v>4403.138861</v>
       </c>
       <c r="J56" t="n">
-        <v>15.9073743682145</v>
+        <v>27.040629985282</v>
       </c>
       <c r="K56" t="n">
-        <v>37.7408286144227</v>
+        <v>39.5064874174496</v>
       </c>
       <c r="L56" t="s">
         <v>15</v>
@@ -2528,34 +2528,34 @@
         <v>8</v>
       </c>
       <c r="B57" t="n">
-        <v>79.726635245</v>
+        <v>151112.69943237</v>
       </c>
       <c r="C57" t="n">
-        <v>1026.47003241</v>
+        <v>5624.593541</v>
       </c>
       <c r="D57" t="n">
-        <v>30.8209653308786</v>
+        <v>116.114020802979</v>
       </c>
       <c r="E57" t="n">
-        <v>49.5157372603914</v>
+        <v>50.3746175429341</v>
       </c>
       <c r="F57" t="n">
-        <v>52182.261167194</v>
+        <v>390983.257279837</v>
       </c>
       <c r="G57" t="n">
-        <v>88634.4746962355</v>
+        <v>485677.007750429</v>
       </c>
       <c r="H57" t="n">
-        <v>5088.2789614688</v>
+        <v>41987.6102970714</v>
       </c>
       <c r="I57" t="n">
-        <v>732.57386334</v>
+        <v>4280.284804</v>
       </c>
       <c r="J57" t="n">
-        <v>30.26670334708</v>
+        <v>40.9002613331147</v>
       </c>
       <c r="K57" t="n">
-        <v>35.3684834509751</v>
+        <v>38.3406887624799</v>
       </c>
       <c r="L57" t="s">
         <v>15</v>
@@ -2566,34 +2566,34 @@
         <v>9</v>
       </c>
       <c r="B58" t="n">
-        <v>443.87846584</v>
+        <v>152666.5324993</v>
       </c>
       <c r="C58" t="n">
-        <v>1026.00030815</v>
+        <v>5663.812742</v>
       </c>
       <c r="D58" t="n">
-        <v>35.9577626154439</v>
+        <v>118.499188828883</v>
       </c>
       <c r="E58" t="n">
-        <v>49.5092849118198</v>
+        <v>50.7373254036727</v>
       </c>
       <c r="F58" t="n">
-        <v>53571.8963520385</v>
+        <v>398442.398152766</v>
       </c>
       <c r="G58" t="n">
-        <v>88593.914561285</v>
+        <v>489063.539425863</v>
       </c>
       <c r="H58" t="n">
-        <v>5278.3648292043</v>
+        <v>43712.7240025002</v>
       </c>
       <c r="I58" t="n">
-        <v>732.10416345</v>
+        <v>4319.504178</v>
       </c>
       <c r="J58" t="n">
-        <v>31.779855167847</v>
+        <v>43.3261238396236</v>
       </c>
       <c r="K58" t="n">
-        <v>35.3620322682811</v>
+        <v>38.7033981521308</v>
       </c>
       <c r="L58" t="s">
         <v>15</v>
@@ -2604,34 +2604,34 @@
         <v>10</v>
       </c>
       <c r="B59" t="n">
-        <v>1139.203523219</v>
+        <v>163074.344820418</v>
       </c>
       <c r="C59" t="n">
-        <v>1019.49318628</v>
+        <v>5647.063745</v>
       </c>
       <c r="D59" t="n">
-        <v>44.9001949912408</v>
+        <v>127.867230108075</v>
       </c>
       <c r="E59" t="n">
-        <v>49.2692583060921</v>
+        <v>50.6348891998656</v>
       </c>
       <c r="F59" t="n">
-        <v>58805.459900072</v>
+        <v>430199.897034407</v>
       </c>
       <c r="G59" t="n">
-        <v>88032.0322748848</v>
+        <v>487617.283321047</v>
       </c>
       <c r="H59" t="n">
-        <v>7122.1085625549</v>
+        <v>54135.973846145</v>
       </c>
       <c r="I59" t="n">
-        <v>725.59702795</v>
+        <v>4302.755109</v>
       </c>
       <c r="J59" t="n">
-        <v>41.6979987959261</v>
+        <v>52.4689615473748</v>
       </c>
       <c r="K59" t="n">
-        <v>35.1220049507782</v>
+        <v>38.6009612904814</v>
       </c>
       <c r="L59" t="s">
         <v>15</v>
@@ -2642,34 +2642,34 @@
         <v>11</v>
       </c>
       <c r="B60" t="n">
-        <v>3969.46783926</v>
+        <v>186418.26606348</v>
       </c>
       <c r="C60" t="n">
-        <v>1069.76081079</v>
+        <v>5744.446926</v>
       </c>
       <c r="D60" t="n">
-        <v>67.4050831953612</v>
+        <v>149.771795109047</v>
       </c>
       <c r="E60" t="n">
-        <v>51.8209032565899</v>
+        <v>51.4989934475539</v>
       </c>
       <c r="F60" t="n">
-        <v>75602.7157132169</v>
+        <v>504709.25768682</v>
       </c>
       <c r="G60" t="n">
-        <v>93690.1136898472</v>
+        <v>503101.142006486</v>
       </c>
       <c r="H60" t="n">
-        <v>11555.9107257463</v>
+        <v>77791.0292286628</v>
       </c>
       <c r="I60" t="n">
-        <v>775.86468003</v>
+        <v>4400.138424</v>
       </c>
       <c r="J60" t="n">
-        <v>63.7279721857703</v>
+        <v>73.4157137815196</v>
       </c>
       <c r="K60" t="n">
-        <v>37.6963463568015</v>
+        <v>39.4844116325389</v>
       </c>
       <c r="L60" t="s">
         <v>15</v>
@@ -2680,34 +2680,34 @@
         <v>12</v>
       </c>
       <c r="B61" t="n">
-        <v>3501.320827441</v>
+        <v>166329.139744071</v>
       </c>
       <c r="C61" t="n">
-        <v>1107.70706023</v>
+        <v>5917.944872</v>
       </c>
       <c r="D61" t="n">
-        <v>58.3894615491085</v>
+        <v>134.026400391812</v>
       </c>
       <c r="E61" t="n">
-        <v>53.5479610122171</v>
+        <v>52.9795177173176</v>
       </c>
       <c r="F61" t="n">
-        <v>67714.3610813534</v>
+        <v>453843.06440615</v>
       </c>
       <c r="G61" t="n">
-        <v>97013.4625995081</v>
+        <v>518296.16702679</v>
       </c>
       <c r="H61" t="n">
-        <v>7919.531663948</v>
+        <v>57907.2156753563</v>
       </c>
       <c r="I61" t="n">
-        <v>813.81091119</v>
+        <v>4573.636293</v>
       </c>
       <c r="J61" t="n">
-        <v>45.9175732204687</v>
+        <v>57.7671898730524</v>
       </c>
       <c r="K61" t="n">
-        <v>39.4234032395588</v>
+        <v>40.9649352029195</v>
       </c>
       <c r="L61" t="s">
         <v>15</v>
@@ -2718,34 +2718,34 @@
         <v>13</v>
       </c>
       <c r="B62" t="n">
-        <v>2900.84930507</v>
+        <v>186159.330271138</v>
       </c>
       <c r="C62" t="n">
-        <v>1034.58997803</v>
+        <v>5619.207819</v>
       </c>
       <c r="D62" t="n">
-        <v>61.4973152628231</v>
+        <v>149.706149466242</v>
       </c>
       <c r="E62" t="n">
-        <v>50.1147803875143</v>
+        <v>50.3839876701363</v>
       </c>
       <c r="F62" t="n">
-        <v>74013.3742364495</v>
+        <v>499313.442393003</v>
       </c>
       <c r="G62" t="n">
-        <v>90609.836971337</v>
+        <v>492132.64694208</v>
       </c>
       <c r="H62" t="n">
-        <v>11179.6821328472</v>
+        <v>77323.7347515964</v>
       </c>
       <c r="I62" t="n">
-        <v>740.69383555</v>
+        <v>4274.89929</v>
       </c>
       <c r="J62" t="n">
-        <v>60.7424368239093</v>
+        <v>73.4206159768654</v>
       </c>
       <c r="K62" t="n">
-        <v>35.9902229052603</v>
+        <v>38.3694056113146</v>
       </c>
       <c r="L62" t="s">
         <v>15</v>
@@ -2756,34 +2756,34 @@
         <v>14</v>
       </c>
       <c r="B63" t="n">
-        <v>4267.09104502</v>
+        <v>183676.64595247</v>
       </c>
       <c r="C63" t="n">
-        <v>1030.46181732</v>
+        <v>5773.985992</v>
       </c>
       <c r="D63" t="n">
-        <v>56.1882413883208</v>
+        <v>142.149458381102</v>
       </c>
       <c r="E63" t="n">
-        <v>49.920815174173</v>
+        <v>51.860282639682</v>
       </c>
       <c r="F63" t="n">
-        <v>72869.0238984282</v>
+        <v>505310.158402147</v>
       </c>
       <c r="G63" t="n">
-        <v>88979.1606075889</v>
+        <v>498576.869412127</v>
       </c>
       <c r="H63" t="n">
-        <v>11140.7236489092</v>
+        <v>75088.843026052</v>
       </c>
       <c r="I63" t="n">
-        <v>736.56565708</v>
+        <v>4429.677375</v>
       </c>
       <c r="J63" t="n">
-        <v>57.0779875603305</v>
+        <v>67.7271809432991</v>
       </c>
       <c r="K63" t="n">
-        <v>35.7735617841142</v>
+        <v>39.8263549331731</v>
       </c>
       <c r="L63" t="s">
         <v>15</v>
@@ -2794,34 +2794,34 @@
         <v>15</v>
       </c>
       <c r="B64" t="n">
-        <v>151.0818007</v>
+        <v>214149.49953893</v>
       </c>
       <c r="C64" t="n">
-        <v>843.41277021</v>
+        <v>4916.777897</v>
       </c>
       <c r="D64" t="n">
-        <v>56.2098101963724</v>
+        <v>168.230102446458</v>
       </c>
       <c r="E64" t="n">
-        <v>40.8915209502375</v>
+        <v>44.1874367512114</v>
       </c>
       <c r="F64" t="n">
-        <v>71271.4190562468</v>
+        <v>528144.410534121</v>
       </c>
       <c r="G64" t="n">
-        <v>72827.6963567513</v>
+        <v>424557.963056624</v>
       </c>
       <c r="H64" t="n">
-        <v>15884.4790040952</v>
+        <v>104436.356307479</v>
       </c>
       <c r="I64" t="n">
-        <v>549.51663448</v>
+        <v>3572.469213</v>
       </c>
       <c r="J64" t="n">
-        <v>79.8586770822312</v>
+        <v>92.8568541236453</v>
       </c>
       <c r="K64" t="n">
-        <v>26.744268718725</v>
+        <v>32.1535083549023</v>
       </c>
       <c r="L64" t="s">
         <v>15</v>
@@ -2832,34 +2832,34 @@
         <v>16</v>
       </c>
       <c r="B65" t="n">
-        <v>11250.1492971</v>
+        <v>197096.38234033</v>
       </c>
       <c r="C65" t="n">
-        <v>1247.39889322</v>
+        <v>6529.732686</v>
       </c>
       <c r="D65" t="n">
-        <v>85.5205283965017</v>
+        <v>152.766732696951</v>
       </c>
       <c r="E65" t="n">
-        <v>60.3360520595744</v>
+        <v>58.5492934473676</v>
       </c>
       <c r="F65" t="n">
-        <v>85315.9997534122</v>
+        <v>538667.296211295</v>
       </c>
       <c r="G65" t="n">
-        <v>107711.420836745</v>
+        <v>563834.703650926</v>
       </c>
       <c r="H65" t="n">
-        <v>14916.3700450375</v>
+        <v>89082.5830168385</v>
       </c>
       <c r="I65" t="n">
-        <v>953.50272313</v>
+        <v>5185.424042</v>
       </c>
       <c r="J65" t="n">
-        <v>68.4760140985721</v>
+        <v>74.3867678145332</v>
       </c>
       <c r="K65" t="n">
-        <v>46.1887981769321</v>
+        <v>46.5153654105036</v>
       </c>
       <c r="L65" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
SZHP baseline package & add CO2 to TDV script
</commit_message>
<xml_diff>
--- a/framework/analysis/lr/TDVAnnual.xlsx
+++ b/framework/analysis/lr/TDVAnnual.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">CZ</t>
   </si>
@@ -30,12 +30,6 @@
     <t xml:space="preserve">kTDV_Total_NG_2022</t>
   </si>
   <si>
-    <t xml:space="preserve">Source_kBtu_Elec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source_kBtu_NG</t>
-  </si>
-  <si>
     <t xml:space="preserve">kWh_Elec_Comp</t>
   </si>
   <si>
@@ -48,22 +42,40 @@
     <t xml:space="preserve">kTDV_Comp_NG_2022</t>
   </si>
   <si>
+    <t xml:space="preserve">Source_kBtu_Elec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source_kBtu_NG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source_kBtu_Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2_ton_Elec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2_ton_NG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2_ton_Total</t>
+  </si>
+  <si>
     <t xml:space="preserve">Measure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lrgs-low-SZHPbase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lrlc-flat19-SZHPbase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lrlc-baseline-all</t>
   </si>
   <si>
     <t xml:space="preserve">lrgs-low-baseszac</t>
   </si>
   <si>
-    <t xml:space="preserve">lrlc-baseline-all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lrgs-low-base</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lrlc-flat19-base</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LifeTime: ,30,TDVMultiplier: ,res,DHW Removed: ,FALSE,PVB Removed: ,TRUE</t>
+    <t xml:space="preserve">LifeTime:  30 TDVMultiplier:  res DHW Removed:  FALSE PVB Removed:  TRUE Date Produced:  2021-03-01</t>
   </si>
 </sst>
 </file>
@@ -432,43 +444,67 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>22412.338059469</v>
+        <v>30735.172454769</v>
       </c>
       <c r="C2" t="n">
-        <v>2109.97350786</v>
+        <v>1328.78917726</v>
       </c>
       <c r="D2" t="n">
-        <v>88.2884163202638</v>
+        <v>122.778491963397</v>
       </c>
       <c r="E2" t="n">
-        <v>102.510602155379</v>
+        <v>63.9254211578953</v>
       </c>
       <c r="F2" t="n">
-        <v>59114.4892718639</v>
+        <v>10825.3347131744</v>
       </c>
       <c r="G2" t="n">
-        <v>184792.390822377</v>
+        <v>1034.89303802</v>
       </c>
       <c r="H2" t="n">
-        <v>2529.16017914569</v>
+        <v>43.9068809473274</v>
       </c>
       <c r="I2" t="n">
-        <v>1816.07737098014</v>
+        <v>49.8008639104389</v>
       </c>
       <c r="J2" t="n">
-        <v>9.51917065356799</v>
+        <v>86083.9336122595</v>
       </c>
       <c r="K2" t="n">
-        <v>88.3860451304422</v>
-      </c>
-      <c r="L2" t="s">
-        <v>12</v>
+        <v>116375.929863603</v>
+      </c>
+      <c r="L2" t="n">
+        <v>202459.863475862</v>
+      </c>
+      <c r="M2" t="n">
+        <v>5.30285905039593</v>
+      </c>
+      <c r="N2" t="n">
+        <v>7.77015058140873</v>
+      </c>
+      <c r="O2" t="n">
+        <v>13.0730096318047</v>
+      </c>
+      <c r="P2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -476,37 +512,49 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>22543.519555299</v>
+        <v>27330.246599304</v>
       </c>
       <c r="C3" t="n">
-        <v>1580.90003854</v>
+        <v>1181.25209414</v>
       </c>
       <c r="D3" t="n">
-        <v>92.6769216449942</v>
+        <v>111.747470904478</v>
       </c>
       <c r="E3" t="n">
-        <v>77.3321558462802</v>
+        <v>56.9669867387733</v>
       </c>
       <c r="F3" t="n">
-        <v>59800.5719615755</v>
+        <v>7293.473423777</v>
       </c>
       <c r="G3" t="n">
-        <v>138455.90794611</v>
+        <v>887.35592234</v>
       </c>
       <c r="H3" t="n">
-        <v>2521.11881163574</v>
+        <v>34.6422812339047</v>
       </c>
       <c r="I3" t="n">
-        <v>1287.0038841677</v>
+        <v>42.8424278851332</v>
       </c>
       <c r="J3" t="n">
-        <v>15.6279803108575</v>
+        <v>77463.5536861589</v>
       </c>
       <c r="K3" t="n">
-        <v>63.2075979046658</v>
-      </c>
-      <c r="L3" t="s">
-        <v>12</v>
+        <v>103454.568423214</v>
+      </c>
+      <c r="L3" t="n">
+        <v>180918.122109373</v>
+      </c>
+      <c r="M3" t="n">
+        <v>4.77183476060367</v>
+      </c>
+      <c r="N3" t="n">
+        <v>6.90742128484109</v>
+      </c>
+      <c r="O3" t="n">
+        <v>11.6792560454448</v>
+      </c>
+      <c r="P3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4">
@@ -514,37 +562,49 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>22162.690861452</v>
+        <v>24385.710717976</v>
       </c>
       <c r="C4" t="n">
-        <v>1374.46742384</v>
+        <v>1180.28488744</v>
       </c>
       <c r="D4" t="n">
-        <v>88.60930678235</v>
+        <v>97.808730748672</v>
       </c>
       <c r="E4" t="n">
-        <v>66.72803064856</v>
+        <v>56.8230823603711</v>
       </c>
       <c r="F4" t="n">
-        <v>58644.3115179705</v>
+        <v>4384.8393753676</v>
       </c>
       <c r="G4" t="n">
-        <v>120376.450421159</v>
+        <v>886.38872916</v>
       </c>
       <c r="H4" t="n">
-        <v>2171.42629957606</v>
+        <v>19.6621832883062</v>
       </c>
       <c r="I4" t="n">
-        <v>1080.5712609843</v>
+        <v>42.6985241518383</v>
       </c>
       <c r="J4" t="n">
-        <v>10.5013610078282</v>
+        <v>67641.3929961064</v>
       </c>
       <c r="K4" t="n">
-        <v>52.6034721607589</v>
-      </c>
-      <c r="L4" t="s">
-        <v>12</v>
+        <v>103369.860042826</v>
+      </c>
+      <c r="L4" t="n">
+        <v>171011.253038932</v>
+      </c>
+      <c r="M4" t="n">
+        <v>4.16677953689268</v>
+      </c>
+      <c r="N4" t="n">
+        <v>6.90176550299777</v>
+      </c>
+      <c r="O4" t="n">
+        <v>11.0685450398904</v>
+      </c>
+      <c r="P4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -552,37 +612,49 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>23103.489031248</v>
+        <v>24646.598120517</v>
       </c>
       <c r="C5" t="n">
-        <v>1281.7087638</v>
+        <v>1107.1874831</v>
       </c>
       <c r="D5" t="n">
-        <v>96.2718150811335</v>
+        <v>104.957698465084</v>
       </c>
       <c r="E5" t="n">
-        <v>62.3227211764989</v>
+        <v>53.4144432284655</v>
       </c>
       <c r="F5" t="n">
-        <v>61743.3095376734</v>
+        <v>4500.402148229</v>
       </c>
       <c r="G5" t="n">
-        <v>112252.606925296</v>
+        <v>813.29133789</v>
       </c>
       <c r="H5" t="n">
-        <v>2965.21171576757</v>
+        <v>27.7713290453116</v>
       </c>
       <c r="I5" t="n">
-        <v>987.81262856462</v>
+        <v>39.289885624116</v>
       </c>
       <c r="J5" t="n">
-        <v>19.1127050617248</v>
+        <v>68772.8910076374</v>
       </c>
       <c r="K5" t="n">
-        <v>48.198164044124</v>
-      </c>
-      <c r="L5" t="s">
-        <v>12</v>
+        <v>96967.9578101296</v>
+      </c>
+      <c r="L5" t="n">
+        <v>165740.848817767</v>
+      </c>
+      <c r="M5" t="n">
+        <v>4.2364809808111</v>
+      </c>
+      <c r="N5" t="n">
+        <v>6.47432535782507</v>
+      </c>
+      <c r="O5" t="n">
+        <v>10.7108063386362</v>
+      </c>
+      <c r="P5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6">
@@ -590,37 +662,49 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>22153.317999506</v>
+        <v>23816.425242964</v>
       </c>
       <c r="C6" t="n">
-        <v>1330.1573014</v>
+        <v>1161.1911062</v>
       </c>
       <c r="D6" t="n">
-        <v>87.49378582589</v>
+        <v>94.7797631775204</v>
       </c>
       <c r="E6" t="n">
-        <v>64.3889010001654</v>
+        <v>55.8479862847407</v>
       </c>
       <c r="F6" t="n">
-        <v>58582.3834437173</v>
+        <v>3793.4306272791</v>
       </c>
       <c r="G6" t="n">
-        <v>116495.750766486</v>
+        <v>867.2949263</v>
       </c>
       <c r="H6" t="n">
-        <v>2142.06295214739</v>
+        <v>15.8472310413094</v>
       </c>
       <c r="I6" t="n">
-        <v>1036.26116291667</v>
+        <v>41.7234270269359</v>
       </c>
       <c r="J6" t="n">
-        <v>8.60612409327883</v>
+        <v>66020.8516541614</v>
       </c>
       <c r="K6" t="n">
-        <v>50.2643437743682</v>
-      </c>
-      <c r="L6" t="s">
-        <v>12</v>
+        <v>101697.618437879</v>
+      </c>
+      <c r="L6" t="n">
+        <v>167718.47009204</v>
+      </c>
+      <c r="M6" t="n">
+        <v>4.06695251968897</v>
+      </c>
+      <c r="N6" t="n">
+        <v>6.79011381442125</v>
+      </c>
+      <c r="O6" t="n">
+        <v>10.8570663341102</v>
+      </c>
+      <c r="P6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7">
@@ -628,37 +712,49 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>22824.736391637</v>
+        <v>22746.892751197</v>
       </c>
       <c r="C7" t="n">
-        <v>1094.31645402</v>
+        <v>1058.35661922</v>
       </c>
       <c r="D7" t="n">
-        <v>94.8985928965348</v>
+        <v>95.3025068368275</v>
       </c>
       <c r="E7" t="n">
-        <v>52.8628290105597</v>
+        <v>51.0161440534564</v>
       </c>
       <c r="F7" t="n">
-        <v>61068.3480344425</v>
+        <v>2543.7667901027</v>
       </c>
       <c r="G7" t="n">
-        <v>94492.9330530789</v>
+        <v>764.46045407</v>
       </c>
       <c r="H7" t="n">
-        <v>2625.31581731824</v>
+        <v>17.2700634894028</v>
       </c>
       <c r="I7" t="n">
-        <v>800.4202732668</v>
+        <v>36.8688903672142</v>
       </c>
       <c r="J7" t="n">
-        <v>16.8807864172737</v>
+        <v>61800.8386667808</v>
       </c>
       <c r="K7" t="n">
-        <v>38.7155745127215</v>
-      </c>
-      <c r="L7" t="s">
-        <v>12</v>
+        <v>91387.843798619</v>
+      </c>
+      <c r="L7" t="n">
+        <v>153188.6824654</v>
+      </c>
+      <c r="M7" t="n">
+        <v>3.8069953694533</v>
+      </c>
+      <c r="N7" t="n">
+        <v>6.18878482825043</v>
+      </c>
+      <c r="O7" t="n">
+        <v>9.99578019770373</v>
+      </c>
+      <c r="P7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8">
@@ -666,37 +762,49 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>22972.210245018</v>
+        <v>22587.00166314</v>
       </c>
       <c r="C8" t="n">
-        <v>1089.44321467</v>
+        <v>1075.48238307</v>
       </c>
       <c r="D8" t="n">
-        <v>93.2347998011782</v>
+        <v>92.1926878080721</v>
       </c>
       <c r="E8" t="n">
-        <v>52.6458675040139</v>
+        <v>51.9219771661029</v>
       </c>
       <c r="F8" t="n">
-        <v>61667.3231348664</v>
+        <v>2359.382988791</v>
       </c>
       <c r="G8" t="n">
-        <v>94072.1345921222</v>
+        <v>781.58620879</v>
       </c>
       <c r="H8" t="n">
-        <v>2746.2528246686</v>
+        <v>13.5130689825586</v>
       </c>
       <c r="I8" t="n">
-        <v>795.54703899072</v>
+        <v>37.7408286144227</v>
       </c>
       <c r="J8" t="n">
-        <v>14.5616778645056</v>
+        <v>61144.4792691667</v>
       </c>
       <c r="K8" t="n">
-        <v>38.4647188794018</v>
-      </c>
-      <c r="L8" t="s">
-        <v>12</v>
+        <v>92866.6332758458</v>
+      </c>
+      <c r="L8" t="n">
+        <v>154011.112545012</v>
+      </c>
+      <c r="M8" t="n">
+        <v>3.76656295395022</v>
+      </c>
+      <c r="N8" t="n">
+        <v>6.28892845239594</v>
+      </c>
+      <c r="O8" t="n">
+        <v>10.0554914063462</v>
+      </c>
+      <c r="P8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9">
@@ -704,37 +812,49 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>24891.113121748</v>
+        <v>24752.592293304</v>
       </c>
       <c r="C9" t="n">
-        <v>1041.96822101</v>
+        <v>1026.47003241</v>
       </c>
       <c r="D9" t="n">
-        <v>103.665282581345</v>
+        <v>103.983172164702</v>
       </c>
       <c r="E9" t="n">
-        <v>50.3130887356167</v>
+        <v>49.5157372603914</v>
       </c>
       <c r="F9" t="n">
-        <v>67358.1377059218</v>
+        <v>4440.5470414688</v>
       </c>
       <c r="G9" t="n">
-        <v>89972.7249733323</v>
+        <v>732.57386334</v>
       </c>
       <c r="H9" t="n">
-        <v>4581.23745280582</v>
+        <v>27.9116698337915</v>
       </c>
       <c r="I9" t="n">
-        <v>748.07204671984</v>
+        <v>35.3684834509751</v>
       </c>
       <c r="J9" t="n">
-        <v>27.6021779609433</v>
+        <v>67726.8367087634</v>
       </c>
       <c r="K9" t="n">
-        <v>36.1658346612252</v>
-      </c>
-      <c r="L9" t="s">
-        <v>12</v>
+        <v>88634.4746962355</v>
+      </c>
+      <c r="L9" t="n">
+        <v>156361.311404999</v>
+      </c>
+      <c r="M9" t="n">
+        <v>4.17204295767226</v>
+      </c>
+      <c r="N9" t="n">
+        <v>6.00232667124485</v>
+      </c>
+      <c r="O9" t="n">
+        <v>10.1743696289171</v>
+      </c>
+      <c r="P9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10">
@@ -742,37 +862,49 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>24637.782387486</v>
+        <v>24904.471852914</v>
       </c>
       <c r="C10" t="n">
-        <v>1075.12231205</v>
+        <v>1026.00030815</v>
       </c>
       <c r="D10" t="n">
-        <v>103.402841217832</v>
+        <v>105.368150545191</v>
       </c>
       <c r="E10" t="n">
-        <v>52.0264230709302</v>
+        <v>49.5092849118198</v>
       </c>
       <c r="F10" t="n">
-        <v>66766.1146227962</v>
+        <v>4630.6329092043</v>
       </c>
       <c r="G10" t="n">
-        <v>92835.5415686324</v>
+        <v>732.10416345</v>
       </c>
       <c r="H10" t="n">
-        <v>4368.3335429612</v>
+        <v>29.4274680262495</v>
       </c>
       <c r="I10" t="n">
-        <v>781.2261764717</v>
+        <v>35.3620322682811</v>
       </c>
       <c r="J10" t="n">
-        <v>27.479545599953</v>
+        <v>68772.9950412314</v>
       </c>
       <c r="K10" t="n">
-        <v>37.8791709070342</v>
-      </c>
-      <c r="L10" t="s">
-        <v>12</v>
+        <v>88593.914561285</v>
+      </c>
+      <c r="L10" t="n">
+        <v>157366.909602516</v>
+      </c>
+      <c r="M10" t="n">
+        <v>4.23648738938774</v>
+      </c>
+      <c r="N10" t="n">
+        <v>5.9995799388855</v>
+      </c>
+      <c r="O10" t="n">
+        <v>10.2360673282732</v>
+      </c>
+      <c r="P10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11">
@@ -780,37 +912,49 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>25699.259990046</v>
+        <v>26753.384927121</v>
       </c>
       <c r="C11" t="n">
-        <v>1120.20199518</v>
+        <v>1019.49318628</v>
       </c>
       <c r="D11" t="n">
-        <v>110.578477409453</v>
+        <v>115.936899223875</v>
       </c>
       <c r="E11" t="n">
-        <v>54.456515719586</v>
+        <v>49.2692583060921</v>
       </c>
       <c r="F11" t="n">
-        <v>69676.7140988046</v>
+        <v>6474.3766425549</v>
       </c>
       <c r="G11" t="n">
-        <v>96728.1189528149</v>
+        <v>725.59702795</v>
       </c>
       <c r="H11" t="n">
-        <v>5426.9141796189</v>
+        <v>39.3462729278307</v>
       </c>
       <c r="I11" t="n">
-        <v>826.3058358483</v>
+        <v>35.1220049507782</v>
       </c>
       <c r="J11" t="n">
-        <v>34.0138954295134</v>
+        <v>75003.7607279967</v>
       </c>
       <c r="K11" t="n">
-        <v>40.309262321822</v>
-      </c>
-      <c r="L11" t="s">
-        <v>12</v>
+        <v>88032.0322748848</v>
+      </c>
+      <c r="L11" t="n">
+        <v>163035.793002882</v>
+      </c>
+      <c r="M11" t="n">
+        <v>4.62030897869595</v>
+      </c>
+      <c r="N11" t="n">
+        <v>5.96152927016637</v>
+      </c>
+      <c r="O11" t="n">
+        <v>10.5818382488623</v>
+      </c>
+      <c r="P11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12">
@@ -818,37 +962,49 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>27196.29254902</v>
+        <v>31774.69057071</v>
       </c>
       <c r="C12" t="n">
-        <v>1421.09476549</v>
+        <v>1069.76081079</v>
       </c>
       <c r="D12" t="n">
-        <v>122.230661607986</v>
+        <v>141.387224394219</v>
       </c>
       <c r="E12" t="n">
-        <v>69.837867050281</v>
+        <v>51.8209032565899</v>
       </c>
       <c r="F12" t="n">
-        <v>73012.0443149839</v>
+        <v>11555.9107257463</v>
       </c>
       <c r="G12" t="n">
-        <v>124460.093134727</v>
+        <v>775.86468003</v>
       </c>
       <c r="H12" t="n">
-        <v>6988.90714459473</v>
+        <v>63.7279721857703</v>
       </c>
       <c r="I12" t="n">
-        <v>1127.19865573481</v>
+        <v>37.6963463568015</v>
       </c>
       <c r="J12" t="n">
-        <v>44.6179577092243</v>
+        <v>90866.036016694</v>
       </c>
       <c r="K12" t="n">
-        <v>55.7133112090727</v>
-      </c>
-      <c r="L12" t="s">
-        <v>12</v>
+        <v>93690.1136898472</v>
+      </c>
+      <c r="L12" t="n">
+        <v>184556.149706541</v>
+      </c>
+      <c r="M12" t="n">
+        <v>5.59744148815368</v>
+      </c>
+      <c r="N12" t="n">
+        <v>6.25547131793185</v>
+      </c>
+      <c r="O12" t="n">
+        <v>11.8529128060855</v>
+      </c>
+      <c r="P12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13">
@@ -856,37 +1012,49 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>24091.675496012</v>
+        <v>28079.633851031</v>
       </c>
       <c r="C13" t="n">
-        <v>1433.67323173</v>
+        <v>1107.70706023</v>
       </c>
       <c r="D13" t="n">
-        <v>106.063459218684</v>
+        <v>123.478478549197</v>
       </c>
       <c r="E13" t="n">
-        <v>70.2604368080786</v>
+        <v>53.5479610122171</v>
       </c>
       <c r="F13" t="n">
-        <v>64778.6269724753</v>
+        <v>7919.531663948</v>
       </c>
       <c r="G13" t="n">
-        <v>125561.720638916</v>
+        <v>813.81091119</v>
       </c>
       <c r="H13" t="n">
-        <v>3942.46287148064</v>
+        <v>45.9175732204687</v>
       </c>
       <c r="I13" t="n">
-        <v>1139.77708303009</v>
+        <v>39.4234032395588</v>
       </c>
       <c r="J13" t="n">
-        <v>28.5464985966722</v>
+        <v>80574.649564886</v>
       </c>
       <c r="K13" t="n">
-        <v>56.1358790510155</v>
-      </c>
-      <c r="L13" t="s">
-        <v>12</v>
+        <v>97013.4625995081</v>
+      </c>
+      <c r="L13" t="n">
+        <v>177588.112164394</v>
+      </c>
+      <c r="M13" t="n">
+        <v>4.96348147381577</v>
+      </c>
+      <c r="N13" t="n">
+        <v>6.47736360693776</v>
+      </c>
+      <c r="O13" t="n">
+        <v>11.4408450807535</v>
+      </c>
+      <c r="P13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14">
@@ -894,37 +1062,49 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>27895.3627617635</v>
+        <v>31437.9920177735</v>
       </c>
       <c r="C14" t="n">
-        <v>1293.96971283</v>
+        <v>1034.58997803</v>
       </c>
       <c r="D14" t="n">
-        <v>123.036424866407</v>
+        <v>138.271901604602</v>
       </c>
       <c r="E14" t="n">
-        <v>63.4464474354856</v>
+        <v>50.1147803875143</v>
       </c>
       <c r="F14" t="n">
-        <v>75546.1545320567</v>
+        <v>11179.6821328472</v>
       </c>
       <c r="G14" t="n">
-        <v>113326.426135141</v>
+        <v>740.69383555</v>
       </c>
       <c r="H14" t="n">
-        <v>7645.8934712822</v>
+        <v>60.7424368239093</v>
       </c>
       <c r="I14" t="n">
-        <v>1000.07356264392</v>
+        <v>35.9902229052603</v>
       </c>
       <c r="J14" t="n">
-        <v>45.5448177633257</v>
+        <v>89535.5868956426</v>
       </c>
       <c r="K14" t="n">
-        <v>49.3218895840806</v>
-      </c>
-      <c r="L14" t="s">
-        <v>12</v>
+        <v>90609.836971337</v>
+      </c>
+      <c r="L14" t="n">
+        <v>180145.42386698</v>
+      </c>
+      <c r="M14" t="n">
+        <v>5.51548445079946</v>
+      </c>
+      <c r="N14" t="n">
+        <v>6.04980839465138</v>
+      </c>
+      <c r="O14" t="n">
+        <v>11.5652928454508</v>
+      </c>
+      <c r="P14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15">
@@ -932,37 +1112,49 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>26492.45677319</v>
+        <v>30701.417777173</v>
       </c>
       <c r="C15" t="n">
-        <v>1359.74079552</v>
+        <v>1030.46181732</v>
       </c>
       <c r="D15" t="n">
-        <v>110.557331935402</v>
+        <v>130.060531198755</v>
       </c>
       <c r="E15" t="n">
-        <v>66.834128246961</v>
+        <v>49.920815174173</v>
       </c>
       <c r="F15" t="n">
-        <v>71822.0066868266</v>
+        <v>10492.9917289092</v>
       </c>
       <c r="G15" t="n">
-        <v>117412.011387214</v>
+        <v>736.56565708</v>
       </c>
       <c r="H15" t="n">
-        <v>6296.27529205534</v>
+        <v>54.7400612373811</v>
       </c>
       <c r="I15" t="n">
-        <v>1065.84462763463</v>
+        <v>35.7735617841142</v>
       </c>
       <c r="J15" t="n">
-        <v>35.2806189234038</v>
+        <v>89823.0155062414</v>
       </c>
       <c r="K15" t="n">
-        <v>52.6868745376419</v>
-      </c>
-      <c r="L15" t="s">
-        <v>12</v>
+        <v>88979.1606075889</v>
+      </c>
+      <c r="L15" t="n">
+        <v>178802.17611383</v>
+      </c>
+      <c r="M15" t="n">
+        <v>5.53319034950898</v>
+      </c>
+      <c r="N15" t="n">
+        <v>6.02566880133599</v>
+      </c>
+      <c r="O15" t="n">
+        <v>11.558859150845</v>
+      </c>
+      <c r="P15" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16">
@@ -970,37 +1162,49 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>35387.785734647</v>
+        <v>35700.297252207</v>
       </c>
       <c r="C16" t="n">
-        <v>847.71650831</v>
+        <v>843.41277021</v>
       </c>
       <c r="D16" t="n">
-        <v>151.824172414797</v>
+        <v>154.191011930537</v>
       </c>
       <c r="E16" t="n">
-        <v>41.1137036774873</v>
+        <v>40.8915209502375</v>
       </c>
       <c r="F16" t="n">
-        <v>93769.1497170609</v>
+        <v>15236.7471610952</v>
       </c>
       <c r="G16" t="n">
-        <v>73199.3190575408</v>
+        <v>549.51663448</v>
       </c>
       <c r="H16" t="n">
-        <v>14925.0356490264</v>
+        <v>77.5155395528787</v>
       </c>
       <c r="I16" t="n">
-        <v>553.8203714833</v>
+        <v>26.744268718725</v>
       </c>
       <c r="J16" t="n">
-        <v>75.1518529256129</v>
+        <v>95041.3508276929</v>
       </c>
       <c r="K16" t="n">
-        <v>26.9664513892842</v>
-      </c>
-      <c r="L16" t="s">
-        <v>12</v>
+        <v>72827.6963567513</v>
+      </c>
+      <c r="L16" t="n">
+        <v>167869.047184444</v>
+      </c>
+      <c r="M16" t="n">
+        <v>5.85464518464699</v>
+      </c>
+      <c r="N16" t="n">
+        <v>4.93189163410268</v>
+      </c>
+      <c r="O16" t="n">
+        <v>10.7865368187497</v>
+      </c>
+      <c r="P16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17">
@@ -1008,37 +1212,49 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>23297.692842667</v>
+        <v>26218.662641436</v>
       </c>
       <c r="C17" t="n">
-        <v>2189.08371792</v>
+        <v>1921.00252112</v>
       </c>
       <c r="D17" t="n">
-        <v>93.275593705566</v>
+        <v>103.751709288742</v>
       </c>
       <c r="E17" t="n">
-        <v>107.632350620382</v>
+        <v>94.3091114171104</v>
       </c>
       <c r="F17" t="n">
-        <v>62385.293211311</v>
+        <v>6164.975399906</v>
       </c>
       <c r="G17" t="n">
-        <v>189024.793006739</v>
+        <v>1627.106401489</v>
       </c>
       <c r="H17" t="n">
-        <v>3253.3613152666</v>
+        <v>23.7465502947439</v>
       </c>
       <c r="I17" t="n">
-        <v>1895.1876262228</v>
+        <v>80.1618601192387</v>
       </c>
       <c r="J17" t="n">
-        <v>13.3046884508655</v>
+        <v>71009.532541722</v>
       </c>
       <c r="K17" t="n">
-        <v>93.4851007054751</v>
-      </c>
-      <c r="L17" t="s">
-        <v>12</v>
+        <v>165876.298356079</v>
+      </c>
+      <c r="L17" t="n">
+        <v>236885.830897801</v>
+      </c>
+      <c r="M17" t="n">
+        <v>4.37426040495934</v>
+      </c>
+      <c r="N17" t="n">
+        <v>11.2331430085448</v>
+      </c>
+      <c r="O17" t="n">
+        <v>15.6074034135042</v>
+      </c>
+      <c r="P17" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18">
@@ -1046,37 +1262,49 @@
         <v>1</v>
       </c>
       <c r="B18" t="n">
-        <v>149753.982479712</v>
+        <v>174539.349900922</v>
       </c>
       <c r="C18" t="n">
-        <v>8696.770195</v>
+        <v>6619.330973</v>
       </c>
       <c r="D18" t="n">
-        <v>109.294308175781</v>
+        <v>128.510969462808</v>
       </c>
       <c r="E18" t="n">
-        <v>78.2650760720572</v>
+        <v>59.1067270304137</v>
       </c>
       <c r="F18" t="n">
-        <v>387593.56732525</v>
+        <v>67286.8278348038</v>
       </c>
       <c r="G18" t="n">
-        <v>761666.888603171</v>
+        <v>5275.022421</v>
       </c>
       <c r="H18" t="n">
-        <v>42586.8161831916</v>
+        <v>51.0179576622851</v>
       </c>
       <c r="I18" t="n">
-        <v>7352.46149568424</v>
+        <v>47.0921446191635</v>
       </c>
       <c r="J18" t="n">
-        <v>31.8627964983222</v>
+        <v>469390.159800459</v>
       </c>
       <c r="K18" t="n">
-        <v>66.2504924891521</v>
-      </c>
-      <c r="L18" t="s">
-        <v>13</v>
+        <v>579723.864583444</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1049114.0243839</v>
+      </c>
+      <c r="M18" t="n">
+        <v>28.9149177159601</v>
+      </c>
+      <c r="N18" t="n">
+        <v>38.7068161666168</v>
+      </c>
+      <c r="O18" t="n">
+        <v>67.6217338825769</v>
+      </c>
+      <c r="P18" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19">
@@ -1084,37 +1312,49 @@
         <v>2</v>
       </c>
       <c r="B19" t="n">
-        <v>143041.6992896</v>
+        <v>158415.57558209</v>
       </c>
       <c r="C19" t="n">
-        <v>7341.997463</v>
+        <v>6186.758084</v>
       </c>
       <c r="D19" t="n">
-        <v>108.997595565136</v>
+        <v>120.557879089585</v>
       </c>
       <c r="E19" t="n">
-        <v>66.2800542546027</v>
+        <v>55.31458802475</v>
       </c>
       <c r="F19" t="n">
-        <v>373325.813865395</v>
+        <v>50560.2932897283</v>
       </c>
       <c r="G19" t="n">
-        <v>643015.307796756</v>
+        <v>4842.449626</v>
       </c>
       <c r="H19" t="n">
-        <v>35232.7420231726</v>
+        <v>44.4427335927938</v>
       </c>
       <c r="I19" t="n">
-        <v>5997.6890156942</v>
+        <v>43.3000065195435</v>
       </c>
       <c r="J19" t="n">
-        <v>32.916111155739</v>
+        <v>430516.548583787</v>
       </c>
       <c r="K19" t="n">
-        <v>54.2654728395149</v>
-      </c>
-      <c r="L19" t="s">
-        <v>13</v>
+        <v>541838.944196776</v>
+      </c>
+      <c r="L19" t="n">
+        <v>972355.492780563</v>
+      </c>
+      <c r="M19" t="n">
+        <v>26.5202631920346</v>
+      </c>
+      <c r="N19" t="n">
+        <v>36.17732801117</v>
+      </c>
+      <c r="O19" t="n">
+        <v>62.6975912032046</v>
+      </c>
+      <c r="P19" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20">
@@ -1122,37 +1362,49 @@
         <v>3</v>
       </c>
       <c r="B20" t="n">
-        <v>136229.96591973</v>
+        <v>142451.48789468</v>
       </c>
       <c r="C20" t="n">
-        <v>6625.982674</v>
+        <v>6176.655733</v>
       </c>
       <c r="D20" t="n">
-        <v>100.565010403691</v>
+        <v>105.472106669281</v>
       </c>
       <c r="E20" t="n">
-        <v>59.4585968502382</v>
+        <v>55.1829882749937</v>
       </c>
       <c r="F20" t="n">
-        <v>353206.967151864</v>
+        <v>34692.2513553354</v>
       </c>
       <c r="G20" t="n">
-        <v>580306.423428968</v>
+        <v>4832.347197</v>
       </c>
       <c r="H20" t="n">
-        <v>28498.1004077125</v>
+        <v>28.4750778340043</v>
       </c>
       <c r="I20" t="n">
-        <v>5281.6741805551</v>
+        <v>43.1684061377285</v>
       </c>
       <c r="J20" t="n">
-        <v>23.5884503389445</v>
+        <v>378741.555426775</v>
       </c>
       <c r="K20" t="n">
-        <v>47.4440151078061</v>
-      </c>
-      <c r="L20" t="s">
-        <v>13</v>
+        <v>540954.175934396</v>
+      </c>
+      <c r="L20" t="n">
+        <v>919695.731361172</v>
+      </c>
+      <c r="M20" t="n">
+        <v>23.3308702411559</v>
+      </c>
+      <c r="N20" t="n">
+        <v>36.118254088956</v>
+      </c>
+      <c r="O20" t="n">
+        <v>59.449124330112</v>
+      </c>
+      <c r="P20" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21">
@@ -1160,37 +1412,49 @@
         <v>4</v>
       </c>
       <c r="B21" t="n">
-        <v>143535.24887464</v>
+        <v>147493.06751551</v>
       </c>
       <c r="C21" t="n">
-        <v>6375.030487</v>
+        <v>5916.584654</v>
       </c>
       <c r="D21" t="n">
-        <v>111.307895238578</v>
+        <v>115.764514220389</v>
       </c>
       <c r="E21" t="n">
-        <v>57.279707155273</v>
+        <v>52.9186196440184</v>
       </c>
       <c r="F21" t="n">
-        <v>373253.095152146</v>
+        <v>39068.0117372254</v>
       </c>
       <c r="G21" t="n">
-        <v>558327.922540173</v>
+        <v>4572.276035</v>
       </c>
       <c r="H21" t="n">
-        <v>35134.3757147033</v>
+        <v>39.6907269127699</v>
       </c>
       <c r="I21" t="n">
-        <v>5030.7218267762</v>
+        <v>40.90403674999</v>
       </c>
       <c r="J21" t="n">
-        <v>35.2501284085163</v>
+        <v>393221.658867331</v>
       </c>
       <c r="K21" t="n">
-        <v>45.265123941294</v>
-      </c>
-      <c r="L21" t="s">
-        <v>13</v>
+        <v>518177.038547061</v>
+      </c>
+      <c r="L21" t="n">
+        <v>911398.697414392</v>
+      </c>
+      <c r="M21" t="n">
+        <v>24.2228595399522</v>
+      </c>
+      <c r="N21" t="n">
+        <v>34.5974775201203</v>
+      </c>
+      <c r="O21" t="n">
+        <v>58.8203370600725</v>
+      </c>
+      <c r="P21" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="22">
@@ -1198,37 +1462,49 @@
         <v>5</v>
       </c>
       <c r="B22" t="n">
-        <v>136820.48302102</v>
+        <v>140297.490604088</v>
       </c>
       <c r="C22" t="n">
-        <v>6554.546615</v>
+        <v>6177.467889</v>
       </c>
       <c r="D22" t="n">
-        <v>99.7372002783615</v>
+        <v>102.840327839211</v>
       </c>
       <c r="E22" t="n">
-        <v>58.7383453960818</v>
+        <v>55.1824275327287</v>
       </c>
       <c r="F22" t="n">
-        <v>355026.99625769</v>
+        <v>32393.3827800968</v>
       </c>
       <c r="G22" t="n">
-        <v>574050.022538453</v>
+        <v>4833.159286</v>
       </c>
       <c r="H22" t="n">
-        <v>28949.4752215308</v>
+        <v>25.2633649332074</v>
       </c>
       <c r="I22" t="n">
-        <v>5210.237931358</v>
+        <v>43.1678448063354</v>
       </c>
       <c r="J22" t="n">
-        <v>22.1835100841028</v>
+        <v>373264.070795594</v>
       </c>
       <c r="K22" t="n">
-        <v>46.7237619116295</v>
-      </c>
-      <c r="L22" t="s">
-        <v>13</v>
+        <v>541025.304907534</v>
+      </c>
+      <c r="L22" t="n">
+        <v>914289.375703128</v>
+      </c>
+      <c r="M22" t="n">
+        <v>22.9934515413937</v>
+      </c>
+      <c r="N22" t="n">
+        <v>36.1230032053122</v>
+      </c>
+      <c r="O22" t="n">
+        <v>59.1164547467059</v>
+      </c>
+      <c r="P22" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="23">
@@ -1236,37 +1512,49 @@
         <v>6</v>
       </c>
       <c r="B23" t="n">
-        <v>139719.99736543</v>
+        <v>138467.50910603</v>
       </c>
       <c r="C23" t="n">
-        <v>5810.479147</v>
+        <v>5760.430606</v>
       </c>
       <c r="D23" t="n">
-        <v>107.586362881489</v>
+        <v>107.320439711938</v>
       </c>
       <c r="E23" t="n">
-        <v>52.0435003408487</v>
+        <v>51.5664691108899</v>
       </c>
       <c r="F23" t="n">
-        <v>360841.743775931</v>
+        <v>29688.3152938539</v>
       </c>
       <c r="G23" t="n">
-        <v>501728.010235828</v>
+        <v>4416.12169</v>
       </c>
       <c r="H23" t="n">
-        <v>30949.3851436631</v>
+        <v>30.4225256930972</v>
       </c>
       <c r="I23" t="n">
-        <v>4466.1702918795</v>
+        <v>39.5325387384548</v>
       </c>
       <c r="J23" t="n">
-        <v>30.6945074197909</v>
+        <v>360167.423522868</v>
       </c>
       <c r="K23" t="n">
-        <v>40.0095705356774</v>
-      </c>
-      <c r="L23" t="s">
-        <v>13</v>
+        <v>497406.377844445</v>
+      </c>
+      <c r="L23" t="n">
+        <v>857573.801367312</v>
+      </c>
+      <c r="M23" t="n">
+        <v>22.1866845686757</v>
+      </c>
+      <c r="N23" t="n">
+        <v>33.6843601591267</v>
+      </c>
+      <c r="O23" t="n">
+        <v>55.8710447278025</v>
+      </c>
+      <c r="P23" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="24">
@@ -1274,37 +1562,49 @@
         <v>7</v>
       </c>
       <c r="B24" t="n">
-        <v>137992.0018959</v>
+        <v>135945.913557306</v>
       </c>
       <c r="C24" t="n">
-        <v>5760.495689</v>
+        <v>5747.447556</v>
       </c>
       <c r="D24" t="n">
-        <v>103.36197207864</v>
+        <v>102.363543579989</v>
       </c>
       <c r="E24" t="n">
-        <v>51.6950752895751</v>
+        <v>51.5693343359411</v>
       </c>
       <c r="F24" t="n">
-        <v>357931.598064233</v>
+        <v>27044.5887182028</v>
       </c>
       <c r="G24" t="n">
-        <v>497411.99768461</v>
+        <v>4403.138861</v>
       </c>
       <c r="H24" t="n">
-        <v>29093.0850377257</v>
+        <v>24.9812350645138</v>
       </c>
       <c r="I24" t="n">
-        <v>4416.187017021</v>
+        <v>39.5064874174496</v>
       </c>
       <c r="J24" t="n">
-        <v>25.9811005159642</v>
+        <v>354149.034013217</v>
       </c>
       <c r="K24" t="n">
-        <v>39.6322285929515</v>
-      </c>
-      <c r="L24" t="s">
-        <v>13</v>
+        <v>496285.306814243</v>
+      </c>
+      <c r="L24" t="n">
+        <v>850434.34082746</v>
+      </c>
+      <c r="M24" t="n">
+        <v>21.8159455708064</v>
+      </c>
+      <c r="N24" t="n">
+        <v>33.6084412283946</v>
+      </c>
+      <c r="O24" t="n">
+        <v>55.4243867992011</v>
+      </c>
+      <c r="P24" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="25">
@@ -1312,37 +1612,49 @@
         <v>8</v>
       </c>
       <c r="B25" t="n">
-        <v>149113.68023369</v>
+        <v>148116.09817302</v>
       </c>
       <c r="C25" t="n">
-        <v>5649.62038</v>
+        <v>5624.593541</v>
       </c>
       <c r="D25" t="n">
-        <v>114.130295366572</v>
+        <v>114.088421286293</v>
       </c>
       <c r="E25" t="n">
-        <v>50.614321783342</v>
+        <v>50.3746175429341</v>
       </c>
       <c r="F25" t="n">
-        <v>383473.062026314</v>
+        <v>38990.9894970714</v>
       </c>
       <c r="G25" t="n">
-        <v>487838.045733061</v>
+        <v>4280.284804</v>
       </c>
       <c r="H25" t="n">
-        <v>39993.7012375079</v>
+        <v>38.8746450167663</v>
       </c>
       <c r="I25" t="n">
-        <v>4305.311699464</v>
+        <v>38.3406887624799</v>
       </c>
       <c r="J25" t="n">
-        <v>38.9201490411927</v>
+        <v>383384.46850856</v>
       </c>
       <c r="K25" t="n">
-        <v>38.5803935371693</v>
-      </c>
-      <c r="L25" t="s">
-        <v>13</v>
+        <v>485677.007750429</v>
+      </c>
+      <c r="L25" t="n">
+        <v>869061.476258988</v>
+      </c>
+      <c r="M25" t="n">
+        <v>23.6168784731547</v>
+      </c>
+      <c r="N25" t="n">
+        <v>32.8900472104293</v>
+      </c>
+      <c r="O25" t="n">
+        <v>56.506925683584</v>
+      </c>
+      <c r="P25" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="26">
@@ -1350,37 +1662,49 @@
         <v>9</v>
       </c>
       <c r="B26" t="n">
-        <v>149508.53552941</v>
+        <v>149669.92751234</v>
       </c>
       <c r="C26" t="n">
-        <v>5770.703551</v>
+        <v>5663.812742</v>
       </c>
       <c r="D26" t="n">
-        <v>115.628263460512</v>
+        <v>116.475856817925</v>
       </c>
       <c r="E26" t="n">
-        <v>51.7548839427498</v>
+        <v>50.7373254036727</v>
       </c>
       <c r="F26" t="n">
-        <v>386228.761938985</v>
+        <v>40716.1032025002</v>
       </c>
       <c r="G26" t="n">
-        <v>498293.434509431</v>
+        <v>4319.504178</v>
       </c>
       <c r="H26" t="n">
-        <v>40566.4232453719</v>
+        <v>41.3027837259902</v>
       </c>
       <c r="I26" t="n">
-        <v>4426.394947388</v>
+        <v>38.7033981521308</v>
       </c>
       <c r="J26" t="n">
-        <v>40.4635656667657</v>
+        <v>390843.585683635</v>
       </c>
       <c r="K26" t="n">
-        <v>39.7209563184306</v>
-      </c>
-      <c r="L26" t="s">
-        <v>13</v>
+        <v>489063.539425863</v>
+      </c>
+      <c r="L26" t="n">
+        <v>879907.125109498</v>
+      </c>
+      <c r="M26" t="n">
+        <v>24.0763677803926</v>
+      </c>
+      <c r="N26" t="n">
+        <v>33.1193831372021</v>
+      </c>
+      <c r="O26" t="n">
+        <v>57.1957509175947</v>
+      </c>
+      <c r="P26" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="27">
@@ -1388,37 +1712,49 @@
         <v>10</v>
       </c>
       <c r="B27" t="n">
-        <v>157035.044007763</v>
+        <v>160077.74032347</v>
       </c>
       <c r="C27" t="n">
-        <v>5928.14455</v>
+        <v>5647.063745</v>
       </c>
       <c r="D27" t="n">
-        <v>122.696684221462</v>
+        <v>125.844471203967</v>
       </c>
       <c r="E27" t="n">
-        <v>53.3281616110487</v>
+        <v>50.6348891998656</v>
       </c>
       <c r="F27" t="n">
-        <v>405896.3527276</v>
+        <v>51139.353046145</v>
       </c>
       <c r="G27" t="n">
-        <v>511888.278782919</v>
+        <v>4302.755109</v>
       </c>
       <c r="H27" t="n">
-        <v>48118.6978464883</v>
+        <v>50.4461902096793</v>
       </c>
       <c r="I27" t="n">
-        <v>4583.835910441</v>
+        <v>38.6009612904814</v>
       </c>
       <c r="J27" t="n">
-        <v>47.3143877531963</v>
+        <v>422601.091358531</v>
       </c>
       <c r="K27" t="n">
-        <v>41.2942336632156</v>
-      </c>
-      <c r="L27" t="s">
-        <v>13</v>
+        <v>487617.283321047</v>
+      </c>
+      <c r="L27" t="n">
+        <v>910218.374679578</v>
+      </c>
+      <c r="M27" t="n">
+        <v>26.032662867286</v>
+      </c>
+      <c r="N27" t="n">
+        <v>33.0214426730527</v>
+      </c>
+      <c r="O27" t="n">
+        <v>59.0541055403387</v>
+      </c>
+      <c r="P27" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="28">
@@ -1426,37 +1762,49 @@
         <v>11</v>
       </c>
       <c r="B28" t="n">
-        <v>170484.51045498</v>
+        <v>186418.26606348</v>
       </c>
       <c r="C28" t="n">
-        <v>6840.718989</v>
+        <v>5744.446926</v>
       </c>
       <c r="D28" t="n">
-        <v>137.275071783378</v>
+        <v>149.771795109047</v>
       </c>
       <c r="E28" t="n">
-        <v>61.9669056801819</v>
+        <v>51.4989934475539</v>
       </c>
       <c r="F28" t="n">
-        <v>442736.873909379</v>
+        <v>77791.0292286628</v>
       </c>
       <c r="G28" t="n">
-        <v>599113.122611406</v>
+        <v>4400.138424</v>
       </c>
       <c r="H28" t="n">
-        <v>61895.6682311594</v>
+        <v>73.4157137815196</v>
       </c>
       <c r="I28" t="n">
-        <v>5496.4104890889</v>
+        <v>39.4844116325389</v>
       </c>
       <c r="J28" t="n">
-        <v>60.9481537796566</v>
+        <v>504709.25768682</v>
       </c>
       <c r="K28" t="n">
-        <v>49.95232388295</v>
-      </c>
-      <c r="L28" t="s">
-        <v>13</v>
+        <v>503101.142006486</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1007810.39969331</v>
+      </c>
+      <c r="M28" t="n">
+        <v>31.0906105545578</v>
+      </c>
+      <c r="N28" t="n">
+        <v>33.5908949183117</v>
+      </c>
+      <c r="O28" t="n">
+        <v>64.6815054728695</v>
+      </c>
+      <c r="P28" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="29">
@@ -1464,37 +1812,49 @@
         <v>12</v>
       </c>
       <c r="B29" t="n">
-        <v>152637.976425711</v>
+        <v>166329.139744071</v>
       </c>
       <c r="C29" t="n">
-        <v>6914.970738</v>
+        <v>5917.944872</v>
       </c>
       <c r="D29" t="n">
-        <v>122.523691735952</v>
+        <v>134.026400391812</v>
       </c>
       <c r="E29" t="n">
-        <v>62.4991409877888</v>
+        <v>52.9795177173176</v>
       </c>
       <c r="F29" t="n">
-        <v>399849.078186213</v>
+        <v>57907.2156753563</v>
       </c>
       <c r="G29" t="n">
-        <v>605616.122847826</v>
+        <v>4573.636293</v>
       </c>
       <c r="H29" t="n">
-        <v>44251.9394230849</v>
+        <v>57.7671898730524</v>
       </c>
       <c r="I29" t="n">
-        <v>5570.662225892</v>
+        <v>40.9649352029195</v>
       </c>
       <c r="J29" t="n">
-        <v>46.290917311368</v>
+        <v>453843.06440615</v>
       </c>
       <c r="K29" t="n">
-        <v>50.4845590993907</v>
-      </c>
-      <c r="L29" t="s">
-        <v>13</v>
+        <v>518296.16702679</v>
+      </c>
+      <c r="L29" t="n">
+        <v>972139.23143294</v>
+      </c>
+      <c r="M29" t="n">
+        <v>27.9572006129008</v>
+      </c>
+      <c r="N29" t="n">
+        <v>34.6054314520641</v>
+      </c>
+      <c r="O29" t="n">
+        <v>62.5626320649649</v>
+      </c>
+      <c r="P29" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="30">
@@ -1502,37 +1862,49 @@
         <v>13</v>
       </c>
       <c r="B30" t="n">
-        <v>173851.647550698</v>
+        <v>186159.330271138</v>
       </c>
       <c r="C30" t="n">
-        <v>6393.784235</v>
+        <v>5619.207819</v>
       </c>
       <c r="D30" t="n">
-        <v>139.759897715118</v>
+        <v>149.706149466242</v>
       </c>
       <c r="E30" t="n">
-        <v>57.7931467903642</v>
+        <v>50.3839876701363</v>
       </c>
       <c r="F30" t="n">
-        <v>451482.82266961</v>
+        <v>77323.7347515964</v>
       </c>
       <c r="G30" t="n">
-        <v>559970.383887148</v>
+        <v>4274.89929</v>
       </c>
       <c r="H30" t="n">
-        <v>65045.247717797</v>
+        <v>73.4206159768654</v>
       </c>
       <c r="I30" t="n">
-        <v>5049.4757180326</v>
+        <v>38.3694056113146</v>
       </c>
       <c r="J30" t="n">
-        <v>63.4976705978154</v>
+        <v>499313.442393003</v>
       </c>
       <c r="K30" t="n">
-        <v>45.7785648282996</v>
-      </c>
-      <c r="L30" t="s">
-        <v>13</v>
+        <v>492132.64694208</v>
+      </c>
+      <c r="L30" t="n">
+        <v>991446.089335083</v>
+      </c>
+      <c r="M30" t="n">
+        <v>30.7582227701663</v>
+      </c>
+      <c r="N30" t="n">
+        <v>32.858553974598</v>
+      </c>
+      <c r="O30" t="n">
+        <v>63.6167767447643</v>
+      </c>
+      <c r="P30" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="31">
@@ -1540,37 +1912,49 @@
         <v>14</v>
       </c>
       <c r="B31" t="n">
-        <v>167366.62840467</v>
+        <v>180680.04207583</v>
       </c>
       <c r="C31" t="n">
-        <v>6754.363389</v>
+        <v>5773.985992</v>
       </c>
       <c r="D31" t="n">
-        <v>128.18728039526</v>
+        <v>140.138563091106</v>
       </c>
       <c r="E31" t="n">
-        <v>61.2338668307596</v>
+        <v>51.860282639682</v>
       </c>
       <c r="F31" t="n">
-        <v>439591.284920256</v>
+        <v>72092.222226052</v>
       </c>
       <c r="G31" t="n">
-        <v>583231.299491435</v>
+        <v>4429.677375</v>
       </c>
       <c r="H31" t="n">
-        <v>58819.8813587715</v>
+        <v>65.7162788990333</v>
       </c>
       <c r="I31" t="n">
-        <v>5410.0548007928</v>
+        <v>39.8263549331731</v>
       </c>
       <c r="J31" t="n">
-        <v>53.792049413419</v>
+        <v>497711.343527713</v>
       </c>
       <c r="K31" t="n">
-        <v>49.1999394187638</v>
-      </c>
-      <c r="L31" t="s">
-        <v>13</v>
+        <v>498576.869412127</v>
+      </c>
+      <c r="L31" t="n">
+        <v>996288.21293984</v>
+      </c>
+      <c r="M31" t="n">
+        <v>30.659531828536</v>
+      </c>
+      <c r="N31" t="n">
+        <v>33.763625848682</v>
+      </c>
+      <c r="O31" t="n">
+        <v>64.423157677218</v>
+      </c>
+      <c r="P31" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="32">
@@ -1578,37 +1962,49 @@
         <v>15</v>
       </c>
       <c r="B32" t="n">
-        <v>209942.47879774</v>
+        <v>211152.89393144</v>
       </c>
       <c r="C32" t="n">
-        <v>4919.170673</v>
+        <v>4916.777897</v>
       </c>
       <c r="D32" t="n">
-        <v>164.413306323774</v>
+        <v>166.214722555389</v>
       </c>
       <c r="E32" t="n">
-        <v>44.2103882820078</v>
+        <v>44.1874367512114</v>
       </c>
       <c r="F32" t="n">
-        <v>516032.561230557</v>
+        <v>101439.735897479</v>
       </c>
       <c r="G32" t="n">
-        <v>424764.57643756</v>
+        <v>3572.469213</v>
       </c>
       <c r="H32" t="n">
-        <v>100229.835889598</v>
+        <v>90.8414698268805</v>
       </c>
       <c r="I32" t="n">
-        <v>3574.8619825</v>
+        <v>32.1535083549023</v>
       </c>
       <c r="J32" t="n">
-        <v>89.0403794961183</v>
+        <v>520545.593243852</v>
       </c>
       <c r="K32" t="n">
-        <v>32.1764598235932</v>
-      </c>
-      <c r="L32" t="s">
-        <v>13</v>
+        <v>424557.963056624</v>
+      </c>
+      <c r="L32" t="n">
+        <v>945103.556300476</v>
+      </c>
+      <c r="M32" t="n">
+        <v>32.0661451498049</v>
+      </c>
+      <c r="N32" t="n">
+        <v>28.7510654728616</v>
+      </c>
+      <c r="O32" t="n">
+        <v>60.8172106226665</v>
+      </c>
+      <c r="P32" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="33">
@@ -1616,37 +2012,49 @@
         <v>16</v>
       </c>
       <c r="B33" t="n">
-        <v>158004.16494594</v>
+        <v>166585.70162063</v>
       </c>
       <c r="C33" t="n">
-        <v>9471.761148</v>
+        <v>8815.635998</v>
       </c>
       <c r="D33" t="n">
-        <v>117.849214719056</v>
+        <v>123.594517975002</v>
       </c>
       <c r="E33" t="n">
-        <v>86.0533486654822</v>
+        <v>79.996164902328</v>
       </c>
       <c r="F33" t="n">
-        <v>414267.954531748</v>
+        <v>58623.441985743</v>
       </c>
       <c r="G33" t="n">
-        <v>817875.385830907</v>
+        <v>7471.32727414</v>
       </c>
       <c r="H33" t="n">
-        <v>50065.887172835</v>
+        <v>45.2530923313518</v>
       </c>
       <c r="I33" t="n">
-        <v>8127.4525328601</v>
+        <v>67.9622361508723</v>
       </c>
       <c r="J33" t="n">
-        <v>39.5226900278527</v>
+        <v>438989.350274025</v>
       </c>
       <c r="K33" t="n">
-        <v>74.0194207932843</v>
-      </c>
-      <c r="L33" t="s">
-        <v>13</v>
+        <v>761219.754230345</v>
+      </c>
+      <c r="L33" t="n">
+        <v>1200209.10450437</v>
+      </c>
+      <c r="M33" t="n">
+        <v>27.0421965103662</v>
+      </c>
+      <c r="N33" t="n">
+        <v>51.5498021413704</v>
+      </c>
+      <c r="O33" t="n">
+        <v>78.5919986517367</v>
+      </c>
+      <c r="P33" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="34">
@@ -1654,37 +2062,49 @@
         <v>1</v>
       </c>
       <c r="B34" t="n">
-        <v>30735.172454769</v>
+        <v>149753.982479712</v>
       </c>
       <c r="C34" t="n">
-        <v>1328.78917726</v>
+        <v>8696.770195</v>
       </c>
       <c r="D34" t="n">
-        <v>122.778491963397</v>
+        <v>109.294308175781</v>
       </c>
       <c r="E34" t="n">
-        <v>63.9254211578953</v>
+        <v>78.2650760720572</v>
       </c>
       <c r="F34" t="n">
-        <v>86083.9336122595</v>
+        <v>42586.8161831916</v>
       </c>
       <c r="G34" t="n">
-        <v>116375.929863603</v>
+        <v>7352.46149568424</v>
       </c>
       <c r="H34" t="n">
-        <v>10825.3347131744</v>
+        <v>31.8627964983222</v>
       </c>
       <c r="I34" t="n">
-        <v>1034.89303802</v>
+        <v>66.2504924891521</v>
       </c>
       <c r="J34" t="n">
-        <v>43.9068809473274</v>
+        <v>387593.56732525</v>
       </c>
       <c r="K34" t="n">
-        <v>49.8008639104389</v>
-      </c>
-      <c r="L34" t="s">
-        <v>14</v>
+        <v>761666.888603171</v>
+      </c>
+      <c r="L34" t="n">
+        <v>1149260.45592842</v>
+      </c>
+      <c r="M34" t="n">
+        <v>23.876163299225</v>
+      </c>
+      <c r="N34" t="n">
+        <v>50.8547293607548</v>
+      </c>
+      <c r="O34" t="n">
+        <v>74.7308926599798</v>
+      </c>
+      <c r="P34" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="35">
@@ -1692,37 +2112,49 @@
         <v>2</v>
       </c>
       <c r="B35" t="n">
-        <v>27330.246599304</v>
+        <v>143041.6992896</v>
       </c>
       <c r="C35" t="n">
-        <v>1181.25209414</v>
+        <v>7341.997463</v>
       </c>
       <c r="D35" t="n">
-        <v>111.747470904478</v>
+        <v>108.997595565136</v>
       </c>
       <c r="E35" t="n">
-        <v>56.9669867387733</v>
+        <v>66.2800542546027</v>
       </c>
       <c r="F35" t="n">
-        <v>77463.5536861589</v>
+        <v>35232.7420231726</v>
       </c>
       <c r="G35" t="n">
-        <v>103454.568423214</v>
+        <v>5997.6890156942</v>
       </c>
       <c r="H35" t="n">
-        <v>7293.473423777</v>
+        <v>32.916111155739</v>
       </c>
       <c r="I35" t="n">
-        <v>887.35592234</v>
+        <v>54.2654728395149</v>
       </c>
       <c r="J35" t="n">
-        <v>34.6422812339047</v>
+        <v>373325.813865395</v>
       </c>
       <c r="K35" t="n">
-        <v>42.8424278851332</v>
-      </c>
-      <c r="L35" t="s">
-        <v>14</v>
+        <v>643015.307796756</v>
+      </c>
+      <c r="L35" t="n">
+        <v>1016341.12166215</v>
+      </c>
+      <c r="M35" t="n">
+        <v>22.9972549781415</v>
+      </c>
+      <c r="N35" t="n">
+        <v>42.9326388505559</v>
+      </c>
+      <c r="O35" t="n">
+        <v>65.9298938286974</v>
+      </c>
+      <c r="P35" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="36">
@@ -1730,37 +2162,49 @@
         <v>3</v>
       </c>
       <c r="B36" t="n">
-        <v>24385.710717976</v>
+        <v>136229.96591973</v>
       </c>
       <c r="C36" t="n">
-        <v>1180.28488744</v>
+        <v>6625.982674</v>
       </c>
       <c r="D36" t="n">
-        <v>97.808730748672</v>
+        <v>100.565010403691</v>
       </c>
       <c r="E36" t="n">
-        <v>56.8230823603711</v>
+        <v>59.4585968502382</v>
       </c>
       <c r="F36" t="n">
-        <v>67641.3929961064</v>
+        <v>28498.1004077125</v>
       </c>
       <c r="G36" t="n">
-        <v>103369.860042826</v>
+        <v>5281.6741805551</v>
       </c>
       <c r="H36" t="n">
-        <v>4384.8393753676</v>
+        <v>23.5884503389445</v>
       </c>
       <c r="I36" t="n">
-        <v>886.38872916</v>
+        <v>47.4440151078061</v>
       </c>
       <c r="J36" t="n">
-        <v>19.6621832883062</v>
+        <v>353206.967151864</v>
       </c>
       <c r="K36" t="n">
-        <v>42.6985241518383</v>
-      </c>
-      <c r="L36" t="s">
-        <v>14</v>
+        <v>580306.423428968</v>
+      </c>
+      <c r="L36" t="n">
+        <v>933513.390580831</v>
+      </c>
+      <c r="M36" t="n">
+        <v>21.7579132810146</v>
+      </c>
+      <c r="N36" t="n">
+        <v>38.7457122678772</v>
+      </c>
+      <c r="O36" t="n">
+        <v>60.5036255488918</v>
+      </c>
+      <c r="P36" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="37">
@@ -1768,37 +2212,49 @@
         <v>4</v>
       </c>
       <c r="B37" t="n">
-        <v>25294.326779408</v>
+        <v>143535.24887464</v>
       </c>
       <c r="C37" t="n">
-        <v>1107.1874831</v>
+        <v>6375.030487</v>
       </c>
       <c r="D37" t="n">
-        <v>107.347662692801</v>
+        <v>111.307895238578</v>
       </c>
       <c r="E37" t="n">
-        <v>53.4144432284655</v>
+        <v>57.279707155273</v>
       </c>
       <c r="F37" t="n">
-        <v>70405.4090751455</v>
+        <v>35134.3757147033</v>
       </c>
       <c r="G37" t="n">
-        <v>96967.9578101296</v>
+        <v>5030.7218267762</v>
       </c>
       <c r="H37" t="n">
-        <v>5148.134068229</v>
+        <v>35.2501284085163</v>
       </c>
       <c r="I37" t="n">
-        <v>813.29133789</v>
+        <v>45.265123941294</v>
       </c>
       <c r="J37" t="n">
-        <v>30.1613083051692</v>
+        <v>373253.095152146</v>
       </c>
       <c r="K37" t="n">
-        <v>39.289885624116</v>
-      </c>
-      <c r="L37" t="s">
-        <v>14</v>
+        <v>558327.922540173</v>
+      </c>
+      <c r="L37" t="n">
+        <v>931581.017692319</v>
+      </c>
+      <c r="M37" t="n">
+        <v>22.992775430443</v>
+      </c>
+      <c r="N37" t="n">
+        <v>37.2782588034047</v>
+      </c>
+      <c r="O37" t="n">
+        <v>60.2710342338477</v>
+      </c>
+      <c r="P37" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="38">
@@ -1806,37 +2262,49 @@
         <v>5</v>
       </c>
       <c r="B38" t="n">
-        <v>24464.15438881</v>
+        <v>136820.48302102</v>
       </c>
       <c r="C38" t="n">
-        <v>1161.1911062</v>
+        <v>6554.546615</v>
       </c>
       <c r="D38" t="n">
-        <v>97.1909158330939</v>
+        <v>99.7372002783615</v>
       </c>
       <c r="E38" t="n">
-        <v>55.8479862847407</v>
+        <v>58.7383453960818</v>
       </c>
       <c r="F38" t="n">
-        <v>67653.3689246836</v>
+        <v>28949.4752215308</v>
       </c>
       <c r="G38" t="n">
-        <v>101697.618437879</v>
+        <v>5210.237931358</v>
       </c>
       <c r="H38" t="n">
-        <v>4441.1625472791</v>
+        <v>22.1835100841028</v>
       </c>
       <c r="I38" t="n">
-        <v>867.2949263</v>
+        <v>46.7237619116295</v>
       </c>
       <c r="J38" t="n">
-        <v>18.2583930264168</v>
+        <v>355026.99625769</v>
       </c>
       <c r="K38" t="n">
-        <v>41.7234270269359</v>
-      </c>
-      <c r="L38" t="s">
-        <v>14</v>
+        <v>574050.022538453</v>
+      </c>
+      <c r="L38" t="n">
+        <v>929077.018796143</v>
+      </c>
+      <c r="M38" t="n">
+        <v>21.870028950116</v>
+      </c>
+      <c r="N38" t="n">
+        <v>38.3279869094295</v>
+      </c>
+      <c r="O38" t="n">
+        <v>60.1980158595454</v>
+      </c>
+      <c r="P38" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="39">
@@ -1844,37 +2312,49 @@
         <v>6</v>
       </c>
       <c r="B39" t="n">
-        <v>23394.621338671</v>
+        <v>139719.99736543</v>
       </c>
       <c r="C39" t="n">
-        <v>1058.35661922</v>
+        <v>5810.479147</v>
       </c>
       <c r="D39" t="n">
-        <v>97.6882410478758</v>
+        <v>107.586362881489</v>
       </c>
       <c r="E39" t="n">
-        <v>51.0161440534564</v>
+        <v>52.0435003408487</v>
       </c>
       <c r="F39" t="n">
-        <v>63443.3536028196</v>
+        <v>30949.3851436631</v>
       </c>
       <c r="G39" t="n">
-        <v>91387.843798619</v>
+        <v>4466.1702918795</v>
       </c>
       <c r="H39" t="n">
-        <v>3191.4987101027</v>
+        <v>30.6945074197909</v>
       </c>
       <c r="I39" t="n">
-        <v>764.46045407</v>
+        <v>40.0095705356774</v>
       </c>
       <c r="J39" t="n">
-        <v>19.6558107601317</v>
+        <v>360841.743775931</v>
       </c>
       <c r="K39" t="n">
-        <v>36.8688903672142</v>
-      </c>
-      <c r="L39" t="s">
-        <v>14</v>
+        <v>501728.010235828</v>
+      </c>
+      <c r="L39" t="n">
+        <v>862569.75401176</v>
+      </c>
+      <c r="M39" t="n">
+        <v>22.2282233913895</v>
+      </c>
+      <c r="N39" t="n">
+        <v>33.9770211068564</v>
+      </c>
+      <c r="O39" t="n">
+        <v>56.2052444982459</v>
+      </c>
+      <c r="P39" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="40">
@@ -1882,37 +2362,49 @@
         <v>7</v>
       </c>
       <c r="B40" t="n">
-        <v>23234.731644616</v>
+        <v>137992.0018959</v>
       </c>
       <c r="C40" t="n">
-        <v>1075.48238307</v>
+        <v>5760.495689</v>
       </c>
       <c r="D40" t="n">
-        <v>94.5869859119648</v>
+        <v>103.36197207864</v>
       </c>
       <c r="E40" t="n">
-        <v>51.9219771661029</v>
+        <v>51.6950752895751</v>
       </c>
       <c r="F40" t="n">
-        <v>62782.1994446294</v>
+        <v>29093.0850377257</v>
       </c>
       <c r="G40" t="n">
-        <v>92866.6332758458</v>
+        <v>4416.187017021</v>
       </c>
       <c r="H40" t="n">
-        <v>3007.114908791</v>
+        <v>25.9811005159642</v>
       </c>
       <c r="I40" t="n">
-        <v>781.58620879</v>
+        <v>39.6322285929515</v>
       </c>
       <c r="J40" t="n">
-        <v>15.9073743682145</v>
+        <v>357931.598064233</v>
       </c>
       <c r="K40" t="n">
-        <v>37.7408286144227</v>
-      </c>
-      <c r="L40" t="s">
-        <v>14</v>
+        <v>497411.99768461</v>
+      </c>
+      <c r="L40" t="n">
+        <v>855343.595748843</v>
+      </c>
+      <c r="M40" t="n">
+        <v>22.0489554156165</v>
+      </c>
+      <c r="N40" t="n">
+        <v>33.6847407347056</v>
+      </c>
+      <c r="O40" t="n">
+        <v>55.7336961503221</v>
+      </c>
+      <c r="P40" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="41">
@@ -1920,37 +2412,49 @@
         <v>8</v>
       </c>
       <c r="B41" t="n">
-        <v>25400.320883739</v>
+        <v>149113.68023369</v>
       </c>
       <c r="C41" t="n">
-        <v>1026.47003241</v>
+        <v>5649.62038</v>
       </c>
       <c r="D41" t="n">
-        <v>106.338195006113</v>
+        <v>114.130295366572</v>
       </c>
       <c r="E41" t="n">
-        <v>49.5157372603914</v>
+        <v>50.614321783342</v>
       </c>
       <c r="F41" t="n">
-        <v>69369.3520135814</v>
+        <v>39993.7012375079</v>
       </c>
       <c r="G41" t="n">
-        <v>88634.4746962355</v>
+        <v>4305.311699464</v>
       </c>
       <c r="H41" t="n">
-        <v>5088.2789614688</v>
+        <v>38.9201490411927</v>
       </c>
       <c r="I41" t="n">
-        <v>732.57386334</v>
+        <v>38.5803935371693</v>
       </c>
       <c r="J41" t="n">
-        <v>30.26670334708</v>
+        <v>383473.062026314</v>
       </c>
       <c r="K41" t="n">
-        <v>35.3684834509751</v>
-      </c>
-      <c r="L41" t="s">
-        <v>14</v>
+        <v>487838.045733061</v>
+      </c>
+      <c r="L41" t="n">
+        <v>871311.107759375</v>
+      </c>
+      <c r="M41" t="n">
+        <v>23.6223359251753</v>
+      </c>
+      <c r="N41" t="n">
+        <v>33.0363927037059</v>
+      </c>
+      <c r="O41" t="n">
+        <v>56.6587286288811</v>
+      </c>
+      <c r="P41" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42">
@@ -1958,37 +2462,49 @@
         <v>9</v>
       </c>
       <c r="B42" t="n">
-        <v>25552.200325904</v>
+        <v>149508.53552941</v>
       </c>
       <c r="C42" t="n">
-        <v>1026.00030815</v>
+        <v>5770.703551</v>
       </c>
       <c r="D42" t="n">
-        <v>107.720522500849</v>
+        <v>115.628263460512</v>
       </c>
       <c r="E42" t="n">
-        <v>49.5092849118198</v>
+        <v>51.7548839427498</v>
       </c>
       <c r="F42" t="n">
-        <v>70415.5100839497</v>
+        <v>40566.4232453719</v>
       </c>
       <c r="G42" t="n">
-        <v>88593.914561285</v>
+        <v>4426.394947388</v>
       </c>
       <c r="H42" t="n">
-        <v>5278.3648292043</v>
+        <v>40.4635656667657</v>
       </c>
       <c r="I42" t="n">
-        <v>732.10416345</v>
+        <v>39.7209563184306</v>
       </c>
       <c r="J42" t="n">
-        <v>31.779855167847</v>
+        <v>386228.761938985</v>
       </c>
       <c r="K42" t="n">
-        <v>35.3620322682811</v>
-      </c>
-      <c r="L42" t="s">
-        <v>14</v>
+        <v>498293.434509431</v>
+      </c>
+      <c r="L42" t="n">
+        <v>884522.196448417</v>
+      </c>
+      <c r="M42" t="n">
+        <v>23.7920898805173</v>
+      </c>
+      <c r="N42" t="n">
+        <v>33.7444316369281</v>
+      </c>
+      <c r="O42" t="n">
+        <v>57.5365215174455</v>
+      </c>
+      <c r="P42" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="43">
@@ -1996,37 +2512,49 @@
         <v>10</v>
       </c>
       <c r="B43" t="n">
-        <v>27401.114402095</v>
+        <v>157035.044007763</v>
       </c>
       <c r="C43" t="n">
-        <v>1019.49318628</v>
+        <v>5928.14455</v>
       </c>
       <c r="D43" t="n">
-        <v>118.288615945215</v>
+        <v>122.696684221462</v>
       </c>
       <c r="E43" t="n">
-        <v>49.2692583060921</v>
+        <v>53.3281616110487</v>
       </c>
       <c r="F43" t="n">
-        <v>76646.2760011499</v>
+        <v>48118.6978464883</v>
       </c>
       <c r="G43" t="n">
-        <v>88032.0322748848</v>
+        <v>4583.835910441</v>
       </c>
       <c r="H43" t="n">
-        <v>7122.1085625549</v>
+        <v>47.3143877531963</v>
       </c>
       <c r="I43" t="n">
-        <v>725.59702795</v>
+        <v>41.2942336632156</v>
       </c>
       <c r="J43" t="n">
-        <v>41.6979987959261</v>
+        <v>405896.3527276</v>
       </c>
       <c r="K43" t="n">
-        <v>35.1220049507782</v>
-      </c>
-      <c r="L43" t="s">
-        <v>14</v>
+        <v>511888.278782919</v>
+      </c>
+      <c r="L43" t="n">
+        <v>917784.631510518</v>
+      </c>
+      <c r="M43" t="n">
+        <v>25.0036337474909</v>
+      </c>
+      <c r="N43" t="n">
+        <v>34.6650744980026</v>
+      </c>
+      <c r="O43" t="n">
+        <v>59.6687082454935</v>
+      </c>
+      <c r="P43" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="44">
@@ -2034,37 +2562,49 @@
         <v>11</v>
       </c>
       <c r="B44" t="n">
-        <v>31774.69057071</v>
+        <v>170484.51045498</v>
       </c>
       <c r="C44" t="n">
-        <v>1069.76081079</v>
+        <v>6840.718989</v>
       </c>
       <c r="D44" t="n">
-        <v>141.387224394219</v>
+        <v>137.275071783378</v>
       </c>
       <c r="E44" t="n">
-        <v>51.8209032565899</v>
+        <v>61.9669056801819</v>
       </c>
       <c r="F44" t="n">
-        <v>90866.036016694</v>
+        <v>61895.6682311594</v>
       </c>
       <c r="G44" t="n">
-        <v>93690.1136898472</v>
+        <v>5496.4104890889</v>
       </c>
       <c r="H44" t="n">
-        <v>11555.9107257463</v>
+        <v>60.9481537796566</v>
       </c>
       <c r="I44" t="n">
-        <v>775.86468003</v>
+        <v>49.95232388295</v>
       </c>
       <c r="J44" t="n">
-        <v>63.7279721857703</v>
+        <v>442736.873909379</v>
       </c>
       <c r="K44" t="n">
-        <v>37.6963463568015</v>
-      </c>
-      <c r="L44" t="s">
-        <v>14</v>
+        <v>599113.122611406</v>
+      </c>
+      <c r="L44" t="n">
+        <v>1041849.99652079</v>
+      </c>
+      <c r="M44" t="n">
+        <v>27.27304782945</v>
+      </c>
+      <c r="N44" t="n">
+        <v>40.001391898176</v>
+      </c>
+      <c r="O44" t="n">
+        <v>67.274439727626</v>
+      </c>
+      <c r="P44" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="45">
@@ -2072,37 +2612,49 @@
         <v>12</v>
       </c>
       <c r="B45" t="n">
-        <v>28079.633851031</v>
+        <v>152637.976425711</v>
       </c>
       <c r="C45" t="n">
-        <v>1107.70706023</v>
+        <v>6914.970738</v>
       </c>
       <c r="D45" t="n">
-        <v>123.478478549197</v>
+        <v>122.523691735952</v>
       </c>
       <c r="E45" t="n">
-        <v>53.5479610122171</v>
+        <v>62.4991409877888</v>
       </c>
       <c r="F45" t="n">
-        <v>80574.649564886</v>
+        <v>44251.9394230849</v>
       </c>
       <c r="G45" t="n">
-        <v>97013.4625995081</v>
+        <v>5570.662225892</v>
       </c>
       <c r="H45" t="n">
-        <v>7919.531663948</v>
+        <v>46.290917311368</v>
       </c>
       <c r="I45" t="n">
-        <v>813.81091119</v>
+        <v>50.4845590993907</v>
       </c>
       <c r="J45" t="n">
-        <v>45.9175732204687</v>
+        <v>399849.078186213</v>
       </c>
       <c r="K45" t="n">
-        <v>39.4234032395588</v>
-      </c>
-      <c r="L45" t="s">
-        <v>14</v>
+        <v>605616.122847826</v>
+      </c>
+      <c r="L45" t="n">
+        <v>1005465.20103404</v>
+      </c>
+      <c r="M45" t="n">
+        <v>24.6311154018903</v>
+      </c>
+      <c r="N45" t="n">
+        <v>40.4355821222811</v>
+      </c>
+      <c r="O45" t="n">
+        <v>65.0666975241714</v>
+      </c>
+      <c r="P45" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="46">
@@ -2110,37 +2662,49 @@
         <v>13</v>
       </c>
       <c r="B46" t="n">
-        <v>31437.9920177735</v>
+        <v>173851.647550698</v>
       </c>
       <c r="C46" t="n">
-        <v>1034.58997803</v>
+        <v>6393.784235</v>
       </c>
       <c r="D46" t="n">
-        <v>138.271901604602</v>
+        <v>139.759897715118</v>
       </c>
       <c r="E46" t="n">
-        <v>50.1147803875143</v>
+        <v>57.7931467903642</v>
       </c>
       <c r="F46" t="n">
-        <v>89535.5868956426</v>
+        <v>65045.247717797</v>
       </c>
       <c r="G46" t="n">
-        <v>90609.836971337</v>
+        <v>5049.4757180326</v>
       </c>
       <c r="H46" t="n">
-        <v>11179.6821328472</v>
+        <v>63.4976705978154</v>
       </c>
       <c r="I46" t="n">
-        <v>740.69383555</v>
+        <v>45.7785648282996</v>
       </c>
       <c r="J46" t="n">
-        <v>60.7424368239093</v>
+        <v>451482.82266961</v>
       </c>
       <c r="K46" t="n">
-        <v>35.9902229052603</v>
-      </c>
-      <c r="L46" t="s">
-        <v>14</v>
+        <v>559970.383887148</v>
+      </c>
+      <c r="L46" t="n">
+        <v>1011453.20655676</v>
+      </c>
+      <c r="M46" t="n">
+        <v>27.8118072888677</v>
+      </c>
+      <c r="N46" t="n">
+        <v>37.387922133314</v>
+      </c>
+      <c r="O46" t="n">
+        <v>65.1997294221817</v>
+      </c>
+      <c r="P46" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="47">
@@ -2148,37 +2712,49 @@
         <v>14</v>
       </c>
       <c r="B47" t="n">
-        <v>31349.14673276</v>
+        <v>167366.62840467</v>
       </c>
       <c r="C47" t="n">
-        <v>1030.46181732</v>
+        <v>6754.363389</v>
       </c>
       <c r="D47" t="n">
-        <v>132.398443399189</v>
+        <v>128.18728039526</v>
       </c>
       <c r="E47" t="n">
-        <v>49.920815174173</v>
+        <v>61.2338668307596</v>
       </c>
       <c r="F47" t="n">
-        <v>91465.5303112534</v>
+        <v>58819.8813587715</v>
       </c>
       <c r="G47" t="n">
-        <v>88979.1606075889</v>
+        <v>5410.0548007928</v>
       </c>
       <c r="H47" t="n">
-        <v>11140.7236489092</v>
+        <v>53.792049413419</v>
       </c>
       <c r="I47" t="n">
-        <v>736.56565708</v>
+        <v>49.1999394187638</v>
       </c>
       <c r="J47" t="n">
-        <v>57.0779875603305</v>
+        <v>439591.284920256</v>
       </c>
       <c r="K47" t="n">
-        <v>35.7735617841142</v>
-      </c>
-      <c r="L47" t="s">
-        <v>14</v>
+        <v>583231.299491435</v>
+      </c>
+      <c r="L47" t="n">
+        <v>1022822.58441169</v>
+      </c>
+      <c r="M47" t="n">
+        <v>27.0792763050802</v>
+      </c>
+      <c r="N47" t="n">
+        <v>39.4964238964562</v>
+      </c>
+      <c r="O47" t="n">
+        <v>66.5757002015363</v>
+      </c>
+      <c r="P47" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="48">
@@ -2186,37 +2762,49 @@
         <v>15</v>
       </c>
       <c r="B48" t="n">
-        <v>36348.027145147</v>
+        <v>209942.47879774</v>
       </c>
       <c r="C48" t="n">
-        <v>843.41277021</v>
+        <v>4919.170673</v>
       </c>
       <c r="D48" t="n">
-        <v>156.534115111584</v>
+        <v>164.413306323774</v>
       </c>
       <c r="E48" t="n">
-        <v>40.8915209502375</v>
+        <v>44.2103882820078</v>
       </c>
       <c r="F48" t="n">
-        <v>96683.86451116</v>
+        <v>100229.835889598</v>
       </c>
       <c r="G48" t="n">
-        <v>72827.6963567513</v>
+        <v>3574.8619825</v>
       </c>
       <c r="H48" t="n">
-        <v>15884.4790040952</v>
+        <v>89.0403794961183</v>
       </c>
       <c r="I48" t="n">
-        <v>549.51663448</v>
+        <v>32.1764598235932</v>
       </c>
       <c r="J48" t="n">
-        <v>79.8586770822312</v>
+        <v>516032.561230557</v>
       </c>
       <c r="K48" t="n">
-        <v>26.744268718725</v>
-      </c>
-      <c r="L48" t="s">
-        <v>14</v>
+        <v>424764.57643756</v>
+      </c>
+      <c r="L48" t="n">
+        <v>940797.137668117</v>
+      </c>
+      <c r="M48" t="n">
+        <v>31.7881377255134</v>
+      </c>
+      <c r="N48" t="n">
+        <v>28.765057331123</v>
+      </c>
+      <c r="O48" t="n">
+        <v>60.5531950566364</v>
+      </c>
+      <c r="P48" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="49">
@@ -2224,37 +2812,49 @@
         <v>16</v>
       </c>
       <c r="B49" t="n">
-        <v>34983.889619326</v>
+        <v>158004.16494594</v>
       </c>
       <c r="C49" t="n">
-        <v>1247.39889322</v>
+        <v>9471.761148</v>
       </c>
       <c r="D49" t="n">
-        <v>148.536486762246</v>
+        <v>117.849214719056</v>
       </c>
       <c r="E49" t="n">
-        <v>60.3360520595744</v>
+        <v>86.0533486654822</v>
       </c>
       <c r="F49" t="n">
-        <v>99583.0427430117</v>
+        <v>50065.887172835</v>
       </c>
       <c r="G49" t="n">
-        <v>107711.420836745</v>
+        <v>8127.4525328601</v>
       </c>
       <c r="H49" t="n">
-        <v>14916.3700450375</v>
+        <v>39.5226900278527</v>
       </c>
       <c r="I49" t="n">
-        <v>953.50272313</v>
+        <v>74.0194207932843</v>
       </c>
       <c r="J49" t="n">
-        <v>68.4760140985721</v>
+        <v>414267.954531748</v>
       </c>
       <c r="K49" t="n">
-        <v>46.1887981769321</v>
-      </c>
-      <c r="L49" t="s">
-        <v>14</v>
+        <v>817875.385830907</v>
+      </c>
+      <c r="L49" t="n">
+        <v>1232143.34036266</v>
+      </c>
+      <c r="M49" t="n">
+        <v>25.5193330485171</v>
+      </c>
+      <c r="N49" t="n">
+        <v>55.3865215420071</v>
+      </c>
+      <c r="O49" t="n">
+        <v>80.9058545905242</v>
+      </c>
+      <c r="P49" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="50">
@@ -2262,37 +2862,49 @@
         <v>1</v>
       </c>
       <c r="B50" t="n">
-        <v>174539.349900922</v>
+        <v>22412.338059469</v>
       </c>
       <c r="C50" t="n">
-        <v>6619.330973</v>
+        <v>2109.97350786</v>
       </c>
       <c r="D50" t="n">
-        <v>128.510969462808</v>
+        <v>88.2884163202638</v>
       </c>
       <c r="E50" t="n">
-        <v>59.1067270304137</v>
+        <v>102.510602155379</v>
       </c>
       <c r="F50" t="n">
-        <v>469390.159800459</v>
+        <v>2529.16017914569</v>
       </c>
       <c r="G50" t="n">
-        <v>579723.864583444</v>
+        <v>1816.07737098014</v>
       </c>
       <c r="H50" t="n">
-        <v>67286.8278348038</v>
+        <v>9.51917065356799</v>
       </c>
       <c r="I50" t="n">
-        <v>5275.022421</v>
+        <v>88.3860451304422</v>
       </c>
       <c r="J50" t="n">
-        <v>51.0179576622851</v>
+        <v>59114.4892718639</v>
       </c>
       <c r="K50" t="n">
-        <v>47.0921446191635</v>
-      </c>
-      <c r="L50" t="s">
-        <v>15</v>
+        <v>184792.390822377</v>
+      </c>
+      <c r="L50" t="n">
+        <v>243906.880094241</v>
+      </c>
+      <c r="M50" t="n">
+        <v>3.64151347749511</v>
+      </c>
+      <c r="N50" t="n">
+        <v>12.3381587985703</v>
+      </c>
+      <c r="O50" t="n">
+        <v>15.9796722760654</v>
+      </c>
+      <c r="P50" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="51">
@@ -2300,37 +2912,49 @@
         <v>2</v>
       </c>
       <c r="B51" t="n">
-        <v>158415.57558209</v>
+        <v>22543.519555299</v>
       </c>
       <c r="C51" t="n">
-        <v>6186.758084</v>
+        <v>1580.90003854</v>
       </c>
       <c r="D51" t="n">
-        <v>120.557879089585</v>
+        <v>92.6769216449942</v>
       </c>
       <c r="E51" t="n">
-        <v>55.31458802475</v>
+        <v>77.3321558462802</v>
       </c>
       <c r="F51" t="n">
-        <v>430516.548583787</v>
+        <v>2521.11881163574</v>
       </c>
       <c r="G51" t="n">
-        <v>541838.944196776</v>
+        <v>1287.0038841677</v>
       </c>
       <c r="H51" t="n">
-        <v>50560.2932897283</v>
+        <v>15.6279803108575</v>
       </c>
       <c r="I51" t="n">
-        <v>4842.449626</v>
+        <v>63.2075979046658</v>
       </c>
       <c r="J51" t="n">
-        <v>44.4427335927938</v>
+        <v>59800.5719615755</v>
       </c>
       <c r="K51" t="n">
-        <v>43.3000065195435</v>
-      </c>
-      <c r="L51" t="s">
-        <v>15</v>
+        <v>138455.90794611</v>
+      </c>
+      <c r="L51" t="n">
+        <v>198256.479907686</v>
+      </c>
+      <c r="M51" t="n">
+        <v>3.68377687843173</v>
+      </c>
+      <c r="N51" t="n">
+        <v>9.2443794424487</v>
+      </c>
+      <c r="O51" t="n">
+        <v>12.9281563208804</v>
+      </c>
+      <c r="P51" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="52">
@@ -2338,37 +2962,49 @@
         <v>3</v>
       </c>
       <c r="B52" t="n">
-        <v>142451.48789468</v>
+        <v>22162.690861452</v>
       </c>
       <c r="C52" t="n">
-        <v>6176.655733</v>
+        <v>1374.46742384</v>
       </c>
       <c r="D52" t="n">
-        <v>105.472106669281</v>
+        <v>88.60930678235</v>
       </c>
       <c r="E52" t="n">
-        <v>55.1829882749937</v>
+        <v>66.72803064856</v>
       </c>
       <c r="F52" t="n">
-        <v>378741.555426775</v>
+        <v>2171.42629957606</v>
       </c>
       <c r="G52" t="n">
-        <v>540954.175934396</v>
+        <v>1080.5712609843</v>
       </c>
       <c r="H52" t="n">
-        <v>34692.2513553354</v>
+        <v>10.5013610078282</v>
       </c>
       <c r="I52" t="n">
-        <v>4832.347197</v>
+        <v>52.6034721607589</v>
       </c>
       <c r="J52" t="n">
-        <v>28.4750778340043</v>
+        <v>58644.3115179705</v>
       </c>
       <c r="K52" t="n">
-        <v>43.1684061377285</v>
-      </c>
-      <c r="L52" t="s">
-        <v>15</v>
+        <v>120376.450421159</v>
+      </c>
+      <c r="L52" t="n">
+        <v>179020.761939129</v>
+      </c>
+      <c r="M52" t="n">
+        <v>3.61255004317113</v>
+      </c>
+      <c r="N52" t="n">
+        <v>8.03725604877353</v>
+      </c>
+      <c r="O52" t="n">
+        <v>11.6498060919447</v>
+      </c>
+      <c r="P52" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="53">
@@ -2376,37 +3012,49 @@
         <v>4</v>
       </c>
       <c r="B53" t="n">
-        <v>150489.67179329</v>
+        <v>23103.489031248</v>
       </c>
       <c r="C53" t="n">
-        <v>5916.584654</v>
+        <v>1281.7087638</v>
       </c>
       <c r="D53" t="n">
-        <v>117.820173635166</v>
+        <v>96.2718150811335</v>
       </c>
       <c r="E53" t="n">
-        <v>52.9186196440184</v>
+        <v>62.3227211764989</v>
       </c>
       <c r="F53" t="n">
-        <v>400774.212619399</v>
+        <v>2965.21171576757</v>
       </c>
       <c r="G53" t="n">
-        <v>518177.038547061</v>
+        <v>987.81262856462</v>
       </c>
       <c r="H53" t="n">
-        <v>42064.6325372254</v>
+        <v>19.1127050617248</v>
       </c>
       <c r="I53" t="n">
-        <v>4572.276035</v>
+        <v>48.198164044124</v>
       </c>
       <c r="J53" t="n">
-        <v>41.746400837232</v>
+        <v>61743.3095376734</v>
       </c>
       <c r="K53" t="n">
-        <v>40.90403674999</v>
-      </c>
-      <c r="L53" t="s">
-        <v>15</v>
+        <v>112252.606925296</v>
+      </c>
+      <c r="L53" t="n">
+        <v>173995.916462969</v>
+      </c>
+      <c r="M53" t="n">
+        <v>3.80345151579621</v>
+      </c>
+      <c r="N53" t="n">
+        <v>7.49484588426067</v>
+      </c>
+      <c r="O53" t="n">
+        <v>11.2982974000569</v>
+      </c>
+      <c r="P53" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="54">
@@ -2414,37 +3062,49 @@
         <v>5</v>
       </c>
       <c r="B54" t="n">
-        <v>143294.10220174</v>
+        <v>22153.317999506</v>
       </c>
       <c r="C54" t="n">
-        <v>6177.467889</v>
+        <v>1330.1573014</v>
       </c>
       <c r="D54" t="n">
-        <v>104.914213405078</v>
+        <v>87.49378582589</v>
       </c>
       <c r="E54" t="n">
-        <v>55.1824275327287</v>
+        <v>64.3889010001654</v>
       </c>
       <c r="F54" t="n">
-        <v>380816.650967763</v>
+        <v>2142.06295214739</v>
       </c>
       <c r="G54" t="n">
-        <v>541025.304907534</v>
+        <v>1036.26116291667</v>
       </c>
       <c r="H54" t="n">
-        <v>35390.0035800967</v>
+        <v>8.60612409327883</v>
       </c>
       <c r="I54" t="n">
-        <v>4833.159286</v>
+        <v>50.2643437743682</v>
       </c>
       <c r="J54" t="n">
-        <v>27.3372585873033</v>
+        <v>58582.3834437173</v>
       </c>
       <c r="K54" t="n">
-        <v>43.1678448063354</v>
-      </c>
-      <c r="L54" t="s">
-        <v>15</v>
+        <v>116495.750766486</v>
+      </c>
+      <c r="L54" t="n">
+        <v>175078.134210204</v>
+      </c>
+      <c r="M54" t="n">
+        <v>3.60873520995839</v>
+      </c>
+      <c r="N54" t="n">
+        <v>7.77815074483855</v>
+      </c>
+      <c r="O54" t="n">
+        <v>11.3868859547969</v>
+      </c>
+      <c r="P54" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="55">
@@ -2452,37 +3112,49 @@
         <v>6</v>
       </c>
       <c r="B55" t="n">
-        <v>141464.11055318</v>
+        <v>22824.736391637</v>
       </c>
       <c r="C55" t="n">
-        <v>5760.430606</v>
+        <v>1094.31645402</v>
       </c>
       <c r="D55" t="n">
-        <v>109.372463989217</v>
+        <v>94.8985928965348</v>
       </c>
       <c r="E55" t="n">
-        <v>51.5664691108899</v>
+        <v>52.8628290105597</v>
       </c>
       <c r="F55" t="n">
-        <v>367766.217721587</v>
+        <v>2625.31581731824</v>
       </c>
       <c r="G55" t="n">
-        <v>497406.377844445</v>
+        <v>800.4202732668</v>
       </c>
       <c r="H55" t="n">
-        <v>32684.9360938539</v>
+        <v>16.8807864172737</v>
       </c>
       <c r="I55" t="n">
-        <v>4416.12169</v>
+        <v>38.7155745127215</v>
       </c>
       <c r="J55" t="n">
-        <v>32.474559590281</v>
+        <v>61068.3480344425</v>
       </c>
       <c r="K55" t="n">
-        <v>39.5325387384548</v>
-      </c>
-      <c r="L55" t="s">
-        <v>15</v>
+        <v>94492.9330530789</v>
+      </c>
+      <c r="L55" t="n">
+        <v>155561.281087521</v>
+      </c>
+      <c r="M55" t="n">
+        <v>3.7618731914111</v>
+      </c>
+      <c r="N55" t="n">
+        <v>6.39906147413247</v>
+      </c>
+      <c r="O55" t="n">
+        <v>10.1609346655436</v>
+      </c>
+      <c r="P55" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="56">
@@ -2490,37 +3162,49 @@
         <v>7</v>
       </c>
       <c r="B56" t="n">
-        <v>138942.52003369</v>
+        <v>22972.210245018</v>
       </c>
       <c r="C56" t="n">
-        <v>5747.447556</v>
+        <v>1089.44321467</v>
       </c>
       <c r="D56" t="n">
-        <v>104.422927870384</v>
+        <v>93.2347998011782</v>
       </c>
       <c r="E56" t="n">
-        <v>51.5693343359411</v>
+        <v>52.6458675040139</v>
       </c>
       <c r="F56" t="n">
-        <v>361725.655180016</v>
+        <v>2746.2528246686</v>
       </c>
       <c r="G56" t="n">
-        <v>496285.306814243</v>
+        <v>795.54703899072</v>
       </c>
       <c r="H56" t="n">
-        <v>30041.2095182028</v>
+        <v>14.5616778645056</v>
       </c>
       <c r="I56" t="n">
-        <v>4403.138861</v>
+        <v>38.4647188794018</v>
       </c>
       <c r="J56" t="n">
-        <v>27.040629985282</v>
+        <v>61667.3231348664</v>
       </c>
       <c r="K56" t="n">
-        <v>39.5064874174496</v>
-      </c>
-      <c r="L56" t="s">
-        <v>15</v>
+        <v>94072.1345921222</v>
+      </c>
+      <c r="L56" t="n">
+        <v>155739.457726989</v>
+      </c>
+      <c r="M56" t="n">
+        <v>3.79877067505249</v>
+      </c>
+      <c r="N56" t="n">
+        <v>6.37056500214371</v>
+      </c>
+      <c r="O56" t="n">
+        <v>10.1693356771962</v>
+      </c>
+      <c r="P56" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="57">
@@ -2528,37 +3212,49 @@
         <v>8</v>
       </c>
       <c r="B57" t="n">
-        <v>151112.69943237</v>
+        <v>24891.113121748</v>
       </c>
       <c r="C57" t="n">
-        <v>5624.593541</v>
+        <v>1041.96822101</v>
       </c>
       <c r="D57" t="n">
-        <v>116.114020802979</v>
+        <v>103.665282581345</v>
       </c>
       <c r="E57" t="n">
-        <v>50.3746175429341</v>
+        <v>50.3130887356167</v>
       </c>
       <c r="F57" t="n">
-        <v>390983.257279837</v>
+        <v>4581.23745280582</v>
       </c>
       <c r="G57" t="n">
-        <v>485677.007750429</v>
+        <v>748.07204671984</v>
       </c>
       <c r="H57" t="n">
-        <v>41987.6102970714</v>
+        <v>27.6021779609433</v>
       </c>
       <c r="I57" t="n">
-        <v>4280.284804</v>
+        <v>36.1658346612252</v>
       </c>
       <c r="J57" t="n">
-        <v>40.9002613331147</v>
+        <v>67358.1377059218</v>
       </c>
       <c r="K57" t="n">
-        <v>38.3406887624799</v>
-      </c>
-      <c r="L57" t="s">
-        <v>15</v>
+        <v>89972.7249733323</v>
+      </c>
+      <c r="L57" t="n">
+        <v>157330.862679254</v>
+      </c>
+      <c r="M57" t="n">
+        <v>4.14933071902275</v>
+      </c>
+      <c r="N57" t="n">
+        <v>6.09295298068649</v>
+      </c>
+      <c r="O57" t="n">
+        <v>10.2422836997092</v>
+      </c>
+      <c r="P57" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="58">
@@ -2566,37 +3262,49 @@
         <v>9</v>
       </c>
       <c r="B58" t="n">
-        <v>152666.5324993</v>
+        <v>24637.782387486</v>
       </c>
       <c r="C58" t="n">
-        <v>5663.812742</v>
+        <v>1075.12231205</v>
       </c>
       <c r="D58" t="n">
-        <v>118.499188828883</v>
+        <v>103.402841217832</v>
       </c>
       <c r="E58" t="n">
-        <v>50.7373254036727</v>
+        <v>52.0264230709302</v>
       </c>
       <c r="F58" t="n">
-        <v>398442.398152766</v>
+        <v>4368.3335429612</v>
       </c>
       <c r="G58" t="n">
-        <v>489063.539425863</v>
+        <v>781.2261764717</v>
       </c>
       <c r="H58" t="n">
-        <v>43712.7240025002</v>
+        <v>27.479545599953</v>
       </c>
       <c r="I58" t="n">
-        <v>4319.504178</v>
+        <v>37.8791709070342</v>
       </c>
       <c r="J58" t="n">
-        <v>43.3261238396236</v>
+        <v>66766.1146227962</v>
       </c>
       <c r="K58" t="n">
-        <v>38.7033981521308</v>
-      </c>
-      <c r="L58" t="s">
-        <v>15</v>
+        <v>92835.5415686324</v>
+      </c>
+      <c r="L58" t="n">
+        <v>159601.656191429</v>
+      </c>
+      <c r="M58" t="n">
+        <v>4.11286148681344</v>
+      </c>
+      <c r="N58" t="n">
+        <v>6.28682292196773</v>
+      </c>
+      <c r="O58" t="n">
+        <v>10.3996844087812</v>
+      </c>
+      <c r="P58" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="59">
@@ -2604,37 +3312,49 @@
         <v>10</v>
       </c>
       <c r="B59" t="n">
-        <v>163074.344820418</v>
+        <v>25699.259990046</v>
       </c>
       <c r="C59" t="n">
-        <v>5647.063745</v>
+        <v>1120.20199518</v>
       </c>
       <c r="D59" t="n">
-        <v>127.867230108075</v>
+        <v>110.578477409453</v>
       </c>
       <c r="E59" t="n">
-        <v>50.6348891998656</v>
+        <v>54.456515719586</v>
       </c>
       <c r="F59" t="n">
-        <v>430199.897034407</v>
+        <v>5426.9141796189</v>
       </c>
       <c r="G59" t="n">
-        <v>487617.283321047</v>
+        <v>826.3058358483</v>
       </c>
       <c r="H59" t="n">
-        <v>54135.973846145</v>
+        <v>34.0138954295134</v>
       </c>
       <c r="I59" t="n">
-        <v>4302.755109</v>
+        <v>40.309262321822</v>
       </c>
       <c r="J59" t="n">
-        <v>52.4689615473748</v>
+        <v>69676.7140988046</v>
       </c>
       <c r="K59" t="n">
-        <v>38.6009612904814</v>
-      </c>
-      <c r="L59" t="s">
-        <v>15</v>
+        <v>96728.1189528149</v>
+      </c>
+      <c r="L59" t="n">
+        <v>166404.83305162</v>
+      </c>
+      <c r="M59" t="n">
+        <v>4.29215741493574</v>
+      </c>
+      <c r="N59" t="n">
+        <v>6.55042826439275</v>
+      </c>
+      <c r="O59" t="n">
+        <v>10.8425856793285</v>
+      </c>
+      <c r="P59" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="60">
@@ -2642,37 +3362,49 @@
         <v>11</v>
       </c>
       <c r="B60" t="n">
-        <v>186418.26606348</v>
+        <v>27196.29254902</v>
       </c>
       <c r="C60" t="n">
-        <v>5744.446926</v>
+        <v>1421.09476549</v>
       </c>
       <c r="D60" t="n">
-        <v>149.771795109047</v>
+        <v>122.230661607986</v>
       </c>
       <c r="E60" t="n">
-        <v>51.4989934475539</v>
+        <v>69.837867050281</v>
       </c>
       <c r="F60" t="n">
-        <v>504709.25768682</v>
+        <v>6988.90714459473</v>
       </c>
       <c r="G60" t="n">
-        <v>503101.142006486</v>
+        <v>1127.19865573481</v>
       </c>
       <c r="H60" t="n">
-        <v>77791.0292286628</v>
+        <v>44.6179577092243</v>
       </c>
       <c r="I60" t="n">
-        <v>4400.138424</v>
+        <v>55.7133112090727</v>
       </c>
       <c r="J60" t="n">
-        <v>73.4157137815196</v>
+        <v>73012.0443149839</v>
       </c>
       <c r="K60" t="n">
-        <v>39.4844116325389</v>
-      </c>
-      <c r="L60" t="s">
-        <v>15</v>
+        <v>124460.093134727</v>
+      </c>
+      <c r="L60" t="n">
+        <v>197472.137449711</v>
+      </c>
+      <c r="M60" t="n">
+        <v>4.49761719448753</v>
+      </c>
+      <c r="N60" t="n">
+        <v>8.30991138946374</v>
+      </c>
+      <c r="O60" t="n">
+        <v>12.8075285839513</v>
+      </c>
+      <c r="P60" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="61">
@@ -2680,37 +3412,49 @@
         <v>12</v>
       </c>
       <c r="B61" t="n">
-        <v>166329.139744071</v>
+        <v>24091.675496012</v>
       </c>
       <c r="C61" t="n">
-        <v>5917.944872</v>
+        <v>1433.67323173</v>
       </c>
       <c r="D61" t="n">
-        <v>134.026400391812</v>
+        <v>106.063459218684</v>
       </c>
       <c r="E61" t="n">
-        <v>52.9795177173176</v>
+        <v>70.2604368080786</v>
       </c>
       <c r="F61" t="n">
-        <v>453843.06440615</v>
+        <v>3942.46287148064</v>
       </c>
       <c r="G61" t="n">
-        <v>518296.16702679</v>
+        <v>1139.77708303009</v>
       </c>
       <c r="H61" t="n">
-        <v>57907.2156753563</v>
+        <v>28.5464985966722</v>
       </c>
       <c r="I61" t="n">
-        <v>4573.636293</v>
+        <v>56.1358790510155</v>
       </c>
       <c r="J61" t="n">
-        <v>57.7671898730524</v>
+        <v>64778.6269724753</v>
       </c>
       <c r="K61" t="n">
-        <v>40.9649352029195</v>
-      </c>
-      <c r="L61" t="s">
-        <v>15</v>
+        <v>125561.720638916</v>
+      </c>
+      <c r="L61" t="n">
+        <v>190340.347611391</v>
+      </c>
+      <c r="M61" t="n">
+        <v>3.99043019874607</v>
+      </c>
+      <c r="N61" t="n">
+        <v>8.38346449964899</v>
+      </c>
+      <c r="O61" t="n">
+        <v>12.3738946983951</v>
+      </c>
+      <c r="P61" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="62">
@@ -2718,37 +3462,49 @@
         <v>13</v>
       </c>
       <c r="B62" t="n">
-        <v>186159.330271138</v>
+        <v>27895.3627617635</v>
       </c>
       <c r="C62" t="n">
-        <v>5619.207819</v>
+        <v>1293.96971283</v>
       </c>
       <c r="D62" t="n">
-        <v>149.706149466242</v>
+        <v>123.036424866407</v>
       </c>
       <c r="E62" t="n">
-        <v>50.3839876701363</v>
+        <v>63.4464474354856</v>
       </c>
       <c r="F62" t="n">
-        <v>499313.442393003</v>
+        <v>7645.8934712822</v>
       </c>
       <c r="G62" t="n">
-        <v>492132.64694208</v>
+        <v>1000.07356264392</v>
       </c>
       <c r="H62" t="n">
-        <v>77323.7347515964</v>
+        <v>45.5448177633257</v>
       </c>
       <c r="I62" t="n">
-        <v>4274.89929</v>
+        <v>49.3218895840806</v>
       </c>
       <c r="J62" t="n">
-        <v>73.4206159768654</v>
+        <v>75546.1545320567</v>
       </c>
       <c r="K62" t="n">
-        <v>38.3694056113146</v>
-      </c>
-      <c r="L62" t="s">
-        <v>15</v>
+        <v>113326.426135141</v>
+      </c>
+      <c r="L62" t="n">
+        <v>188872.580667198</v>
+      </c>
+      <c r="M62" t="n">
+        <v>4.65372099615432</v>
+      </c>
+      <c r="N62" t="n">
+        <v>7.5665422992108</v>
+      </c>
+      <c r="O62" t="n">
+        <v>12.2202632953651</v>
+      </c>
+      <c r="P62" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="63">
@@ -2756,37 +3512,49 @@
         <v>14</v>
       </c>
       <c r="B63" t="n">
-        <v>183676.64595247</v>
+        <v>26492.45677319</v>
       </c>
       <c r="C63" t="n">
-        <v>5773.985992</v>
+        <v>1359.74079552</v>
       </c>
       <c r="D63" t="n">
-        <v>142.149458381102</v>
+        <v>110.557331935402</v>
       </c>
       <c r="E63" t="n">
-        <v>51.860282639682</v>
+        <v>66.834128246961</v>
       </c>
       <c r="F63" t="n">
-        <v>505310.158402147</v>
+        <v>6296.27529205534</v>
       </c>
       <c r="G63" t="n">
-        <v>498576.869412127</v>
+        <v>1065.84462763463</v>
       </c>
       <c r="H63" t="n">
-        <v>75088.843026052</v>
+        <v>35.2806189234038</v>
       </c>
       <c r="I63" t="n">
-        <v>4429.677375</v>
+        <v>52.6868745376419</v>
       </c>
       <c r="J63" t="n">
-        <v>67.7271809432991</v>
+        <v>71822.0066868266</v>
       </c>
       <c r="K63" t="n">
-        <v>39.8263549331731</v>
-      </c>
-      <c r="L63" t="s">
-        <v>15</v>
+        <v>117412.011387214</v>
+      </c>
+      <c r="L63" t="n">
+        <v>189234.01807404</v>
+      </c>
+      <c r="M63" t="n">
+        <v>4.42430964983919</v>
+      </c>
+      <c r="N63" t="n">
+        <v>7.95114147050853</v>
+      </c>
+      <c r="O63" t="n">
+        <v>12.3754511203477</v>
+      </c>
+      <c r="P63" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="64">
@@ -2794,37 +3562,49 @@
         <v>15</v>
       </c>
       <c r="B64" t="n">
-        <v>214149.49953893</v>
+        <v>35387.785734647</v>
       </c>
       <c r="C64" t="n">
-        <v>4916.777897</v>
+        <v>847.71650831</v>
       </c>
       <c r="D64" t="n">
-        <v>168.230102446458</v>
+        <v>151.824172414797</v>
       </c>
       <c r="E64" t="n">
-        <v>44.1874367512114</v>
+        <v>41.1137036774873</v>
       </c>
       <c r="F64" t="n">
-        <v>528144.410534121</v>
+        <v>14925.0356490264</v>
       </c>
       <c r="G64" t="n">
-        <v>424557.963056624</v>
+        <v>553.8203714833</v>
       </c>
       <c r="H64" t="n">
-        <v>104436.356307479</v>
+        <v>75.1518529256129</v>
       </c>
       <c r="I64" t="n">
-        <v>3572.469213</v>
+        <v>26.9664513892842</v>
       </c>
       <c r="J64" t="n">
-        <v>92.8568541236453</v>
+        <v>93769.1497170609</v>
       </c>
       <c r="K64" t="n">
-        <v>32.1535083549023</v>
-      </c>
-      <c r="L64" t="s">
-        <v>15</v>
+        <v>73199.3190575408</v>
+      </c>
+      <c r="L64" t="n">
+        <v>166968.468774602</v>
+      </c>
+      <c r="M64" t="n">
+        <v>5.77627628477973</v>
+      </c>
+      <c r="N64" t="n">
+        <v>4.95705792358805</v>
+      </c>
+      <c r="O64" t="n">
+        <v>10.7333342083678</v>
+      </c>
+      <c r="P64" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="65">
@@ -2832,37 +3612,49 @@
         <v>16</v>
       </c>
       <c r="B65" t="n">
-        <v>197096.38234033</v>
+        <v>23297.692842667</v>
       </c>
       <c r="C65" t="n">
-        <v>6529.732686</v>
+        <v>2189.08371792</v>
       </c>
       <c r="D65" t="n">
-        <v>152.766732696951</v>
+        <v>93.275593705566</v>
       </c>
       <c r="E65" t="n">
-        <v>58.5492934473676</v>
+        <v>107.632350620382</v>
       </c>
       <c r="F65" t="n">
-        <v>538667.296211295</v>
+        <v>3253.3613152666</v>
       </c>
       <c r="G65" t="n">
-        <v>563834.703650926</v>
+        <v>1895.1876262228</v>
       </c>
       <c r="H65" t="n">
-        <v>89082.5830168385</v>
+        <v>13.3046884508655</v>
       </c>
       <c r="I65" t="n">
-        <v>5185.424042</v>
+        <v>93.4851007054751</v>
       </c>
       <c r="J65" t="n">
-        <v>74.3867678145332</v>
+        <v>62385.293211311</v>
       </c>
       <c r="K65" t="n">
-        <v>46.5153654105036</v>
-      </c>
-      <c r="L65" t="s">
-        <v>15</v>
+        <v>189024.793006739</v>
+      </c>
+      <c r="L65" t="n">
+        <v>251410.086218051</v>
+      </c>
+      <c r="M65" t="n">
+        <v>3.84299837188308</v>
+      </c>
+      <c r="N65" t="n">
+        <v>12.800759077992</v>
+      </c>
+      <c r="O65" t="n">
+        <v>16.6437574498751</v>
+      </c>
+      <c r="P65" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2881,7 +3673,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HRV CZ15 67% SRE Re-run
</commit_message>
<xml_diff>
--- a/framework/analysis/lr/TDVAnnual.xlsx
+++ b/framework/analysis/lr/TDVAnnual.xlsx
@@ -812,46 +812,46 @@
         <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>36348.027145147</v>
+        <v>35697.057505597</v>
       </c>
       <c r="C9" t="n">
         <v>843.41277021</v>
       </c>
       <c r="D9" t="n">
-        <v>156.534115111584</v>
+        <v>151.115833761224</v>
       </c>
       <c r="E9" t="n">
         <v>40.8915209502375</v>
       </c>
       <c r="F9" t="n">
-        <v>15884.4790040952</v>
+        <v>15176.937152828</v>
       </c>
       <c r="G9" t="n">
         <v>549.51663448</v>
       </c>
       <c r="H9" t="n">
-        <v>79.8586770822312</v>
+        <v>74.2330705107738</v>
       </c>
       <c r="I9" t="n">
         <v>26.744268718725</v>
       </c>
       <c r="J9" t="n">
-        <v>96683.86451116</v>
+        <v>95953.019481924</v>
       </c>
       <c r="K9" t="n">
         <v>72827.6963567513</v>
       </c>
       <c r="L9" t="n">
-        <v>169511.560867911</v>
+        <v>168780.715838675</v>
       </c>
       <c r="M9" t="n">
-        <v>5.95582572073871</v>
+        <v>5.91080491354399</v>
       </c>
       <c r="N9" t="n">
         <v>4.93189163410268</v>
       </c>
       <c r="O9" t="n">
-        <v>10.8877173548414</v>
+        <v>10.8426965476467</v>
       </c>
       <c r="P9" t="s">
         <v>19</v>

</xml_diff>